<commit_message>
Add highlighting and active game selection methods
</commit_message>
<xml_diff>
--- a/_DESIGN/Book4b.xlsx
+++ b/_DESIGN/Book4b.xlsx
@@ -17,7 +17,6 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -282,13 +281,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF303336"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="9">
@@ -353,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -365,6 +369,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,13 +693,13 @@
       <selection activeCell="I9" sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="9" width="3" bestFit="1" customWidth="1"/>
     <col min="11" max="19" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1">
         <v>11</v>
       </c>
@@ -757,7 +764,7 @@
         <v>button19</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>21</v>
       </c>
@@ -822,7 +829,7 @@
         <v>button29</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>31</v>
       </c>
@@ -887,7 +894,7 @@
         <v>button39</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>41</v>
       </c>
@@ -952,7 +959,7 @@
         <v>button49</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>51</v>
       </c>
@@ -1017,7 +1024,7 @@
         <v>button59</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>61</v>
       </c>
@@ -1082,7 +1089,7 @@
         <v>button69</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>71</v>
       </c>
@@ -1147,7 +1154,7 @@
         <v>button79</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>81</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>button89</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>91</v>
       </c>
@@ -1277,7 +1284,7 @@
         <v>button99</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="K11" s="1" t="str">
         <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/button12"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button11" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button11" app:layout_constraintEnd_toStartOf="@id/button12" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
@@ -1315,7 +1322,7 @@
         <v>&lt;Button android:id="@+id/button19" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button19" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button18" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="K12" s="4" t="str">
         <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;K1&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button21" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button21" app:layout_constraintEnd_toStartOf="@id/button22" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button11" /&gt;</v>
@@ -1353,7 +1360,7 @@
         <v>&lt;Button android:id="@+id/button29" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button29" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button28" app:layout_constraintTop_toBottomOf="@id/button19" /&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="K13" s="4" t="str">
         <f t="shared" ref="K13:K19" si="12">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K3&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;L3&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;K2&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button31" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button31" app:layout_constraintEnd_toStartOf="@id/button32" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button21" /&gt;</v>
@@ -1391,7 +1398,7 @@
         <v>&lt;Button android:id="@+id/button39" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button39" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button38" app:layout_constraintTop_toBottomOf="@id/button29" /&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="K14" s="4" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button41" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button41" app:layout_constraintEnd_toStartOf="@id/button42" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button31" /&gt;</v>
@@ -1429,7 +1436,7 @@
         <v>&lt;Button android:id="@+id/button49" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button49" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button48" app:layout_constraintTop_toBottomOf="@id/button39" /&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="K15" s="4" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button51" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button51" app:layout_constraintEnd_toStartOf="@id/button52" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button41" /&gt;</v>
@@ -1467,7 +1474,7 @@
         <v>&lt;Button android:id="@+id/button59" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button59" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button58" app:layout_constraintTop_toBottomOf="@id/button49" /&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="K16" s="4" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button61" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button61" app:layout_constraintEnd_toStartOf="@id/button62" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button51" /&gt;</v>
@@ -1505,7 +1512,7 @@
         <v>&lt;Button android:id="@+id/button69" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button69" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button68" app:layout_constraintTop_toBottomOf="@id/button59" /&gt;</v>
       </c>
     </row>
-    <row r="17" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:19">
       <c r="K17" s="4" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button71" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button71" app:layout_constraintEnd_toStartOf="@id/button72" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button61" /&gt;</v>
@@ -1543,7 +1550,7 @@
         <v>&lt;Button android:id="@+id/button79" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button79" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button78" app:layout_constraintTop_toBottomOf="@id/button69" /&gt;</v>
       </c>
     </row>
-    <row r="18" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:19">
       <c r="K18" s="4" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button81" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button81" app:layout_constraintEnd_toStartOf="@id/button82" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button71" /&gt;</v>
@@ -1581,7 +1588,7 @@
         <v>&lt;Button android:id="@+id/button89" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button89" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button88" app:layout_constraintTop_toBottomOf="@id/button79" /&gt;</v>
       </c>
     </row>
-    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:19">
       <c r="K19" s="4" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button91" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button91" app:layout_constraintEnd_toStartOf="@id/button92" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button81" /&gt;</v>
@@ -1630,16 +1637,16 @@
   <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D1" sqref="D1:D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1651,12 +1658,12 @@
         <f>A1&amp;" = findViewById(R.id."&amp;A1&amp;");"</f>
         <v>button11 = findViewById(R.id.button11);</v>
       </c>
-      <c r="D1" t="str">
-        <f>A1&amp;".setBackgroundResource(android.R.drawable.btn_default);"</f>
-        <v>button11.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="10" t="str">
+        <f>A1&amp;".getBackground().setColorFilter(null);"</f>
+        <v>button11.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1668,12 +1675,12 @@
         <f t="shared" ref="C2:C65" si="1">A2&amp;" = findViewById(R.id."&amp;A2&amp;");"</f>
         <v>button12 = findViewById(R.id.button12);</v>
       </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D65" si="2">A2&amp;".setBackgroundResource(android.R.drawable.btn_default);"</f>
-        <v>button12.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="10" t="str">
+        <f t="shared" ref="D2:D65" si="2">A2&amp;".getBackground().setColorFilter(null);"</f>
+        <v>button12.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1685,12 +1692,12 @@
         <f t="shared" si="1"/>
         <v>button13 = findViewById(R.id.button13);</v>
       </c>
-      <c r="D3" t="str">
-        <f t="shared" si="2"/>
-        <v>button13.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button13.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1702,12 +1709,12 @@
         <f t="shared" si="1"/>
         <v>button14 = findViewById(R.id.button14);</v>
       </c>
-      <c r="D4" t="str">
-        <f t="shared" si="2"/>
-        <v>button14.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button14.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1719,12 +1726,12 @@
         <f t="shared" si="1"/>
         <v>button15 = findViewById(R.id.button15);</v>
       </c>
-      <c r="D5" t="str">
-        <f t="shared" si="2"/>
-        <v>button15.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button15.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1736,12 +1743,12 @@
         <f t="shared" si="1"/>
         <v>button16 = findViewById(R.id.button16);</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" si="2"/>
-        <v>button16.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button16.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1753,12 +1760,12 @@
         <f t="shared" si="1"/>
         <v>button17 = findViewById(R.id.button17);</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" si="2"/>
-        <v>button17.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button17.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1770,12 +1777,12 @@
         <f t="shared" si="1"/>
         <v>button18 = findViewById(R.id.button18);</v>
       </c>
-      <c r="D8" t="str">
-        <f t="shared" si="2"/>
-        <v>button18.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button18.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1787,12 +1794,12 @@
         <f t="shared" si="1"/>
         <v>button19 = findViewById(R.id.button19);</v>
       </c>
-      <c r="D9" t="str">
-        <f t="shared" si="2"/>
-        <v>button19.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button19.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1804,12 +1811,12 @@
         <f t="shared" si="1"/>
         <v>button21 = findViewById(R.id.button21);</v>
       </c>
-      <c r="D10" t="str">
-        <f t="shared" si="2"/>
-        <v>button21.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button21.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1821,12 +1828,12 @@
         <f t="shared" si="1"/>
         <v>button22 = findViewById(R.id.button22);</v>
       </c>
-      <c r="D11" t="str">
-        <f t="shared" si="2"/>
-        <v>button22.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button22.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1838,12 +1845,12 @@
         <f t="shared" si="1"/>
         <v>button23 = findViewById(R.id.button23);</v>
       </c>
-      <c r="D12" t="str">
-        <f t="shared" si="2"/>
-        <v>button23.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button23.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1855,12 +1862,12 @@
         <f t="shared" si="1"/>
         <v>button24 = findViewById(R.id.button24);</v>
       </c>
-      <c r="D13" t="str">
-        <f t="shared" si="2"/>
-        <v>button24.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button24.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1872,12 +1879,12 @@
         <f t="shared" si="1"/>
         <v>button25 = findViewById(R.id.button25);</v>
       </c>
-      <c r="D14" t="str">
-        <f t="shared" si="2"/>
-        <v>button25.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button25.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1889,12 +1896,12 @@
         <f t="shared" si="1"/>
         <v>button26 = findViewById(R.id.button26);</v>
       </c>
-      <c r="D15" t="str">
-        <f t="shared" si="2"/>
-        <v>button26.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button26.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1906,12 +1913,12 @@
         <f t="shared" si="1"/>
         <v>button27 = findViewById(R.id.button27);</v>
       </c>
-      <c r="D16" t="str">
-        <f t="shared" si="2"/>
-        <v>button27.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button27.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1923,12 +1930,12 @@
         <f t="shared" si="1"/>
         <v>button28 = findViewById(R.id.button28);</v>
       </c>
-      <c r="D17" t="str">
-        <f t="shared" si="2"/>
-        <v>button28.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button28.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1940,12 +1947,12 @@
         <f t="shared" si="1"/>
         <v>button29 = findViewById(R.id.button29);</v>
       </c>
-      <c r="D18" t="str">
-        <f t="shared" si="2"/>
-        <v>button29.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button29.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1957,12 +1964,12 @@
         <f t="shared" si="1"/>
         <v>button31 = findViewById(R.id.button31);</v>
       </c>
-      <c r="D19" t="str">
-        <f t="shared" si="2"/>
-        <v>button31.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button31.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1974,12 +1981,12 @@
         <f t="shared" si="1"/>
         <v>button32 = findViewById(R.id.button32);</v>
       </c>
-      <c r="D20" t="str">
-        <f t="shared" si="2"/>
-        <v>button32.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button32.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1991,12 +1998,12 @@
         <f t="shared" si="1"/>
         <v>button33 = findViewById(R.id.button33);</v>
       </c>
-      <c r="D21" t="str">
-        <f t="shared" si="2"/>
-        <v>button33.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button33.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2008,12 +2015,12 @@
         <f t="shared" si="1"/>
         <v>button34 = findViewById(R.id.button34);</v>
       </c>
-      <c r="D22" t="str">
-        <f t="shared" si="2"/>
-        <v>button34.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button34.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2025,12 +2032,12 @@
         <f t="shared" si="1"/>
         <v>button35 = findViewById(R.id.button35);</v>
       </c>
-      <c r="D23" t="str">
-        <f t="shared" si="2"/>
-        <v>button35.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button35.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2042,12 +2049,12 @@
         <f t="shared" si="1"/>
         <v>button36 = findViewById(R.id.button36);</v>
       </c>
-      <c r="D24" t="str">
-        <f t="shared" si="2"/>
-        <v>button36.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button36.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2059,12 +2066,12 @@
         <f t="shared" si="1"/>
         <v>button37 = findViewById(R.id.button37);</v>
       </c>
-      <c r="D25" t="str">
-        <f t="shared" si="2"/>
-        <v>button37.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button37.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2076,12 +2083,12 @@
         <f t="shared" si="1"/>
         <v>button38 = findViewById(R.id.button38);</v>
       </c>
-      <c r="D26" t="str">
-        <f t="shared" si="2"/>
-        <v>button38.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button38.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2093,12 +2100,12 @@
         <f t="shared" si="1"/>
         <v>button39 = findViewById(R.id.button39);</v>
       </c>
-      <c r="D27" t="str">
-        <f t="shared" si="2"/>
-        <v>button39.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button39.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2110,12 +2117,12 @@
         <f t="shared" si="1"/>
         <v>button41 = findViewById(R.id.button41);</v>
       </c>
-      <c r="D28" t="str">
-        <f t="shared" si="2"/>
-        <v>button41.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button41.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2127,12 +2134,12 @@
         <f t="shared" si="1"/>
         <v>button42 = findViewById(R.id.button42);</v>
       </c>
-      <c r="D29" t="str">
-        <f t="shared" si="2"/>
-        <v>button42.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button42.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2144,12 +2151,12 @@
         <f t="shared" si="1"/>
         <v>button43 = findViewById(R.id.button43);</v>
       </c>
-      <c r="D30" t="str">
-        <f t="shared" si="2"/>
-        <v>button43.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button43.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2161,12 +2168,12 @@
         <f t="shared" si="1"/>
         <v>button44 = findViewById(R.id.button44);</v>
       </c>
-      <c r="D31" t="str">
-        <f t="shared" si="2"/>
-        <v>button44.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button44.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2178,12 +2185,12 @@
         <f t="shared" si="1"/>
         <v>button45 = findViewById(R.id.button45);</v>
       </c>
-      <c r="D32" t="str">
-        <f t="shared" si="2"/>
-        <v>button45.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button45.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2195,12 +2202,12 @@
         <f t="shared" si="1"/>
         <v>button46 = findViewById(R.id.button46);</v>
       </c>
-      <c r="D33" t="str">
-        <f t="shared" si="2"/>
-        <v>button46.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button46.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2212,12 +2219,12 @@
         <f t="shared" si="1"/>
         <v>button47 = findViewById(R.id.button47);</v>
       </c>
-      <c r="D34" t="str">
-        <f t="shared" si="2"/>
-        <v>button47.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button47.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2229,12 +2236,12 @@
         <f t="shared" si="1"/>
         <v>button48 = findViewById(R.id.button48);</v>
       </c>
-      <c r="D35" t="str">
-        <f t="shared" si="2"/>
-        <v>button48.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button48.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2246,12 +2253,12 @@
         <f t="shared" si="1"/>
         <v>button49 = findViewById(R.id.button49);</v>
       </c>
-      <c r="D36" t="str">
-        <f t="shared" si="2"/>
-        <v>button49.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button49.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2263,12 +2270,12 @@
         <f t="shared" si="1"/>
         <v>button51 = findViewById(R.id.button51);</v>
       </c>
-      <c r="D37" t="str">
-        <f t="shared" si="2"/>
-        <v>button51.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button51.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2280,12 +2287,12 @@
         <f t="shared" si="1"/>
         <v>button52 = findViewById(R.id.button52);</v>
       </c>
-      <c r="D38" t="str">
-        <f t="shared" si="2"/>
-        <v>button52.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button52.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2297,12 +2304,12 @@
         <f t="shared" si="1"/>
         <v>button53 = findViewById(R.id.button53);</v>
       </c>
-      <c r="D39" t="str">
-        <f t="shared" si="2"/>
-        <v>button53.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button53.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2314,12 +2321,12 @@
         <f t="shared" si="1"/>
         <v>button54 = findViewById(R.id.button54);</v>
       </c>
-      <c r="D40" t="str">
-        <f t="shared" si="2"/>
-        <v>button54.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button54.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2331,12 +2338,12 @@
         <f t="shared" si="1"/>
         <v>button55 = findViewById(R.id.button55);</v>
       </c>
-      <c r="D41" t="str">
-        <f t="shared" si="2"/>
-        <v>button55.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button55.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2348,12 +2355,12 @@
         <f t="shared" si="1"/>
         <v>button56 = findViewById(R.id.button56);</v>
       </c>
-      <c r="D42" t="str">
-        <f t="shared" si="2"/>
-        <v>button56.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button56.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2365,12 +2372,12 @@
         <f t="shared" si="1"/>
         <v>button57 = findViewById(R.id.button57);</v>
       </c>
-      <c r="D43" t="str">
-        <f t="shared" si="2"/>
-        <v>button57.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button57.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2382,12 +2389,12 @@
         <f t="shared" si="1"/>
         <v>button58 = findViewById(R.id.button58);</v>
       </c>
-      <c r="D44" t="str">
-        <f t="shared" si="2"/>
-        <v>button58.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button58.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2399,12 +2406,12 @@
         <f t="shared" si="1"/>
         <v>button59 = findViewById(R.id.button59);</v>
       </c>
-      <c r="D45" t="str">
-        <f t="shared" si="2"/>
-        <v>button59.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button59.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2416,12 +2423,12 @@
         <f t="shared" si="1"/>
         <v>button61 = findViewById(R.id.button61);</v>
       </c>
-      <c r="D46" t="str">
-        <f t="shared" si="2"/>
-        <v>button61.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button61.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2433,12 +2440,12 @@
         <f t="shared" si="1"/>
         <v>button62 = findViewById(R.id.button62);</v>
       </c>
-      <c r="D47" t="str">
-        <f t="shared" si="2"/>
-        <v>button62.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button62.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2450,12 +2457,12 @@
         <f t="shared" si="1"/>
         <v>button63 = findViewById(R.id.button63);</v>
       </c>
-      <c r="D48" t="str">
-        <f t="shared" si="2"/>
-        <v>button63.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button63.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2467,12 +2474,12 @@
         <f t="shared" si="1"/>
         <v>button64 = findViewById(R.id.button64);</v>
       </c>
-      <c r="D49" t="str">
-        <f t="shared" si="2"/>
-        <v>button64.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button64.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2484,12 +2491,12 @@
         <f t="shared" si="1"/>
         <v>button65 = findViewById(R.id.button65);</v>
       </c>
-      <c r="D50" t="str">
-        <f t="shared" si="2"/>
-        <v>button65.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button65.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2501,12 +2508,12 @@
         <f t="shared" si="1"/>
         <v>button66 = findViewById(R.id.button66);</v>
       </c>
-      <c r="D51" t="str">
-        <f t="shared" si="2"/>
-        <v>button66.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button66.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2518,12 +2525,12 @@
         <f t="shared" si="1"/>
         <v>button67 = findViewById(R.id.button67);</v>
       </c>
-      <c r="D52" t="str">
-        <f t="shared" si="2"/>
-        <v>button67.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button67.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2535,12 +2542,12 @@
         <f t="shared" si="1"/>
         <v>button68 = findViewById(R.id.button68);</v>
       </c>
-      <c r="D53" t="str">
-        <f t="shared" si="2"/>
-        <v>button68.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button68.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2552,12 +2559,12 @@
         <f t="shared" si="1"/>
         <v>button69 = findViewById(R.id.button69);</v>
       </c>
-      <c r="D54" t="str">
-        <f t="shared" si="2"/>
-        <v>button69.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button69.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2569,12 +2576,12 @@
         <f t="shared" si="1"/>
         <v>button71 = findViewById(R.id.button71);</v>
       </c>
-      <c r="D55" t="str">
-        <f t="shared" si="2"/>
-        <v>button71.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button71.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2586,12 +2593,12 @@
         <f t="shared" si="1"/>
         <v>button72 = findViewById(R.id.button72);</v>
       </c>
-      <c r="D56" t="str">
-        <f t="shared" si="2"/>
-        <v>button72.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button72.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2603,12 +2610,12 @@
         <f t="shared" si="1"/>
         <v>button73 = findViewById(R.id.button73);</v>
       </c>
-      <c r="D57" t="str">
-        <f t="shared" si="2"/>
-        <v>button73.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button73.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2620,12 +2627,12 @@
         <f t="shared" si="1"/>
         <v>button74 = findViewById(R.id.button74);</v>
       </c>
-      <c r="D58" t="str">
-        <f t="shared" si="2"/>
-        <v>button74.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button74.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2637,12 +2644,12 @@
         <f t="shared" si="1"/>
         <v>button75 = findViewById(R.id.button75);</v>
       </c>
-      <c r="D59" t="str">
-        <f t="shared" si="2"/>
-        <v>button75.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button75.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2654,12 +2661,12 @@
         <f t="shared" si="1"/>
         <v>button76 = findViewById(R.id.button76);</v>
       </c>
-      <c r="D60" t="str">
-        <f t="shared" si="2"/>
-        <v>button76.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button76.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2671,12 +2678,12 @@
         <f t="shared" si="1"/>
         <v>button77 = findViewById(R.id.button77);</v>
       </c>
-      <c r="D61" t="str">
-        <f t="shared" si="2"/>
-        <v>button77.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button77.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2688,12 +2695,12 @@
         <f t="shared" si="1"/>
         <v>button78 = findViewById(R.id.button78);</v>
       </c>
-      <c r="D62" t="str">
-        <f t="shared" si="2"/>
-        <v>button78.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button78.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2705,12 +2712,12 @@
         <f t="shared" si="1"/>
         <v>button79 = findViewById(R.id.button79);</v>
       </c>
-      <c r="D63" t="str">
-        <f t="shared" si="2"/>
-        <v>button79.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button79.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2722,12 +2729,12 @@
         <f t="shared" si="1"/>
         <v>button81 = findViewById(R.id.button81);</v>
       </c>
-      <c r="D64" t="str">
-        <f t="shared" si="2"/>
-        <v>button81.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button81.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2739,12 +2746,12 @@
         <f t="shared" si="1"/>
         <v>button82 = findViewById(R.id.button82);</v>
       </c>
-      <c r="D65" t="str">
-        <f t="shared" si="2"/>
-        <v>button82.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>button82.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2756,12 +2763,12 @@
         <f t="shared" ref="C66:C81" si="4">A66&amp;" = findViewById(R.id."&amp;A66&amp;");"</f>
         <v>button83 = findViewById(R.id.button83);</v>
       </c>
-      <c r="D66" t="str">
-        <f t="shared" ref="D66:D81" si="5">A66&amp;".setBackgroundResource(android.R.drawable.btn_default);"</f>
-        <v>button83.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="10" t="str">
+        <f t="shared" ref="D66:D81" si="5">A66&amp;".getBackground().setColorFilter(null);"</f>
+        <v>button83.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2773,12 +2780,12 @@
         <f t="shared" si="4"/>
         <v>button84 = findViewById(R.id.button84);</v>
       </c>
-      <c r="D67" t="str">
+      <c r="D67" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button84.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button84.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2790,12 +2797,12 @@
         <f t="shared" si="4"/>
         <v>button85 = findViewById(R.id.button85);</v>
       </c>
-      <c r="D68" t="str">
+      <c r="D68" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button85.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button85.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2807,12 +2814,12 @@
         <f t="shared" si="4"/>
         <v>button86 = findViewById(R.id.button86);</v>
       </c>
-      <c r="D69" t="str">
+      <c r="D69" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button86.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button86.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2824,12 +2831,12 @@
         <f t="shared" si="4"/>
         <v>button87 = findViewById(R.id.button87);</v>
       </c>
-      <c r="D70" t="str">
+      <c r="D70" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button87.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button87.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2841,12 +2848,12 @@
         <f t="shared" si="4"/>
         <v>button88 = findViewById(R.id.button88);</v>
       </c>
-      <c r="D71" t="str">
+      <c r="D71" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button88.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button88.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2858,12 +2865,12 @@
         <f t="shared" si="4"/>
         <v>button89 = findViewById(R.id.button89);</v>
       </c>
-      <c r="D72" t="str">
+      <c r="D72" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button89.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button89.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2875,12 +2882,12 @@
         <f t="shared" si="4"/>
         <v>button91 = findViewById(R.id.button91);</v>
       </c>
-      <c r="D73" t="str">
+      <c r="D73" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button91.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button91.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2892,12 +2899,12 @@
         <f t="shared" si="4"/>
         <v>button92 = findViewById(R.id.button92);</v>
       </c>
-      <c r="D74" t="str">
+      <c r="D74" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button92.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button92.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2909,12 +2916,12 @@
         <f t="shared" si="4"/>
         <v>button93 = findViewById(R.id.button93);</v>
       </c>
-      <c r="D75" t="str">
+      <c r="D75" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button93.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button93.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2926,12 +2933,12 @@
         <f t="shared" si="4"/>
         <v>button94 = findViewById(R.id.button94);</v>
       </c>
-      <c r="D76" t="str">
+      <c r="D76" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button94.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button94.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2943,12 +2950,12 @@
         <f t="shared" si="4"/>
         <v>button95 = findViewById(R.id.button95);</v>
       </c>
-      <c r="D77" t="str">
+      <c r="D77" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button95.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button95.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2960,12 +2967,12 @@
         <f t="shared" si="4"/>
         <v>button96 = findViewById(R.id.button96);</v>
       </c>
-      <c r="D78" t="str">
+      <c r="D78" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button96.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button96.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2977,12 +2984,12 @@
         <f t="shared" si="4"/>
         <v>button97 = findViewById(R.id.button97);</v>
       </c>
-      <c r="D79" t="str">
+      <c r="D79" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button97.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button97.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2994,12 +3001,12 @@
         <f t="shared" si="4"/>
         <v>button98 = findViewById(R.id.button98);</v>
       </c>
-      <c r="D80" t="str">
+      <c r="D80" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button98.setBackgroundResource(android.R.drawable.btn_default);</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>button98.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -3011,9 +3018,9 @@
         <f t="shared" si="4"/>
         <v>button99 = findViewById(R.id.button99);</v>
       </c>
-      <c r="D81" t="str">
+      <c r="D81" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>button99.setBackgroundResource(android.R.drawable.btn_default);</v>
+        <v>button99.getBackground().setColorFilter(null);</v>
       </c>
     </row>
   </sheetData>
@@ -3024,18 +3031,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="9" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="9" t="s">
         <v>81</v>
       </c>
@@ -3048,7 +3055,7 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3077,11 +3084,11 @@
         <v>3</v>
       </c>
       <c r="K2" t="str">
-        <f>"public void button"&amp;A12&amp;" (View view){ game"&amp;A2&amp;"["&amp;A2&amp;"]["&amp;A22&amp;"]=currentPlayer; button"&amp;A12&amp;".setEnabled(false); activeGame"&amp;A22&amp;"();}"</f>
+        <f>"public void button"&amp;A12&amp;" (View view){ game"&amp;A2&amp;"["&amp;LEFT(A22,1)&amp;"]["&amp;RIGHT(A22,1)&amp;"]=currentPlayer; button"&amp;A12&amp;".setEnabled(false); activeGame"&amp;A32&amp;"();}"</f>
         <v>public void button11 (View view){ game1[1][1]=currentPlayer; button11.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:S10" si="0">"public void button"&amp;B12&amp;" (View view){ game"&amp;B2&amp;"["&amp;B2&amp;"]["&amp;B22&amp;"]=currentPlayer; button"&amp;B12&amp;".setEnabled(false); activeGame"&amp;B22&amp;"();}"</f>
+        <f t="shared" ref="L2:S10" si="0">"public void button"&amp;B12&amp;" (View view){ game"&amp;B2&amp;"["&amp;LEFT(B22,1)&amp;"]["&amp;RIGHT(B22,1)&amp;"]=currentPlayer; button"&amp;B12&amp;".setEnabled(false); activeGame"&amp;B32&amp;"();}"</f>
         <v>public void button12 (View view){ game1[1][2]=currentPlayer; button12.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="M2" t="str">
@@ -3090,30 +3097,30 @@
       </c>
       <c r="N2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button14 (View view){ game2[2][1]=currentPlayer; button14.setEnabled(false); activeGame1();}</v>
+        <v>public void button14 (View view){ game2[1][1]=currentPlayer; button14.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="O2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button15 (View view){ game2[2][2]=currentPlayer; button15.setEnabled(false); activeGame2();}</v>
+        <v>public void button15 (View view){ game2[1][2]=currentPlayer; button15.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="P2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button16 (View view){ game2[2][3]=currentPlayer; button16.setEnabled(false); activeGame3();}</v>
+        <v>public void button16 (View view){ game2[1][3]=currentPlayer; button16.setEnabled(false); activeGame3();}</v>
       </c>
       <c r="Q2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button17 (View view){ game3[3][1]=currentPlayer; button17.setEnabled(false); activeGame1();}</v>
+        <v>public void button17 (View view){ game3[1][1]=currentPlayer; button17.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="R2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button18 (View view){ game3[3][2]=currentPlayer; button18.setEnabled(false); activeGame2();}</v>
+        <v>public void button18 (View view){ game3[1][2]=currentPlayer; button18.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="S2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button19 (View view){ game3[3][3]=currentPlayer; button19.setEnabled(false); activeGame3();}</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button19 (View view){ game3[1][3]=currentPlayer; button19.setEnabled(false); activeGame3();}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3142,43 +3149,43 @@
         <v>3</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K10" si="1">"public void button"&amp;A13&amp;" (View view){ game"&amp;A3&amp;"["&amp;A3&amp;"]["&amp;A23&amp;"]=currentPlayer; button"&amp;A13&amp;".setEnabled(false); activeGame"&amp;A23&amp;"();}"</f>
-        <v>public void button21 (View view){ game1[1][4]=currentPlayer; button21.setEnabled(false); activeGame4();}</v>
+        <f t="shared" ref="K3:K10" si="1">"public void button"&amp;A13&amp;" (View view){ game"&amp;A3&amp;"["&amp;LEFT(A23,1)&amp;"]["&amp;RIGHT(A23,1)&amp;"]=currentPlayer; button"&amp;A13&amp;".setEnabled(false); activeGame"&amp;A33&amp;"();}"</f>
+        <v>public void button21 (View view){ game1[2][1]=currentPlayer; button21.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button22 (View view){ game1[1][5]=currentPlayer; button22.setEnabled(false); activeGame5();}</v>
+        <v>public void button22 (View view){ game1[2][2]=currentPlayer; button22.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button23 (View view){ game1[1][6]=currentPlayer; button23.setEnabled(false); activeGame6();}</v>
+        <v>public void button23 (View view){ game1[2][3]=currentPlayer; button23.setEnabled(false); activeGame6();}</v>
       </c>
       <c r="N3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button24 (View view){ game2[2][4]=currentPlayer; button24.setEnabled(false); activeGame4();}</v>
+        <v>public void button24 (View view){ game2[2][1]=currentPlayer; button24.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button25 (View view){ game2[2][5]=currentPlayer; button25.setEnabled(false); activeGame5();}</v>
+        <v>public void button25 (View view){ game2[2][2]=currentPlayer; button25.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button26 (View view){ game2[2][6]=currentPlayer; button26.setEnabled(false); activeGame6();}</v>
+        <v>public void button26 (View view){ game2[2][3]=currentPlayer; button26.setEnabled(false); activeGame6();}</v>
       </c>
       <c r="Q3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button27 (View view){ game3[3][4]=currentPlayer; button27.setEnabled(false); activeGame4();}</v>
+        <v>public void button27 (View view){ game3[2][1]=currentPlayer; button27.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button28 (View view){ game3[3][5]=currentPlayer; button28.setEnabled(false); activeGame5();}</v>
+        <v>public void button28 (View view){ game3[2][2]=currentPlayer; button28.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="S3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button29 (View view){ game3[3][6]=currentPlayer; button29.setEnabled(false); activeGame6();}</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button29 (View view){ game3[2][3]=currentPlayer; button29.setEnabled(false); activeGame6();}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3208,42 +3215,42 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>public void button31 (View view){ game1[1][7]=currentPlayer; button31.setEnabled(false); activeGame7();}</v>
+        <v>public void button31 (View view){ game1[3][1]=currentPlayer; button31.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button32 (View view){ game1[1][8]=currentPlayer; button32.setEnabled(false); activeGame8();}</v>
+        <v>public void button32 (View view){ game1[3][2]=currentPlayer; button32.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button33 (View view){ game1[1][9]=currentPlayer; button33.setEnabled(false); activeGame9();}</v>
+        <v>public void button33 (View view){ game1[3][3]=currentPlayer; button33.setEnabled(false); activeGame9();}</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button34 (View view){ game2[2][7]=currentPlayer; button34.setEnabled(false); activeGame7();}</v>
+        <v>public void button34 (View view){ game2[3][1]=currentPlayer; button34.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button35 (View view){ game2[2][8]=currentPlayer; button35.setEnabled(false); activeGame8();}</v>
+        <v>public void button35 (View view){ game2[3][2]=currentPlayer; button35.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button36 (View view){ game2[2][9]=currentPlayer; button36.setEnabled(false); activeGame9();}</v>
+        <v>public void button36 (View view){ game2[3][3]=currentPlayer; button36.setEnabled(false); activeGame9();}</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button37 (View view){ game3[3][7]=currentPlayer; button37.setEnabled(false); activeGame7();}</v>
+        <v>public void button37 (View view){ game3[3][1]=currentPlayer; button37.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button38 (View view){ game3[3][8]=currentPlayer; button38.setEnabled(false); activeGame8();}</v>
+        <v>public void button38 (View view){ game3[3][2]=currentPlayer; button38.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="S4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button39 (View view){ game3[3][9]=currentPlayer; button39.setEnabled(false); activeGame9();}</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button39 (View view){ game3[3][3]=currentPlayer; button39.setEnabled(false); activeGame9();}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3273,42 +3280,42 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>public void button41 (View view){ game4[4][1]=currentPlayer; button41.setEnabled(false); activeGame1();}</v>
+        <v>public void button41 (View view){ game4[1][1]=currentPlayer; button41.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button42 (View view){ game4[4][2]=currentPlayer; button42.setEnabled(false); activeGame2();}</v>
+        <v>public void button42 (View view){ game4[1][2]=currentPlayer; button42.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button43 (View view){ game4[4][3]=currentPlayer; button43.setEnabled(false); activeGame3();}</v>
+        <v>public void button43 (View view){ game4[1][3]=currentPlayer; button43.setEnabled(false); activeGame3();}</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button44 (View view){ game5[5][1]=currentPlayer; button44.setEnabled(false); activeGame1();}</v>
+        <v>public void button44 (View view){ game5[1][1]=currentPlayer; button44.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button45 (View view){ game5[5][2]=currentPlayer; button45.setEnabled(false); activeGame2();}</v>
+        <v>public void button45 (View view){ game5[1][2]=currentPlayer; button45.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button46 (View view){ game5[5][3]=currentPlayer; button46.setEnabled(false); activeGame3();}</v>
+        <v>public void button46 (View view){ game5[1][3]=currentPlayer; button46.setEnabled(false); activeGame3();}</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button47 (View view){ game6[6][1]=currentPlayer; button47.setEnabled(false); activeGame1();}</v>
+        <v>public void button47 (View view){ game6[1][1]=currentPlayer; button47.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button48 (View view){ game6[6][2]=currentPlayer; button48.setEnabled(false); activeGame2();}</v>
+        <v>public void button48 (View view){ game6[1][2]=currentPlayer; button48.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button49 (View view){ game6[6][3]=currentPlayer; button49.setEnabled(false); activeGame3();}</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button49 (View view){ game6[1][3]=currentPlayer; button49.setEnabled(false); activeGame3();}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3338,42 +3345,42 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>public void button51 (View view){ game4[4][4]=currentPlayer; button51.setEnabled(false); activeGame4();}</v>
+        <v>public void button51 (View view){ game4[2][1]=currentPlayer; button51.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button52 (View view){ game4[4][5]=currentPlayer; button52.setEnabled(false); activeGame5();}</v>
+        <v>public void button52 (View view){ game4[2][2]=currentPlayer; button52.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button53 (View view){ game4[4][6]=currentPlayer; button53.setEnabled(false); activeGame6();}</v>
+        <v>public void button53 (View view){ game4[2][3]=currentPlayer; button53.setEnabled(false); activeGame6();}</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button54 (View view){ game5[5][4]=currentPlayer; button54.setEnabled(false); activeGame4();}</v>
+        <v>public void button54 (View view){ game5[2][1]=currentPlayer; button54.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button55 (View view){ game5[5][5]=currentPlayer; button55.setEnabled(false); activeGame5();}</v>
+        <v>public void button55 (View view){ game5[2][2]=currentPlayer; button55.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button56 (View view){ game5[5][6]=currentPlayer; button56.setEnabled(false); activeGame6();}</v>
+        <v>public void button56 (View view){ game5[2][3]=currentPlayer; button56.setEnabled(false); activeGame6();}</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button57 (View view){ game6[6][4]=currentPlayer; button57.setEnabled(false); activeGame4();}</v>
+        <v>public void button57 (View view){ game6[2][1]=currentPlayer; button57.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button58 (View view){ game6[6][5]=currentPlayer; button58.setEnabled(false); activeGame5();}</v>
+        <v>public void button58 (View view){ game6[2][2]=currentPlayer; button58.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button59 (View view){ game6[6][6]=currentPlayer; button59.setEnabled(false); activeGame6();}</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button59 (View view){ game6[2][3]=currentPlayer; button59.setEnabled(false); activeGame6();}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>4</v>
       </c>
@@ -3403,42 +3410,42 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>public void button61 (View view){ game4[4][7]=currentPlayer; button61.setEnabled(false); activeGame7();}</v>
+        <v>public void button61 (View view){ game4[3][1]=currentPlayer; button61.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button62 (View view){ game4[4][8]=currentPlayer; button62.setEnabled(false); activeGame8();}</v>
+        <v>public void button62 (View view){ game4[3][2]=currentPlayer; button62.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button63 (View view){ game4[4][9]=currentPlayer; button63.setEnabled(false); activeGame9();}</v>
+        <v>public void button63 (View view){ game4[3][3]=currentPlayer; button63.setEnabled(false); activeGame9();}</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button64 (View view){ game5[5][7]=currentPlayer; button64.setEnabled(false); activeGame7();}</v>
+        <v>public void button64 (View view){ game5[3][1]=currentPlayer; button64.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button65 (View view){ game5[5][8]=currentPlayer; button65.setEnabled(false); activeGame8();}</v>
+        <v>public void button65 (View view){ game5[3][2]=currentPlayer; button65.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button66 (View view){ game5[5][9]=currentPlayer; button66.setEnabled(false); activeGame9();}</v>
+        <v>public void button66 (View view){ game5[3][3]=currentPlayer; button66.setEnabled(false); activeGame9();}</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button67 (View view){ game6[6][7]=currentPlayer; button67.setEnabled(false); activeGame7();}</v>
+        <v>public void button67 (View view){ game6[3][1]=currentPlayer; button67.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button68 (View view){ game6[6][8]=currentPlayer; button68.setEnabled(false); activeGame8();}</v>
+        <v>public void button68 (View view){ game6[3][2]=currentPlayer; button68.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button69 (View view){ game6[6][9]=currentPlayer; button69.setEnabled(false); activeGame9();}</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button69 (View view){ game6[3][3]=currentPlayer; button69.setEnabled(false); activeGame9();}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3468,42 +3475,42 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>public void button71 (View view){ game7[7][1]=currentPlayer; button71.setEnabled(false); activeGame1();}</v>
+        <v>public void button71 (View view){ game7[1][1]=currentPlayer; button71.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button72 (View view){ game7[7][2]=currentPlayer; button72.setEnabled(false); activeGame2();}</v>
+        <v>public void button72 (View view){ game7[1][2]=currentPlayer; button72.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button73 (View view){ game7[7][3]=currentPlayer; button73.setEnabled(false); activeGame3();}</v>
+        <v>public void button73 (View view){ game7[1][3]=currentPlayer; button73.setEnabled(false); activeGame3();}</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button74 (View view){ game8[8][1]=currentPlayer; button74.setEnabled(false); activeGame1();}</v>
+        <v>public void button74 (View view){ game8[1][1]=currentPlayer; button74.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button75 (View view){ game8[8][2]=currentPlayer; button75.setEnabled(false); activeGame2();}</v>
+        <v>public void button75 (View view){ game8[1][2]=currentPlayer; button75.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button76 (View view){ game8[8][3]=currentPlayer; button76.setEnabled(false); activeGame3();}</v>
+        <v>public void button76 (View view){ game8[1][3]=currentPlayer; button76.setEnabled(false); activeGame3();}</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button77 (View view){ game9[9][1]=currentPlayer; button77.setEnabled(false); activeGame1();}</v>
+        <v>public void button77 (View view){ game9[1][1]=currentPlayer; button77.setEnabled(false); activeGame1();}</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button78 (View view){ game9[9][2]=currentPlayer; button78.setEnabled(false); activeGame2();}</v>
+        <v>public void button78 (View view){ game9[1][2]=currentPlayer; button78.setEnabled(false); activeGame2();}</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button79 (View view){ game9[9][3]=currentPlayer; button79.setEnabled(false); activeGame3();}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button79 (View view){ game9[1][3]=currentPlayer; button79.setEnabled(false); activeGame3();}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3533,42 +3540,42 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>public void button81 (View view){ game7[7][4]=currentPlayer; button81.setEnabled(false); activeGame4();}</v>
+        <v>public void button81 (View view){ game7[2][1]=currentPlayer; button81.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button82 (View view){ game7[7][5]=currentPlayer; button82.setEnabled(false); activeGame5();}</v>
+        <v>public void button82 (View view){ game7[2][2]=currentPlayer; button82.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button83 (View view){ game7[7][6]=currentPlayer; button83.setEnabled(false); activeGame6();}</v>
+        <v>public void button83 (View view){ game7[2][3]=currentPlayer; button83.setEnabled(false); activeGame6();}</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button84 (View view){ game8[8][4]=currentPlayer; button84.setEnabled(false); activeGame4();}</v>
+        <v>public void button84 (View view){ game8[2][1]=currentPlayer; button84.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button85 (View view){ game8[8][5]=currentPlayer; button85.setEnabled(false); activeGame5();}</v>
+        <v>public void button85 (View view){ game8[2][2]=currentPlayer; button85.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button86 (View view){ game8[8][6]=currentPlayer; button86.setEnabled(false); activeGame6();}</v>
+        <v>public void button86 (View view){ game8[2][3]=currentPlayer; button86.setEnabled(false); activeGame6();}</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button87 (View view){ game9[9][4]=currentPlayer; button87.setEnabled(false); activeGame4();}</v>
+        <v>public void button87 (View view){ game9[2][1]=currentPlayer; button87.setEnabled(false); activeGame4();}</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button88 (View view){ game9[9][5]=currentPlayer; button88.setEnabled(false); activeGame5();}</v>
+        <v>public void button88 (View view){ game9[2][2]=currentPlayer; button88.setEnabled(false); activeGame5();}</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button89 (View view){ game9[9][6]=currentPlayer; button89.setEnabled(false); activeGame6();}</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button89 (View view){ game9[2][3]=currentPlayer; button89.setEnabled(false); activeGame6();}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>7</v>
       </c>
@@ -3598,42 +3605,42 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>public void button91 (View view){ game7[7][7]=currentPlayer; button91.setEnabled(false); activeGame7();}</v>
+        <v>public void button91 (View view){ game7[3][1]=currentPlayer; button91.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button92 (View view){ game7[7][8]=currentPlayer; button92.setEnabled(false); activeGame8();}</v>
+        <v>public void button92 (View view){ game7[3][2]=currentPlayer; button92.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button93 (View view){ game7[7][9]=currentPlayer; button93.setEnabled(false); activeGame9();}</v>
+        <v>public void button93 (View view){ game7[3][3]=currentPlayer; button93.setEnabled(false); activeGame9();}</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button94 (View view){ game8[8][7]=currentPlayer; button94.setEnabled(false); activeGame7();}</v>
+        <v>public void button94 (View view){ game8[3][1]=currentPlayer; button94.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button95 (View view){ game8[8][8]=currentPlayer; button95.setEnabled(false); activeGame8();}</v>
+        <v>public void button95 (View view){ game8[3][2]=currentPlayer; button95.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button96 (View view){ game8[8][9]=currentPlayer; button96.setEnabled(false); activeGame9();}</v>
+        <v>public void button96 (View view){ game8[3][3]=currentPlayer; button96.setEnabled(false); activeGame9();}</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button97 (View view){ game9[9][7]=currentPlayer; button97.setEnabled(false); activeGame7();}</v>
+        <v>public void button97 (View view){ game9[3][1]=currentPlayer; button97.setEnabled(false); activeGame7();}</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button98 (View view){ game9[9][8]=currentPlayer; button98.setEnabled(false); activeGame8();}</v>
+        <v>public void button98 (View view){ game9[3][2]=currentPlayer; button98.setEnabled(false); activeGame8();}</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button99 (View view){ game9[9][9]=currentPlayer; button99.setEnabled(false); activeGame9();}</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>public void button99 (View view){ game9[3][3]=currentPlayer; button99.setEnabled(false); activeGame9();}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="9" t="s">
         <v>82</v>
       </c>
@@ -3646,7 +3653,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3674,8 +3681,44 @@
       <c r="I12">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K12" t="str">
+        <f>"button"&amp;A12&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button11.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" ref="L12:S12" si="2">"button"&amp;B12&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button12.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="2"/>
+        <v>button13.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="2"/>
+        <v>button14.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="2"/>
+        <v>button15.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>button16.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="2"/>
+        <v>button17.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="2"/>
+        <v>button18.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="2"/>
+        <v>button19.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>21</v>
       </c>
@@ -3703,8 +3746,44 @@
       <c r="I13">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K13" t="str">
+        <f t="shared" ref="K13:K20" si="3">"button"&amp;A13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button21.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" ref="L13:L20" si="4">"button"&amp;B13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button22.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" ref="M13:M20" si="5">"button"&amp;C13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button23.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" ref="N13:N20" si="6">"button"&amp;D13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button24.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" ref="O13:O20" si="7">"button"&amp;E13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button25.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" ref="P13:P20" si="8">"button"&amp;F13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button26.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" ref="Q13:Q20" si="9">"button"&amp;G13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button27.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R13" t="str">
+        <f t="shared" ref="R13:R20" si="10">"button"&amp;H13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button28.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" ref="S13:S20" si="11">"button"&amp;I13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
+        <v>button29.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>31</v>
       </c>
@@ -3732,8 +3811,44 @@
       <c r="I14">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K14" t="str">
+        <f t="shared" si="3"/>
+        <v>button31.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="4"/>
+        <v>button32.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="5"/>
+        <v>button33.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="6"/>
+        <v>button34.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="7"/>
+        <v>button35.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="8"/>
+        <v>button36.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="9"/>
+        <v>button37.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R14" t="str">
+        <f t="shared" si="10"/>
+        <v>button38.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="11"/>
+        <v>button39.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>41</v>
       </c>
@@ -3761,8 +3876,44 @@
       <c r="I15">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K15" t="str">
+        <f t="shared" si="3"/>
+        <v>button41.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="4"/>
+        <v>button42.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="5"/>
+        <v>button43.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="6"/>
+        <v>button44.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="7"/>
+        <v>button45.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="8"/>
+        <v>button46.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="9"/>
+        <v>button47.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R15" t="str">
+        <f t="shared" si="10"/>
+        <v>button48.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="11"/>
+        <v>button49.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>51</v>
       </c>
@@ -3790,8 +3941,44 @@
       <c r="I16">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" t="str">
+        <f t="shared" si="3"/>
+        <v>button51.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="4"/>
+        <v>button52.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="5"/>
+        <v>button53.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="6"/>
+        <v>button54.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="7"/>
+        <v>button55.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="8"/>
+        <v>button56.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="9"/>
+        <v>button57.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R16" t="str">
+        <f t="shared" si="10"/>
+        <v>button58.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="11"/>
+        <v>button59.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>61</v>
       </c>
@@ -3819,8 +4006,44 @@
       <c r="I17">
         <v>69</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" t="str">
+        <f t="shared" si="3"/>
+        <v>button61.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="4"/>
+        <v>button62.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="5"/>
+        <v>button63.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="6"/>
+        <v>button64.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="7"/>
+        <v>button65.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="8"/>
+        <v>button66.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="9"/>
+        <v>button67.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R17" t="str">
+        <f t="shared" si="10"/>
+        <v>button68.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S17" t="str">
+        <f t="shared" si="11"/>
+        <v>button69.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>71</v>
       </c>
@@ -3848,8 +4071,44 @@
       <c r="I18">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f t="shared" si="3"/>
+        <v>button71.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="4"/>
+        <v>button72.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="5"/>
+        <v>button73.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="6"/>
+        <v>button74.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="7"/>
+        <v>button75.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="8"/>
+        <v>button76.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="9"/>
+        <v>button77.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R18" t="str">
+        <f t="shared" si="10"/>
+        <v>button78.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" si="11"/>
+        <v>button79.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>81</v>
       </c>
@@ -3877,8 +4136,44 @@
       <c r="I19">
         <v>89</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19" t="str">
+        <f t="shared" si="3"/>
+        <v>button81.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="4"/>
+        <v>button82.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="5"/>
+        <v>button83.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="6"/>
+        <v>button84.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="7"/>
+        <v>button85.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="8"/>
+        <v>button86.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="9"/>
+        <v>button87.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R19" t="str">
+        <f t="shared" si="10"/>
+        <v>button88.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S19" t="str">
+        <f t="shared" si="11"/>
+        <v>button89.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>91</v>
       </c>
@@ -3906,265 +4201,562 @@
       <c r="I20">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" t="str">
+        <f t="shared" si="3"/>
+        <v>button91.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="4"/>
+        <v>button92.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="5"/>
+        <v>button93.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="6"/>
+        <v>button94.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="7"/>
+        <v>button95.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="8"/>
+        <v>button96.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="9"/>
+        <v>button97.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="R20" t="str">
+        <f t="shared" si="10"/>
+        <v>button98.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+      <c r="S20" t="str">
+        <f t="shared" si="11"/>
+        <v>button99.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>11</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>13</v>
+      </c>
+      <c r="G22">
+        <v>11</v>
+      </c>
+      <c r="H22">
+        <v>12</v>
+      </c>
+      <c r="I22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>23</v>
+      </c>
+      <c r="G23">
+        <v>21</v>
+      </c>
+      <c r="H23">
+        <v>22</v>
+      </c>
+      <c r="I23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="C24">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>31</v>
+      </c>
+      <c r="E24">
+        <v>32</v>
+      </c>
+      <c r="F24">
+        <v>33</v>
+      </c>
+      <c r="G24">
+        <v>31</v>
+      </c>
+      <c r="H24">
+        <v>32</v>
+      </c>
+      <c r="I24">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>13</v>
+      </c>
+      <c r="G25">
+        <v>11</v>
+      </c>
+      <c r="H25">
+        <v>12</v>
+      </c>
+      <c r="I25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <v>22</v>
+      </c>
+      <c r="F26">
+        <v>23</v>
+      </c>
+      <c r="G26">
+        <v>21</v>
+      </c>
+      <c r="H26">
+        <v>22</v>
+      </c>
+      <c r="I26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>32</v>
+      </c>
+      <c r="F27">
+        <v>33</v>
+      </c>
+      <c r="G27">
+        <v>31</v>
+      </c>
+      <c r="H27">
+        <v>32</v>
+      </c>
+      <c r="I27">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>13</v>
+      </c>
+      <c r="D28">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>13</v>
+      </c>
+      <c r="G28">
+        <v>11</v>
+      </c>
+      <c r="H28">
+        <v>12</v>
+      </c>
+      <c r="I28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>23</v>
+      </c>
+      <c r="D29">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <v>22</v>
+      </c>
+      <c r="F29">
+        <v>23</v>
+      </c>
+      <c r="G29">
+        <v>21</v>
+      </c>
+      <c r="H29">
+        <v>22</v>
+      </c>
+      <c r="I29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>33</v>
+      </c>
+      <c r="D30">
+        <v>31</v>
+      </c>
+      <c r="E30">
+        <v>32</v>
+      </c>
+      <c r="F30">
+        <v>33</v>
+      </c>
+      <c r="G30">
+        <v>31</v>
+      </c>
+      <c r="H30">
+        <v>32</v>
+      </c>
+      <c r="I30">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32">
         <v>1</v>
       </c>
-      <c r="B22">
+      <c r="B32">
         <v>2</v>
       </c>
-      <c r="C22">
+      <c r="C32">
         <v>3</v>
       </c>
-      <c r="D22">
+      <c r="D32">
         <v>1</v>
       </c>
-      <c r="E22">
+      <c r="E32">
         <v>2</v>
       </c>
-      <c r="F22">
+      <c r="F32">
         <v>3</v>
       </c>
-      <c r="G22">
+      <c r="G32">
         <v>1</v>
       </c>
-      <c r="H22">
+      <c r="H32">
         <v>2</v>
       </c>
-      <c r="I22">
+      <c r="I32">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="33" spans="1:9">
+      <c r="A33">
         <v>4</v>
       </c>
-      <c r="B23">
+      <c r="B33">
         <v>5</v>
       </c>
-      <c r="C23">
+      <c r="C33">
         <v>6</v>
       </c>
-      <c r="D23">
+      <c r="D33">
         <v>4</v>
       </c>
-      <c r="E23">
+      <c r="E33">
         <v>5</v>
       </c>
-      <c r="F23">
+      <c r="F33">
         <v>6</v>
       </c>
-      <c r="G23">
+      <c r="G33">
         <v>4</v>
       </c>
-      <c r="H23">
+      <c r="H33">
         <v>5</v>
       </c>
-      <c r="I23">
+      <c r="I33">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="34" spans="1:9">
+      <c r="A34">
         <v>7</v>
       </c>
-      <c r="B24">
+      <c r="B34">
         <v>8</v>
       </c>
-      <c r="C24">
+      <c r="C34">
         <v>9</v>
       </c>
-      <c r="D24">
+      <c r="D34">
         <v>7</v>
       </c>
-      <c r="E24">
+      <c r="E34">
         <v>8</v>
       </c>
-      <c r="F24">
+      <c r="F34">
         <v>9</v>
       </c>
-      <c r="G24">
+      <c r="G34">
         <v>7</v>
       </c>
-      <c r="H24">
+      <c r="H34">
         <v>8</v>
       </c>
-      <c r="I24">
+      <c r="I34">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="35" spans="1:9">
+      <c r="A35">
         <v>1</v>
       </c>
-      <c r="B25">
+      <c r="B35">
         <v>2</v>
       </c>
-      <c r="C25">
+      <c r="C35">
         <v>3</v>
       </c>
-      <c r="D25">
+      <c r="D35">
         <v>1</v>
       </c>
-      <c r="E25">
+      <c r="E35">
         <v>2</v>
       </c>
-      <c r="F25">
+      <c r="F35">
         <v>3</v>
       </c>
-      <c r="G25">
+      <c r="G35">
         <v>1</v>
       </c>
-      <c r="H25">
+      <c r="H35">
         <v>2</v>
       </c>
-      <c r="I25">
+      <c r="I35">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="36" spans="1:9">
+      <c r="A36">
         <v>4</v>
       </c>
-      <c r="B26">
+      <c r="B36">
         <v>5</v>
       </c>
-      <c r="C26">
+      <c r="C36">
         <v>6</v>
       </c>
-      <c r="D26">
+      <c r="D36">
         <v>4</v>
       </c>
-      <c r="E26">
+      <c r="E36">
         <v>5</v>
       </c>
-      <c r="F26">
+      <c r="F36">
         <v>6</v>
       </c>
-      <c r="G26">
+      <c r="G36">
         <v>4</v>
       </c>
-      <c r="H26">
+      <c r="H36">
         <v>5</v>
       </c>
-      <c r="I26">
+      <c r="I36">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="37" spans="1:9">
+      <c r="A37">
         <v>7</v>
       </c>
-      <c r="B27">
+      <c r="B37">
         <v>8</v>
       </c>
-      <c r="C27">
+      <c r="C37">
         <v>9</v>
       </c>
-      <c r="D27">
+      <c r="D37">
         <v>7</v>
       </c>
-      <c r="E27">
+      <c r="E37">
         <v>8</v>
       </c>
-      <c r="F27">
+      <c r="F37">
         <v>9</v>
       </c>
-      <c r="G27">
+      <c r="G37">
         <v>7</v>
       </c>
-      <c r="H27">
+      <c r="H37">
         <v>8</v>
       </c>
-      <c r="I27">
+      <c r="I37">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="38" spans="1:9">
+      <c r="A38">
         <v>1</v>
       </c>
-      <c r="B28">
+      <c r="B38">
         <v>2</v>
       </c>
-      <c r="C28">
+      <c r="C38">
         <v>3</v>
       </c>
-      <c r="D28">
+      <c r="D38">
         <v>1</v>
       </c>
-      <c r="E28">
+      <c r="E38">
         <v>2</v>
       </c>
-      <c r="F28">
+      <c r="F38">
         <v>3</v>
       </c>
-      <c r="G28">
+      <c r="G38">
         <v>1</v>
       </c>
-      <c r="H28">
+      <c r="H38">
         <v>2</v>
       </c>
-      <c r="I28">
+      <c r="I38">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="39" spans="1:9">
+      <c r="A39">
         <v>4</v>
       </c>
-      <c r="B29">
+      <c r="B39">
         <v>5</v>
       </c>
-      <c r="C29">
+      <c r="C39">
         <v>6</v>
       </c>
-      <c r="D29">
+      <c r="D39">
         <v>4</v>
       </c>
-      <c r="E29">
+      <c r="E39">
         <v>5</v>
       </c>
-      <c r="F29">
+      <c r="F39">
         <v>6</v>
       </c>
-      <c r="G29">
+      <c r="G39">
         <v>4</v>
       </c>
-      <c r="H29">
+      <c r="H39">
         <v>5</v>
       </c>
-      <c r="I29">
+      <c r="I39">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="40" spans="1:9">
+      <c r="A40">
         <v>7</v>
       </c>
-      <c r="B30">
+      <c r="B40">
         <v>8</v>
       </c>
-      <c r="C30">
+      <c r="C40">
         <v>9</v>
       </c>
-      <c r="D30">
+      <c r="D40">
         <v>7</v>
       </c>
-      <c r="E30">
+      <c r="E40">
         <v>8</v>
       </c>
-      <c r="F30">
+      <c r="F40">
         <v>9</v>
       </c>
-      <c r="G30">
+      <c r="G40">
         <v>7</v>
       </c>
-      <c r="H30">
+      <c r="H40">
         <v>8</v>
       </c>
-      <c r="I30">
+      <c r="I40">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Work on selective highlighting without disrupting scores already calculated
</commit_message>
<xml_diff>
--- a/_DESIGN/Book4b.xlsx
+++ b/_DESIGN/Book4b.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uibc\Desktop\SuperTicTacToe\_DESIGN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uibc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -367,11 +367,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1634,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D81"/>
+      <selection activeCell="F1" sqref="F1:F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1646,7 +1646,7 @@
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1658,12 +1658,20 @@
         <f>A1&amp;" = findViewById(R.id."&amp;A1&amp;");"</f>
         <v>button11 = findViewById(R.id.button11);</v>
       </c>
-      <c r="D1" s="10" t="str">
+      <c r="D1" s="9" t="str">
         <f>A1&amp;".getBackground().setColorFilter(null);"</f>
         <v>button11.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="str">
+        <f>A1&amp;".setEnabled(true);"</f>
+        <v>button11.setEnabled(true);</v>
+      </c>
+      <c r="F1" t="str">
+        <f>A1&amp;".setEnabled(false);"</f>
+        <v>button11.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1675,12 +1683,20 @@
         <f t="shared" ref="C2:C65" si="1">A2&amp;" = findViewById(R.id."&amp;A2&amp;");"</f>
         <v>button12 = findViewById(R.id.button12);</v>
       </c>
-      <c r="D2" s="10" t="str">
+      <c r="D2" s="9" t="str">
         <f t="shared" ref="D2:D65" si="2">A2&amp;".getBackground().setColorFilter(null);"</f>
         <v>button12.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E65" si="3">A2&amp;".setEnabled(true);"</f>
+        <v>button12.setEnabled(true);</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F65" si="4">A2&amp;".setEnabled(false);"</f>
+        <v>button12.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1692,12 +1708,20 @@
         <f t="shared" si="1"/>
         <v>button13 = findViewById(R.id.button13);</v>
       </c>
-      <c r="D3" s="10" t="str">
+      <c r="D3" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button13.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="str">
+        <f t="shared" si="3"/>
+        <v>button13.setEnabled(true);</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="4"/>
+        <v>button13.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1709,12 +1733,20 @@
         <f t="shared" si="1"/>
         <v>button14 = findViewById(R.id.button14);</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="D4" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button14.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="str">
+        <f t="shared" si="3"/>
+        <v>button14.setEnabled(true);</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="4"/>
+        <v>button14.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1726,12 +1758,20 @@
         <f t="shared" si="1"/>
         <v>button15 = findViewById(R.id.button15);</v>
       </c>
-      <c r="D5" s="10" t="str">
+      <c r="D5" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button15.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="str">
+        <f t="shared" si="3"/>
+        <v>button15.setEnabled(true);</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="4"/>
+        <v>button15.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1743,12 +1783,20 @@
         <f t="shared" si="1"/>
         <v>button16 = findViewById(R.id.button16);</v>
       </c>
-      <c r="D6" s="10" t="str">
+      <c r="D6" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button16.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="str">
+        <f t="shared" si="3"/>
+        <v>button16.setEnabled(true);</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="4"/>
+        <v>button16.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1760,12 +1808,20 @@
         <f t="shared" si="1"/>
         <v>button17 = findViewById(R.id.button17);</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D7" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button17.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="str">
+        <f t="shared" si="3"/>
+        <v>button17.setEnabled(true);</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="4"/>
+        <v>button17.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1777,12 +1833,20 @@
         <f t="shared" si="1"/>
         <v>button18 = findViewById(R.id.button18);</v>
       </c>
-      <c r="D8" s="10" t="str">
+      <c r="D8" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button18.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="str">
+        <f t="shared" si="3"/>
+        <v>button18.setEnabled(true);</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="4"/>
+        <v>button18.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1794,12 +1858,20 @@
         <f t="shared" si="1"/>
         <v>button19 = findViewById(R.id.button19);</v>
       </c>
-      <c r="D9" s="10" t="str">
+      <c r="D9" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button19.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="str">
+        <f t="shared" si="3"/>
+        <v>button19.setEnabled(true);</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="4"/>
+        <v>button19.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1811,12 +1883,20 @@
         <f t="shared" si="1"/>
         <v>button21 = findViewById(R.id.button21);</v>
       </c>
-      <c r="D10" s="10" t="str">
+      <c r="D10" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button21.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v>button21.setEnabled(true);</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="4"/>
+        <v>button21.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1828,12 +1908,20 @@
         <f t="shared" si="1"/>
         <v>button22 = findViewById(R.id.button22);</v>
       </c>
-      <c r="D11" s="10" t="str">
+      <c r="D11" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button22.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v>button22.setEnabled(true);</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="4"/>
+        <v>button22.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1845,12 +1933,20 @@
         <f t="shared" si="1"/>
         <v>button23 = findViewById(R.id.button23);</v>
       </c>
-      <c r="D12" s="10" t="str">
+      <c r="D12" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button23.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="str">
+        <f t="shared" si="3"/>
+        <v>button23.setEnabled(true);</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="4"/>
+        <v>button23.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1862,12 +1958,20 @@
         <f t="shared" si="1"/>
         <v>button24 = findViewById(R.id.button24);</v>
       </c>
-      <c r="D13" s="10" t="str">
+      <c r="D13" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button24.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v>button24.setEnabled(true);</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="4"/>
+        <v>button24.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1879,12 +1983,20 @@
         <f t="shared" si="1"/>
         <v>button25 = findViewById(R.id.button25);</v>
       </c>
-      <c r="D14" s="10" t="str">
+      <c r="D14" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button25.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v>button25.setEnabled(true);</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="4"/>
+        <v>button25.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1896,12 +2008,20 @@
         <f t="shared" si="1"/>
         <v>button26 = findViewById(R.id.button26);</v>
       </c>
-      <c r="D15" s="10" t="str">
+      <c r="D15" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button26.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>button26.setEnabled(true);</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="4"/>
+        <v>button26.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1913,12 +2033,20 @@
         <f t="shared" si="1"/>
         <v>button27 = findViewById(R.id.button27);</v>
       </c>
-      <c r="D16" s="10" t="str">
+      <c r="D16" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button27.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v>button27.setEnabled(true);</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="4"/>
+        <v>button27.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1930,12 +2058,20 @@
         <f t="shared" si="1"/>
         <v>button28 = findViewById(R.id.button28);</v>
       </c>
-      <c r="D17" s="10" t="str">
+      <c r="D17" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button28.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v>button28.setEnabled(true);</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="4"/>
+        <v>button28.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1947,12 +2083,20 @@
         <f t="shared" si="1"/>
         <v>button29 = findViewById(R.id.button29);</v>
       </c>
-      <c r="D18" s="10" t="str">
+      <c r="D18" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button29.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v>button29.setEnabled(true);</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="4"/>
+        <v>button29.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1964,12 +2108,20 @@
         <f t="shared" si="1"/>
         <v>button31 = findViewById(R.id.button31);</v>
       </c>
-      <c r="D19" s="10" t="str">
+      <c r="D19" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button31.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v>button31.setEnabled(true);</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="4"/>
+        <v>button31.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1981,12 +2133,20 @@
         <f t="shared" si="1"/>
         <v>button32 = findViewById(R.id.button32);</v>
       </c>
-      <c r="D20" s="10" t="str">
+      <c r="D20" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button32.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v>button32.setEnabled(true);</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="4"/>
+        <v>button32.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1998,12 +2158,20 @@
         <f t="shared" si="1"/>
         <v>button33 = findViewById(R.id.button33);</v>
       </c>
-      <c r="D21" s="10" t="str">
+      <c r="D21" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button33.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="str">
+        <f t="shared" si="3"/>
+        <v>button33.setEnabled(true);</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="4"/>
+        <v>button33.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2015,12 +2183,20 @@
         <f t="shared" si="1"/>
         <v>button34 = findViewById(R.id.button34);</v>
       </c>
-      <c r="D22" s="10" t="str">
+      <c r="D22" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button34.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="str">
+        <f t="shared" si="3"/>
+        <v>button34.setEnabled(true);</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="4"/>
+        <v>button34.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2032,12 +2208,20 @@
         <f t="shared" si="1"/>
         <v>button35 = findViewById(R.id.button35);</v>
       </c>
-      <c r="D23" s="10" t="str">
+      <c r="D23" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button35.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="str">
+        <f t="shared" si="3"/>
+        <v>button35.setEnabled(true);</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="4"/>
+        <v>button35.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2049,12 +2233,20 @@
         <f t="shared" si="1"/>
         <v>button36 = findViewById(R.id.button36);</v>
       </c>
-      <c r="D24" s="10" t="str">
+      <c r="D24" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button36.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="str">
+        <f t="shared" si="3"/>
+        <v>button36.setEnabled(true);</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="4"/>
+        <v>button36.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2066,12 +2258,20 @@
         <f t="shared" si="1"/>
         <v>button37 = findViewById(R.id.button37);</v>
       </c>
-      <c r="D25" s="10" t="str">
+      <c r="D25" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button37.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="str">
+        <f t="shared" si="3"/>
+        <v>button37.setEnabled(true);</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="4"/>
+        <v>button37.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2083,12 +2283,20 @@
         <f t="shared" si="1"/>
         <v>button38 = findViewById(R.id.button38);</v>
       </c>
-      <c r="D26" s="10" t="str">
+      <c r="D26" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button38.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" t="str">
+        <f t="shared" si="3"/>
+        <v>button38.setEnabled(true);</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="4"/>
+        <v>button38.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2100,12 +2308,20 @@
         <f t="shared" si="1"/>
         <v>button39 = findViewById(R.id.button39);</v>
       </c>
-      <c r="D27" s="10" t="str">
+      <c r="D27" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button39.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="str">
+        <f t="shared" si="3"/>
+        <v>button39.setEnabled(true);</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="4"/>
+        <v>button39.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2117,12 +2333,20 @@
         <f t="shared" si="1"/>
         <v>button41 = findViewById(R.id.button41);</v>
       </c>
-      <c r="D28" s="10" t="str">
+      <c r="D28" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button41.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="str">
+        <f t="shared" si="3"/>
+        <v>button41.setEnabled(true);</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="4"/>
+        <v>button41.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2134,12 +2358,20 @@
         <f t="shared" si="1"/>
         <v>button42 = findViewById(R.id.button42);</v>
       </c>
-      <c r="D29" s="10" t="str">
+      <c r="D29" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button42.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="str">
+        <f t="shared" si="3"/>
+        <v>button42.setEnabled(true);</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="4"/>
+        <v>button42.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2151,12 +2383,20 @@
         <f t="shared" si="1"/>
         <v>button43 = findViewById(R.id.button43);</v>
       </c>
-      <c r="D30" s="10" t="str">
+      <c r="D30" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button43.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="str">
+        <f t="shared" si="3"/>
+        <v>button43.setEnabled(true);</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="4"/>
+        <v>button43.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2168,12 +2408,20 @@
         <f t="shared" si="1"/>
         <v>button44 = findViewById(R.id.button44);</v>
       </c>
-      <c r="D31" s="10" t="str">
+      <c r="D31" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button44.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="str">
+        <f t="shared" si="3"/>
+        <v>button44.setEnabled(true);</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="4"/>
+        <v>button44.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2185,12 +2433,20 @@
         <f t="shared" si="1"/>
         <v>button45 = findViewById(R.id.button45);</v>
       </c>
-      <c r="D32" s="10" t="str">
+      <c r="D32" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button45.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="str">
+        <f t="shared" si="3"/>
+        <v>button45.setEnabled(true);</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="4"/>
+        <v>button45.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2202,12 +2458,20 @@
         <f t="shared" si="1"/>
         <v>button46 = findViewById(R.id.button46);</v>
       </c>
-      <c r="D33" s="10" t="str">
+      <c r="D33" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button46.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="str">
+        <f t="shared" si="3"/>
+        <v>button46.setEnabled(true);</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="4"/>
+        <v>button46.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2219,12 +2483,20 @@
         <f t="shared" si="1"/>
         <v>button47 = findViewById(R.id.button47);</v>
       </c>
-      <c r="D34" s="10" t="str">
+      <c r="D34" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button47.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="str">
+        <f t="shared" si="3"/>
+        <v>button47.setEnabled(true);</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="4"/>
+        <v>button47.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2236,12 +2508,20 @@
         <f t="shared" si="1"/>
         <v>button48 = findViewById(R.id.button48);</v>
       </c>
-      <c r="D35" s="10" t="str">
+      <c r="D35" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button48.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="str">
+        <f t="shared" si="3"/>
+        <v>button48.setEnabled(true);</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="4"/>
+        <v>button48.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2253,12 +2533,20 @@
         <f t="shared" si="1"/>
         <v>button49 = findViewById(R.id.button49);</v>
       </c>
-      <c r="D36" s="10" t="str">
+      <c r="D36" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button49.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="str">
+        <f t="shared" si="3"/>
+        <v>button49.setEnabled(true);</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="4"/>
+        <v>button49.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2270,12 +2558,20 @@
         <f t="shared" si="1"/>
         <v>button51 = findViewById(R.id.button51);</v>
       </c>
-      <c r="D37" s="10" t="str">
+      <c r="D37" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button51.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" t="str">
+        <f t="shared" si="3"/>
+        <v>button51.setEnabled(true);</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="4"/>
+        <v>button51.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2287,12 +2583,20 @@
         <f t="shared" si="1"/>
         <v>button52 = findViewById(R.id.button52);</v>
       </c>
-      <c r="D38" s="10" t="str">
+      <c r="D38" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button52.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" t="str">
+        <f t="shared" si="3"/>
+        <v>button52.setEnabled(true);</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="4"/>
+        <v>button52.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2304,12 +2608,20 @@
         <f t="shared" si="1"/>
         <v>button53 = findViewById(R.id.button53);</v>
       </c>
-      <c r="D39" s="10" t="str">
+      <c r="D39" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button53.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" t="str">
+        <f t="shared" si="3"/>
+        <v>button53.setEnabled(true);</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="4"/>
+        <v>button53.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2321,12 +2633,20 @@
         <f t="shared" si="1"/>
         <v>button54 = findViewById(R.id.button54);</v>
       </c>
-      <c r="D40" s="10" t="str">
+      <c r="D40" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button54.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" t="str">
+        <f t="shared" si="3"/>
+        <v>button54.setEnabled(true);</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="4"/>
+        <v>button54.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2338,12 +2658,20 @@
         <f t="shared" si="1"/>
         <v>button55 = findViewById(R.id.button55);</v>
       </c>
-      <c r="D41" s="10" t="str">
+      <c r="D41" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button55.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" t="str">
+        <f t="shared" si="3"/>
+        <v>button55.setEnabled(true);</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="4"/>
+        <v>button55.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2355,12 +2683,20 @@
         <f t="shared" si="1"/>
         <v>button56 = findViewById(R.id.button56);</v>
       </c>
-      <c r="D42" s="10" t="str">
+      <c r="D42" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button56.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" t="str">
+        <f t="shared" si="3"/>
+        <v>button56.setEnabled(true);</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="4"/>
+        <v>button56.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2372,12 +2708,20 @@
         <f t="shared" si="1"/>
         <v>button57 = findViewById(R.id.button57);</v>
       </c>
-      <c r="D43" s="10" t="str">
+      <c r="D43" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button57.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" t="str">
+        <f t="shared" si="3"/>
+        <v>button57.setEnabled(true);</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="4"/>
+        <v>button57.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2389,12 +2733,20 @@
         <f t="shared" si="1"/>
         <v>button58 = findViewById(R.id.button58);</v>
       </c>
-      <c r="D44" s="10" t="str">
+      <c r="D44" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button58.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" t="str">
+        <f t="shared" si="3"/>
+        <v>button58.setEnabled(true);</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="4"/>
+        <v>button58.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2406,12 +2758,20 @@
         <f t="shared" si="1"/>
         <v>button59 = findViewById(R.id.button59);</v>
       </c>
-      <c r="D45" s="10" t="str">
+      <c r="D45" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button59.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" t="str">
+        <f t="shared" si="3"/>
+        <v>button59.setEnabled(true);</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="4"/>
+        <v>button59.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2423,12 +2783,20 @@
         <f t="shared" si="1"/>
         <v>button61 = findViewById(R.id.button61);</v>
       </c>
-      <c r="D46" s="10" t="str">
+      <c r="D46" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button61.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" t="str">
+        <f t="shared" si="3"/>
+        <v>button61.setEnabled(true);</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="4"/>
+        <v>button61.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2440,12 +2808,20 @@
         <f t="shared" si="1"/>
         <v>button62 = findViewById(R.id.button62);</v>
       </c>
-      <c r="D47" s="10" t="str">
+      <c r="D47" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button62.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" t="str">
+        <f t="shared" si="3"/>
+        <v>button62.setEnabled(true);</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="4"/>
+        <v>button62.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2457,12 +2833,20 @@
         <f t="shared" si="1"/>
         <v>button63 = findViewById(R.id.button63);</v>
       </c>
-      <c r="D48" s="10" t="str">
+      <c r="D48" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button63.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" t="str">
+        <f t="shared" si="3"/>
+        <v>button63.setEnabled(true);</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="4"/>
+        <v>button63.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2474,12 +2858,20 @@
         <f t="shared" si="1"/>
         <v>button64 = findViewById(R.id.button64);</v>
       </c>
-      <c r="D49" s="10" t="str">
+      <c r="D49" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button64.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" t="str">
+        <f t="shared" si="3"/>
+        <v>button64.setEnabled(true);</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="4"/>
+        <v>button64.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2491,12 +2883,20 @@
         <f t="shared" si="1"/>
         <v>button65 = findViewById(R.id.button65);</v>
       </c>
-      <c r="D50" s="10" t="str">
+      <c r="D50" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button65.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" t="str">
+        <f t="shared" si="3"/>
+        <v>button65.setEnabled(true);</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="4"/>
+        <v>button65.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2508,12 +2908,20 @@
         <f t="shared" si="1"/>
         <v>button66 = findViewById(R.id.button66);</v>
       </c>
-      <c r="D51" s="10" t="str">
+      <c r="D51" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button66.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" t="str">
+        <f t="shared" si="3"/>
+        <v>button66.setEnabled(true);</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="4"/>
+        <v>button66.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2525,12 +2933,20 @@
         <f t="shared" si="1"/>
         <v>button67 = findViewById(R.id.button67);</v>
       </c>
-      <c r="D52" s="10" t="str">
+      <c r="D52" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button67.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" t="str">
+        <f t="shared" si="3"/>
+        <v>button67.setEnabled(true);</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="4"/>
+        <v>button67.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2542,12 +2958,20 @@
         <f t="shared" si="1"/>
         <v>button68 = findViewById(R.id.button68);</v>
       </c>
-      <c r="D53" s="10" t="str">
+      <c r="D53" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button68.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" t="str">
+        <f t="shared" si="3"/>
+        <v>button68.setEnabled(true);</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="4"/>
+        <v>button68.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2559,12 +2983,20 @@
         <f t="shared" si="1"/>
         <v>button69 = findViewById(R.id.button69);</v>
       </c>
-      <c r="D54" s="10" t="str">
+      <c r="D54" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button69.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" t="str">
+        <f t="shared" si="3"/>
+        <v>button69.setEnabled(true);</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="4"/>
+        <v>button69.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2576,12 +3008,20 @@
         <f t="shared" si="1"/>
         <v>button71 = findViewById(R.id.button71);</v>
       </c>
-      <c r="D55" s="10" t="str">
+      <c r="D55" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button71.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" t="str">
+        <f t="shared" si="3"/>
+        <v>button71.setEnabled(true);</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="4"/>
+        <v>button71.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2593,12 +3033,20 @@
         <f t="shared" si="1"/>
         <v>button72 = findViewById(R.id.button72);</v>
       </c>
-      <c r="D56" s="10" t="str">
+      <c r="D56" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button72.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" t="str">
+        <f t="shared" si="3"/>
+        <v>button72.setEnabled(true);</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="4"/>
+        <v>button72.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2610,12 +3058,20 @@
         <f t="shared" si="1"/>
         <v>button73 = findViewById(R.id.button73);</v>
       </c>
-      <c r="D57" s="10" t="str">
+      <c r="D57" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button73.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" t="str">
+        <f t="shared" si="3"/>
+        <v>button73.setEnabled(true);</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="4"/>
+        <v>button73.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2627,12 +3083,20 @@
         <f t="shared" si="1"/>
         <v>button74 = findViewById(R.id.button74);</v>
       </c>
-      <c r="D58" s="10" t="str">
+      <c r="D58" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button74.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" t="str">
+        <f t="shared" si="3"/>
+        <v>button74.setEnabled(true);</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="4"/>
+        <v>button74.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2644,12 +3108,20 @@
         <f t="shared" si="1"/>
         <v>button75 = findViewById(R.id.button75);</v>
       </c>
-      <c r="D59" s="10" t="str">
+      <c r="D59" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button75.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" t="str">
+        <f t="shared" si="3"/>
+        <v>button75.setEnabled(true);</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="4"/>
+        <v>button75.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2661,12 +3133,20 @@
         <f t="shared" si="1"/>
         <v>button76 = findViewById(R.id.button76);</v>
       </c>
-      <c r="D60" s="10" t="str">
+      <c r="D60" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button76.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" t="str">
+        <f t="shared" si="3"/>
+        <v>button76.setEnabled(true);</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="4"/>
+        <v>button76.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2678,12 +3158,20 @@
         <f t="shared" si="1"/>
         <v>button77 = findViewById(R.id.button77);</v>
       </c>
-      <c r="D61" s="10" t="str">
+      <c r="D61" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button77.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61" t="str">
+        <f t="shared" si="3"/>
+        <v>button77.setEnabled(true);</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="4"/>
+        <v>button77.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2695,12 +3183,20 @@
         <f t="shared" si="1"/>
         <v>button78 = findViewById(R.id.button78);</v>
       </c>
-      <c r="D62" s="10" t="str">
+      <c r="D62" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button78.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62" t="str">
+        <f t="shared" si="3"/>
+        <v>button78.setEnabled(true);</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="4"/>
+        <v>button78.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2712,12 +3208,20 @@
         <f t="shared" si="1"/>
         <v>button79 = findViewById(R.id.button79);</v>
       </c>
-      <c r="D63" s="10" t="str">
+      <c r="D63" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button79.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63" t="str">
+        <f t="shared" si="3"/>
+        <v>button79.setEnabled(true);</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="4"/>
+        <v>button79.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2729,12 +3233,20 @@
         <f t="shared" si="1"/>
         <v>button81 = findViewById(R.id.button81);</v>
       </c>
-      <c r="D64" s="10" t="str">
+      <c r="D64" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button81.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" t="str">
+        <f t="shared" si="3"/>
+        <v>button81.setEnabled(true);</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="4"/>
+        <v>button81.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2746,281 +3258,417 @@
         <f t="shared" si="1"/>
         <v>button82 = findViewById(R.id.button82);</v>
       </c>
-      <c r="D65" s="10" t="str">
+      <c r="D65" s="9" t="str">
         <f t="shared" si="2"/>
         <v>button82.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" t="str">
+        <f t="shared" si="3"/>
+        <v>button82.setEnabled(true);</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="4"/>
+        <v>button82.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B81" si="3">"Button "&amp;A66&amp;";"</f>
+        <f t="shared" ref="B66:B81" si="5">"Button "&amp;A66&amp;";"</f>
         <v>Button button83;</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C81" si="4">A66&amp;" = findViewById(R.id."&amp;A66&amp;");"</f>
+        <f t="shared" ref="C66:C81" si="6">A66&amp;" = findViewById(R.id."&amp;A66&amp;");"</f>
         <v>button83 = findViewById(R.id.button83);</v>
       </c>
-      <c r="D66" s="10" t="str">
-        <f t="shared" ref="D66:D81" si="5">A66&amp;".getBackground().setColorFilter(null);"</f>
+      <c r="D66" s="9" t="str">
+        <f t="shared" ref="D66:D81" si="7">A66&amp;".getBackground().setColorFilter(null);"</f>
         <v>button83.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" t="str">
+        <f t="shared" ref="E66:E81" si="8">A66&amp;".setEnabled(true);"</f>
+        <v>button83.setEnabled(true);</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" ref="F66:F81" si="9">A66&amp;".setEnabled(false);"</f>
+        <v>button83.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>66</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button84;</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button84 = findViewById(R.id.button84);</v>
       </c>
-      <c r="D67" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D67" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button84.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" t="str">
+        <f t="shared" si="8"/>
+        <v>button84.setEnabled(true);</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="9"/>
+        <v>button84.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>67</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button85;</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button85 = findViewById(R.id.button85);</v>
       </c>
-      <c r="D68" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D68" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button85.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68" t="str">
+        <f t="shared" si="8"/>
+        <v>button85.setEnabled(true);</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="9"/>
+        <v>button85.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button86;</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button86 = findViewById(R.id.button86);</v>
       </c>
-      <c r="D69" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D69" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button86.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69" t="str">
+        <f t="shared" si="8"/>
+        <v>button86.setEnabled(true);</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="9"/>
+        <v>button86.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>69</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button87;</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button87 = findViewById(R.id.button87);</v>
       </c>
-      <c r="D70" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D70" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button87.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70" t="str">
+        <f t="shared" si="8"/>
+        <v>button87.setEnabled(true);</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="9"/>
+        <v>button87.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>70</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button88;</v>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button88 = findViewById(R.id.button88);</v>
       </c>
-      <c r="D71" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D71" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button88.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71" t="str">
+        <f t="shared" si="8"/>
+        <v>button88.setEnabled(true);</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="9"/>
+        <v>button88.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>71</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button89;</v>
       </c>
       <c r="C72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button89 = findViewById(R.id.button89);</v>
       </c>
-      <c r="D72" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D72" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button89.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72" t="str">
+        <f t="shared" si="8"/>
+        <v>button89.setEnabled(true);</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="9"/>
+        <v>button89.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>72</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button91;</v>
       </c>
       <c r="C73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button91 = findViewById(R.id.button91);</v>
       </c>
-      <c r="D73" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D73" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button91.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73" t="str">
+        <f t="shared" si="8"/>
+        <v>button91.setEnabled(true);</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="9"/>
+        <v>button91.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>73</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button92;</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button92 = findViewById(R.id.button92);</v>
       </c>
-      <c r="D74" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D74" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button92.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74" t="str">
+        <f t="shared" si="8"/>
+        <v>button92.setEnabled(true);</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="9"/>
+        <v>button92.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>74</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button93;</v>
       </c>
       <c r="C75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button93 = findViewById(R.id.button93);</v>
       </c>
-      <c r="D75" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D75" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button93.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75" t="str">
+        <f t="shared" si="8"/>
+        <v>button93.setEnabled(true);</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="9"/>
+        <v>button93.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>75</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button94;</v>
       </c>
       <c r="C76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button94 = findViewById(R.id.button94);</v>
       </c>
-      <c r="D76" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D76" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button94.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76" t="str">
+        <f t="shared" si="8"/>
+        <v>button94.setEnabled(true);</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="9"/>
+        <v>button94.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>76</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button95;</v>
       </c>
       <c r="C77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button95 = findViewById(R.id.button95);</v>
       </c>
-      <c r="D77" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D77" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button95.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77" t="str">
+        <f t="shared" si="8"/>
+        <v>button95.setEnabled(true);</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="9"/>
+        <v>button95.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>77</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button96;</v>
       </c>
       <c r="C78" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button96 = findViewById(R.id.button96);</v>
       </c>
-      <c r="D78" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D78" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button96.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78" t="str">
+        <f t="shared" si="8"/>
+        <v>button96.setEnabled(true);</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="9"/>
+        <v>button96.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>78</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button97;</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button97 = findViewById(R.id.button97);</v>
       </c>
-      <c r="D79" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D79" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button97.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79" t="str">
+        <f t="shared" si="8"/>
+        <v>button97.setEnabled(true);</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="9"/>
+        <v>button97.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>79</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button98;</v>
       </c>
       <c r="C80" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button98 = findViewById(R.id.button98);</v>
       </c>
-      <c r="D80" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D80" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button98.getBackground().setColorFilter(null);</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80" t="str">
+        <f t="shared" si="8"/>
+        <v>button98.setEnabled(true);</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="9"/>
+        <v>button98.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>80</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button button99;</v>
       </c>
       <c r="C81" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>button99 = findViewById(R.id.button99);</v>
       </c>
-      <c r="D81" s="10" t="str">
-        <f t="shared" si="5"/>
+      <c r="D81" s="9" t="str">
+        <f t="shared" si="7"/>
         <v>button99.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="8"/>
+        <v>button99.setEnabled(true);</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="9"/>
+        <v>button99.setEnabled(false);</v>
       </c>
     </row>
   </sheetData>
@@ -3031,10 +3679,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:S10"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42:S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3043,17 +3691,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2">
@@ -3084,40 +3732,40 @@
         <v>3</v>
       </c>
       <c r="K2" t="str">
-        <f>"public void button"&amp;A12&amp;" (View view){ game"&amp;A2&amp;"["&amp;LEFT(A22,1)&amp;"]["&amp;RIGHT(A22,1)&amp;"]=currentPlayer; button"&amp;A12&amp;".setEnabled(false); activeGame"&amp;A32&amp;"();}"</f>
-        <v>public void button11 (View view){ game1[1][1]=currentPlayer; button11.setEnabled(false); activeGame1();}</v>
+        <f>"public void button"&amp;A12&amp;" (View view){ game"&amp;A2&amp;"["&amp;LEFT(A22,1)&amp;"]["&amp;RIGHT(A22,1)&amp;"]=currentPlayer; button"&amp;A12&amp;".setEnabled(false); activeGame"&amp;A32&amp;"(); if (currentPlayer == 1) { button"&amp;A12&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); currentPlayer = 2; } else { button"&amp;A12&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); currentPlayer = 1; }}"</f>
+        <v>public void button11 (View view){ game1[1][1]=currentPlayer; button11.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button11.setText("X"); currentPlayer = 2; } else { button11.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:S10" si="0">"public void button"&amp;B12&amp;" (View view){ game"&amp;B2&amp;"["&amp;LEFT(B22,1)&amp;"]["&amp;RIGHT(B22,1)&amp;"]=currentPlayer; button"&amp;B12&amp;".setEnabled(false); activeGame"&amp;B32&amp;"();}"</f>
-        <v>public void button12 (View view){ game1[1][2]=currentPlayer; button12.setEnabled(false); activeGame2();}</v>
+        <f t="shared" ref="L2:S10" si="0">"public void button"&amp;B12&amp;" (View view){ game"&amp;B2&amp;"["&amp;LEFT(B22,1)&amp;"]["&amp;RIGHT(B22,1)&amp;"]=currentPlayer; button"&amp;B12&amp;".setEnabled(false); activeGame"&amp;B32&amp;"(); if (currentPlayer == 1) { button"&amp;B12&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); currentPlayer = 2; } else { button"&amp;B12&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); currentPlayer = 1; }}"</f>
+        <v>public void button12 (View view){ game1[1][2]=currentPlayer; button12.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button12.setText("X"); currentPlayer = 2; } else { button12.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button13 (View view){ game1[1][3]=currentPlayer; button13.setEnabled(false); activeGame3();}</v>
+        <v>public void button13 (View view){ game1[1][3]=currentPlayer; button13.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button13.setText("X"); currentPlayer = 2; } else { button13.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button14 (View view){ game2[1][1]=currentPlayer; button14.setEnabled(false); activeGame1();}</v>
+        <v>public void button14 (View view){ game2[1][1]=currentPlayer; button14.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button14.setText("X"); currentPlayer = 2; } else { button14.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button15 (View view){ game2[1][2]=currentPlayer; button15.setEnabled(false); activeGame2();}</v>
+        <v>public void button15 (View view){ game2[1][2]=currentPlayer; button15.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button15.setText("X"); currentPlayer = 2; } else { button15.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button16 (View view){ game2[1][3]=currentPlayer; button16.setEnabled(false); activeGame3();}</v>
+        <v>public void button16 (View view){ game2[1][3]=currentPlayer; button16.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button16.setText("X"); currentPlayer = 2; } else { button16.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button17 (View view){ game3[1][1]=currentPlayer; button17.setEnabled(false); activeGame1();}</v>
+        <v>public void button17 (View view){ game3[1][1]=currentPlayer; button17.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button17.setText("X"); currentPlayer = 2; } else { button17.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button18 (View view){ game3[1][2]=currentPlayer; button18.setEnabled(false); activeGame2();}</v>
+        <v>public void button18 (View view){ game3[1][2]=currentPlayer; button18.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button18.setText("X"); currentPlayer = 2; } else { button18.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S2" t="str">
         <f t="shared" si="0"/>
-        <v>public void button19 (View view){ game3[1][3]=currentPlayer; button19.setEnabled(false); activeGame3();}</v>
+        <v>public void button19 (View view){ game3[1][3]=currentPlayer; button19.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button19.setText("X"); currentPlayer = 2; } else { button19.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3149,40 +3797,40 @@
         <v>3</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K10" si="1">"public void button"&amp;A13&amp;" (View view){ game"&amp;A3&amp;"["&amp;LEFT(A23,1)&amp;"]["&amp;RIGHT(A23,1)&amp;"]=currentPlayer; button"&amp;A13&amp;".setEnabled(false); activeGame"&amp;A33&amp;"();}"</f>
-        <v>public void button21 (View view){ game1[2][1]=currentPlayer; button21.setEnabled(false); activeGame4();}</v>
+        <f t="shared" ref="K3:K10" si="1">"public void button"&amp;A13&amp;" (View view){ game"&amp;A3&amp;"["&amp;LEFT(A23,1)&amp;"]["&amp;RIGHT(A23,1)&amp;"]=currentPlayer; button"&amp;A13&amp;".setEnabled(false); activeGame"&amp;A33&amp;"(); if (currentPlayer == 1) { button"&amp;A13&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); currentPlayer = 2; } else { button"&amp;A13&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); currentPlayer = 1; }}"</f>
+        <v>public void button21 (View view){ game1[2][1]=currentPlayer; button21.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button21.setText("X"); currentPlayer = 2; } else { button21.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button22 (View view){ game1[2][2]=currentPlayer; button22.setEnabled(false); activeGame5();}</v>
+        <v>public void button22 (View view){ game1[2][2]=currentPlayer; button22.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button22.setText("X"); currentPlayer = 2; } else { button22.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button23 (View view){ game1[2][3]=currentPlayer; button23.setEnabled(false); activeGame6();}</v>
+        <v>public void button23 (View view){ game1[2][3]=currentPlayer; button23.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button23.setText("X"); currentPlayer = 2; } else { button23.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button24 (View view){ game2[2][1]=currentPlayer; button24.setEnabled(false); activeGame4();}</v>
+        <v>public void button24 (View view){ game2[2][1]=currentPlayer; button24.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button24.setText("X"); currentPlayer = 2; } else { button24.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button25 (View view){ game2[2][2]=currentPlayer; button25.setEnabled(false); activeGame5();}</v>
+        <v>public void button25 (View view){ game2[2][2]=currentPlayer; button25.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button25.setText("X"); currentPlayer = 2; } else { button25.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button26 (View view){ game2[2][3]=currentPlayer; button26.setEnabled(false); activeGame6();}</v>
+        <v>public void button26 (View view){ game2[2][3]=currentPlayer; button26.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button26.setText("X"); currentPlayer = 2; } else { button26.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button27 (View view){ game3[2][1]=currentPlayer; button27.setEnabled(false); activeGame4();}</v>
+        <v>public void button27 (View view){ game3[2][1]=currentPlayer; button27.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button27.setText("X"); currentPlayer = 2; } else { button27.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button28 (View view){ game3[2][2]=currentPlayer; button28.setEnabled(false); activeGame5();}</v>
+        <v>public void button28 (View view){ game3[2][2]=currentPlayer; button28.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button28.setText("X"); currentPlayer = 2; } else { button28.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S3" t="str">
         <f t="shared" si="0"/>
-        <v>public void button29 (View view){ game3[2][3]=currentPlayer; button29.setEnabled(false); activeGame6();}</v>
+        <v>public void button29 (View view){ game3[2][3]=currentPlayer; button29.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button29.setText("X"); currentPlayer = 2; } else { button29.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3215,39 +3863,39 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>public void button31 (View view){ game1[3][1]=currentPlayer; button31.setEnabled(false); activeGame7();}</v>
+        <v>public void button31 (View view){ game1[3][1]=currentPlayer; button31.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button31.setText("X"); currentPlayer = 2; } else { button31.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button32 (View view){ game1[3][2]=currentPlayer; button32.setEnabled(false); activeGame8();}</v>
+        <v>public void button32 (View view){ game1[3][2]=currentPlayer; button32.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button32.setText("X"); currentPlayer = 2; } else { button32.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button33 (View view){ game1[3][3]=currentPlayer; button33.setEnabled(false); activeGame9();}</v>
+        <v>public void button33 (View view){ game1[3][3]=currentPlayer; button33.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button33.setText("X"); currentPlayer = 2; } else { button33.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button34 (View view){ game2[3][1]=currentPlayer; button34.setEnabled(false); activeGame7();}</v>
+        <v>public void button34 (View view){ game2[3][1]=currentPlayer; button34.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button34.setText("X"); currentPlayer = 2; } else { button34.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button35 (View view){ game2[3][2]=currentPlayer; button35.setEnabled(false); activeGame8();}</v>
+        <v>public void button35 (View view){ game2[3][2]=currentPlayer; button35.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button35.setText("X"); currentPlayer = 2; } else { button35.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button36 (View view){ game2[3][3]=currentPlayer; button36.setEnabled(false); activeGame9();}</v>
+        <v>public void button36 (View view){ game2[3][3]=currentPlayer; button36.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button36.setText("X"); currentPlayer = 2; } else { button36.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button37 (View view){ game3[3][1]=currentPlayer; button37.setEnabled(false); activeGame7();}</v>
+        <v>public void button37 (View view){ game3[3][1]=currentPlayer; button37.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button37.setText("X"); currentPlayer = 2; } else { button37.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button38 (View view){ game3[3][2]=currentPlayer; button38.setEnabled(false); activeGame8();}</v>
+        <v>public void button38 (View view){ game3[3][2]=currentPlayer; button38.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button38.setText("X"); currentPlayer = 2; } else { button38.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S4" t="str">
         <f t="shared" si="0"/>
-        <v>public void button39 (View view){ game3[3][3]=currentPlayer; button39.setEnabled(false); activeGame9();}</v>
+        <v>public void button39 (View view){ game3[3][3]=currentPlayer; button39.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button39.setText("X"); currentPlayer = 2; } else { button39.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3280,39 +3928,39 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>public void button41 (View view){ game4[1][1]=currentPlayer; button41.setEnabled(false); activeGame1();}</v>
+        <v>public void button41 (View view){ game4[1][1]=currentPlayer; button41.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button41.setText("X"); currentPlayer = 2; } else { button41.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button42 (View view){ game4[1][2]=currentPlayer; button42.setEnabled(false); activeGame2();}</v>
+        <v>public void button42 (View view){ game4[1][2]=currentPlayer; button42.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button42.setText("X"); currentPlayer = 2; } else { button42.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button43 (View view){ game4[1][3]=currentPlayer; button43.setEnabled(false); activeGame3();}</v>
+        <v>public void button43 (View view){ game4[1][3]=currentPlayer; button43.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button43.setText("X"); currentPlayer = 2; } else { button43.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button44 (View view){ game5[1][1]=currentPlayer; button44.setEnabled(false); activeGame1();}</v>
+        <v>public void button44 (View view){ game5[1][1]=currentPlayer; button44.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button44.setText("X"); currentPlayer = 2; } else { button44.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button45 (View view){ game5[1][2]=currentPlayer; button45.setEnabled(false); activeGame2();}</v>
+        <v>public void button45 (View view){ game5[1][2]=currentPlayer; button45.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button45.setText("X"); currentPlayer = 2; } else { button45.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button46 (View view){ game5[1][3]=currentPlayer; button46.setEnabled(false); activeGame3();}</v>
+        <v>public void button46 (View view){ game5[1][3]=currentPlayer; button46.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button46.setText("X"); currentPlayer = 2; } else { button46.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button47 (View view){ game6[1][1]=currentPlayer; button47.setEnabled(false); activeGame1();}</v>
+        <v>public void button47 (View view){ game6[1][1]=currentPlayer; button47.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button47.setText("X"); currentPlayer = 2; } else { button47.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button48 (View view){ game6[1][2]=currentPlayer; button48.setEnabled(false); activeGame2();}</v>
+        <v>public void button48 (View view){ game6[1][2]=currentPlayer; button48.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button48.setText("X"); currentPlayer = 2; } else { button48.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" si="0"/>
-        <v>public void button49 (View view){ game6[1][3]=currentPlayer; button49.setEnabled(false); activeGame3();}</v>
+        <v>public void button49 (View view){ game6[1][3]=currentPlayer; button49.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button49.setText("X"); currentPlayer = 2; } else { button49.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -3345,39 +3993,39 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>public void button51 (View view){ game4[2][1]=currentPlayer; button51.setEnabled(false); activeGame4();}</v>
+        <v>public void button51 (View view){ game4[2][1]=currentPlayer; button51.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button51.setText("X"); currentPlayer = 2; } else { button51.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button52 (View view){ game4[2][2]=currentPlayer; button52.setEnabled(false); activeGame5();}</v>
+        <v>public void button52 (View view){ game4[2][2]=currentPlayer; button52.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button52.setText("X"); currentPlayer = 2; } else { button52.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button53 (View view){ game4[2][3]=currentPlayer; button53.setEnabled(false); activeGame6();}</v>
+        <v>public void button53 (View view){ game4[2][3]=currentPlayer; button53.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button53.setText("X"); currentPlayer = 2; } else { button53.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button54 (View view){ game5[2][1]=currentPlayer; button54.setEnabled(false); activeGame4();}</v>
+        <v>public void button54 (View view){ game5[2][1]=currentPlayer; button54.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button54.setText("X"); currentPlayer = 2; } else { button54.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button55 (View view){ game5[2][2]=currentPlayer; button55.setEnabled(false); activeGame5();}</v>
+        <v>public void button55 (View view){ game5[2][2]=currentPlayer; button55.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button55.setText("X"); currentPlayer = 2; } else { button55.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button56 (View view){ game5[2][3]=currentPlayer; button56.setEnabled(false); activeGame6();}</v>
+        <v>public void button56 (View view){ game5[2][3]=currentPlayer; button56.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button56.setText("X"); currentPlayer = 2; } else { button56.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button57 (View view){ game6[2][1]=currentPlayer; button57.setEnabled(false); activeGame4();}</v>
+        <v>public void button57 (View view){ game6[2][1]=currentPlayer; button57.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button57.setText("X"); currentPlayer = 2; } else { button57.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button58 (View view){ game6[2][2]=currentPlayer; button58.setEnabled(false); activeGame5();}</v>
+        <v>public void button58 (View view){ game6[2][2]=currentPlayer; button58.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button58.setText("X"); currentPlayer = 2; } else { button58.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="0"/>
-        <v>public void button59 (View view){ game6[2][3]=currentPlayer; button59.setEnabled(false); activeGame6();}</v>
+        <v>public void button59 (View view){ game6[2][3]=currentPlayer; button59.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button59.setText("X"); currentPlayer = 2; } else { button59.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -3410,39 +4058,39 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>public void button61 (View view){ game4[3][1]=currentPlayer; button61.setEnabled(false); activeGame7();}</v>
+        <v>public void button61 (View view){ game4[3][1]=currentPlayer; button61.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button61.setText("X"); currentPlayer = 2; } else { button61.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button62 (View view){ game4[3][2]=currentPlayer; button62.setEnabled(false); activeGame8();}</v>
+        <v>public void button62 (View view){ game4[3][2]=currentPlayer; button62.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button62.setText("X"); currentPlayer = 2; } else { button62.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button63 (View view){ game4[3][3]=currentPlayer; button63.setEnabled(false); activeGame9();}</v>
+        <v>public void button63 (View view){ game4[3][3]=currentPlayer; button63.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button63.setText("X"); currentPlayer = 2; } else { button63.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button64 (View view){ game5[3][1]=currentPlayer; button64.setEnabled(false); activeGame7();}</v>
+        <v>public void button64 (View view){ game5[3][1]=currentPlayer; button64.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button64.setText("X"); currentPlayer = 2; } else { button64.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button65 (View view){ game5[3][2]=currentPlayer; button65.setEnabled(false); activeGame8();}</v>
+        <v>public void button65 (View view){ game5[3][2]=currentPlayer; button65.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button65.setText("X"); currentPlayer = 2; } else { button65.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button66 (View view){ game5[3][3]=currentPlayer; button66.setEnabled(false); activeGame9();}</v>
+        <v>public void button66 (View view){ game5[3][3]=currentPlayer; button66.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button66.setText("X"); currentPlayer = 2; } else { button66.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button67 (View view){ game6[3][1]=currentPlayer; button67.setEnabled(false); activeGame7();}</v>
+        <v>public void button67 (View view){ game6[3][1]=currentPlayer; button67.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button67.setText("X"); currentPlayer = 2; } else { button67.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button68 (View view){ game6[3][2]=currentPlayer; button68.setEnabled(false); activeGame8();}</v>
+        <v>public void button68 (View view){ game6[3][2]=currentPlayer; button68.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button68.setText("X"); currentPlayer = 2; } else { button68.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="0"/>
-        <v>public void button69 (View view){ game6[3][3]=currentPlayer; button69.setEnabled(false); activeGame9();}</v>
+        <v>public void button69 (View view){ game6[3][3]=currentPlayer; button69.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button69.setText("X"); currentPlayer = 2; } else { button69.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -3475,39 +4123,39 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>public void button71 (View view){ game7[1][1]=currentPlayer; button71.setEnabled(false); activeGame1();}</v>
+        <v>public void button71 (View view){ game7[1][1]=currentPlayer; button71.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button71.setText("X"); currentPlayer = 2; } else { button71.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button72 (View view){ game7[1][2]=currentPlayer; button72.setEnabled(false); activeGame2();}</v>
+        <v>public void button72 (View view){ game7[1][2]=currentPlayer; button72.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button72.setText("X"); currentPlayer = 2; } else { button72.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button73 (View view){ game7[1][3]=currentPlayer; button73.setEnabled(false); activeGame3();}</v>
+        <v>public void button73 (View view){ game7[1][3]=currentPlayer; button73.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button73.setText("X"); currentPlayer = 2; } else { button73.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button74 (View view){ game8[1][1]=currentPlayer; button74.setEnabled(false); activeGame1();}</v>
+        <v>public void button74 (View view){ game8[1][1]=currentPlayer; button74.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button74.setText("X"); currentPlayer = 2; } else { button74.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button75 (View view){ game8[1][2]=currentPlayer; button75.setEnabled(false); activeGame2();}</v>
+        <v>public void button75 (View view){ game8[1][2]=currentPlayer; button75.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button75.setText("X"); currentPlayer = 2; } else { button75.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button76 (View view){ game8[1][3]=currentPlayer; button76.setEnabled(false); activeGame3();}</v>
+        <v>public void button76 (View view){ game8[1][3]=currentPlayer; button76.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button76.setText("X"); currentPlayer = 2; } else { button76.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button77 (View view){ game9[1][1]=currentPlayer; button77.setEnabled(false); activeGame1();}</v>
+        <v>public void button77 (View view){ game9[1][1]=currentPlayer; button77.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button77.setText("X"); currentPlayer = 2; } else { button77.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button78 (View view){ game9[1][2]=currentPlayer; button78.setEnabled(false); activeGame2();}</v>
+        <v>public void button78 (View view){ game9[1][2]=currentPlayer; button78.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button78.setText("X"); currentPlayer = 2; } else { button78.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="0"/>
-        <v>public void button79 (View view){ game9[1][3]=currentPlayer; button79.setEnabled(false); activeGame3();}</v>
+        <v>public void button79 (View view){ game9[1][3]=currentPlayer; button79.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button79.setText("X"); currentPlayer = 2; } else { button79.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -3540,39 +4188,39 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>public void button81 (View view){ game7[2][1]=currentPlayer; button81.setEnabled(false); activeGame4();}</v>
+        <v>public void button81 (View view){ game7[2][1]=currentPlayer; button81.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button81.setText("X"); currentPlayer = 2; } else { button81.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button82 (View view){ game7[2][2]=currentPlayer; button82.setEnabled(false); activeGame5();}</v>
+        <v>public void button82 (View view){ game7[2][2]=currentPlayer; button82.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button82.setText("X"); currentPlayer = 2; } else { button82.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button83 (View view){ game7[2][3]=currentPlayer; button83.setEnabled(false); activeGame6();}</v>
+        <v>public void button83 (View view){ game7[2][3]=currentPlayer; button83.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button83.setText("X"); currentPlayer = 2; } else { button83.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button84 (View view){ game8[2][1]=currentPlayer; button84.setEnabled(false); activeGame4();}</v>
+        <v>public void button84 (View view){ game8[2][1]=currentPlayer; button84.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button84.setText("X"); currentPlayer = 2; } else { button84.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button85 (View view){ game8[2][2]=currentPlayer; button85.setEnabled(false); activeGame5();}</v>
+        <v>public void button85 (View view){ game8[2][2]=currentPlayer; button85.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button85.setText("X"); currentPlayer = 2; } else { button85.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button86 (View view){ game8[2][3]=currentPlayer; button86.setEnabled(false); activeGame6();}</v>
+        <v>public void button86 (View view){ game8[2][3]=currentPlayer; button86.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button86.setText("X"); currentPlayer = 2; } else { button86.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button87 (View view){ game9[2][1]=currentPlayer; button87.setEnabled(false); activeGame4();}</v>
+        <v>public void button87 (View view){ game9[2][1]=currentPlayer; button87.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button87.setText("X"); currentPlayer = 2; } else { button87.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button88 (View view){ game9[2][2]=currentPlayer; button88.setEnabled(false); activeGame5();}</v>
+        <v>public void button88 (View view){ game9[2][2]=currentPlayer; button88.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button88.setText("X"); currentPlayer = 2; } else { button88.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="0"/>
-        <v>public void button89 (View view){ game9[2][3]=currentPlayer; button89.setEnabled(false); activeGame6();}</v>
+        <v>public void button89 (View view){ game9[2][3]=currentPlayer; button89.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button89.setText("X"); currentPlayer = 2; } else { button89.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -3605,53 +4253,53 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>public void button91 (View view){ game7[3][1]=currentPlayer; button91.setEnabled(false); activeGame7();}</v>
+        <v>public void button91 (View view){ game7[3][1]=currentPlayer; button91.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button91.setText("X"); currentPlayer = 2; } else { button91.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button92 (View view){ game7[3][2]=currentPlayer; button92.setEnabled(false); activeGame8();}</v>
+        <v>public void button92 (View view){ game7[3][2]=currentPlayer; button92.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button92.setText("X"); currentPlayer = 2; } else { button92.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button93 (View view){ game7[3][3]=currentPlayer; button93.setEnabled(false); activeGame9();}</v>
+        <v>public void button93 (View view){ game7[3][3]=currentPlayer; button93.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button93.setText("X"); currentPlayer = 2; } else { button93.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button94 (View view){ game8[3][1]=currentPlayer; button94.setEnabled(false); activeGame7();}</v>
+        <v>public void button94 (View view){ game8[3][1]=currentPlayer; button94.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button94.setText("X"); currentPlayer = 2; } else { button94.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button95 (View view){ game8[3][2]=currentPlayer; button95.setEnabled(false); activeGame8();}</v>
+        <v>public void button95 (View view){ game8[3][2]=currentPlayer; button95.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button95.setText("X"); currentPlayer = 2; } else { button95.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button96 (View view){ game8[3][3]=currentPlayer; button96.setEnabled(false); activeGame9();}</v>
+        <v>public void button96 (View view){ game8[3][3]=currentPlayer; button96.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button96.setText("X"); currentPlayer = 2; } else { button96.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button97 (View view){ game9[3][1]=currentPlayer; button97.setEnabled(false); activeGame7();}</v>
+        <v>public void button97 (View view){ game9[3][1]=currentPlayer; button97.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button97.setText("X"); currentPlayer = 2; } else { button97.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button98 (View view){ game9[3][2]=currentPlayer; button98.setEnabled(false); activeGame8();}</v>
+        <v>public void button98 (View view){ game9[3][2]=currentPlayer; button98.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button98.setText("X"); currentPlayer = 2; } else { button98.setText("O"); currentPlayer = 1; }}</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="0"/>
-        <v>public void button99 (View view){ game9[3][3]=currentPlayer; button99.setEnabled(false); activeGame9();}</v>
+        <v>public void button99 (View view){ game9[3][3]=currentPlayer; button99.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button99.setText("X"); currentPlayer = 2; } else { button99.setText("O"); currentPlayer = 1; }}</v>
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12">
@@ -4266,6 +4914,42 @@
       <c r="I22">
         <v>13</v>
       </c>
+      <c r="K22" t="str">
+        <f>"public void button"&amp;A12&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;A32&amp;"; if (currentGame != "&amp;A2&amp;") return; else { game"&amp;A2&amp;"["&amp;LEFT(A22,1)&amp;"]["&amp;RIGHT(A22,1)&amp;"] = currentPlayer; currentGame="&amp;A32&amp;"; button"&amp;A12&amp;".setEnabled(false); activeGame"&amp;A32&amp;"(); if (currentPlayer == 1) { button"&amp;A12&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;A2&amp;"Win(); currentPlayer = 2; } else { button"&amp;A12&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;A2&amp;"Win(); currentPlayer = 1; } } }"</f>
+        <v>public void button11(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[1][1] = currentPlayer; currentGame=1; button11.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button11.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button11.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" ref="L22:S30" si="12">"public void button"&amp;B12&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;B32&amp;"; if (currentGame != "&amp;B2&amp;") return; else { game"&amp;B2&amp;"["&amp;LEFT(B22,1)&amp;"]["&amp;RIGHT(B22,1)&amp;"] = currentPlayer; currentGame="&amp;B32&amp;"; button"&amp;B12&amp;".setEnabled(false); activeGame"&amp;B32&amp;"(); if (currentPlayer == 1) { button"&amp;B12&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;B2&amp;"Win(); currentPlayer = 2; } else { button"&amp;B12&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;B2&amp;"Win(); currentPlayer = 1; } } }"</f>
+        <v>public void button12(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 1) return; else { game1[1][2] = currentPlayer; currentGame=2; button12.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button12.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button12.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button13(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 1) return; else { game1[1][3] = currentPlayer; currentGame=3; button13.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button13.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button13.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button14(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 2) return; else { game2[1][1] = currentPlayer; currentGame=1; button14.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button14.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button14.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button15(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[1][2] = currentPlayer; currentGame=2; button15.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button15.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button15.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button16(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 2) return; else { game2[1][3] = currentPlayer; currentGame=3; button16.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button16.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button16.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button17(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 3) return; else { game3[1][1] = currentPlayer; currentGame=1; button17.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button17.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button17.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R22" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button18(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 3) return; else { game3[1][2] = currentPlayer; currentGame=2; button18.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button18.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button18.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S22" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button19(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[1][3] = currentPlayer; currentGame=3; button19.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button19.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button19.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23">
@@ -4295,6 +4979,42 @@
       <c r="I23">
         <v>23</v>
       </c>
+      <c r="K23" t="str">
+        <f t="shared" ref="K23:K30" si="13">"public void button"&amp;A13&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;A33&amp;"; if (currentGame != "&amp;A3&amp;") return; else { game"&amp;A3&amp;"["&amp;LEFT(A23,1)&amp;"]["&amp;RIGHT(A23,1)&amp;"] = currentPlayer; currentGame="&amp;A33&amp;"; button"&amp;A13&amp;".setEnabled(false); activeGame"&amp;A33&amp;"(); if (currentPlayer == 1) { button"&amp;A13&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;A3&amp;"Win(); currentPlayer = 2; } else { button"&amp;A13&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;A3&amp;"Win(); currentPlayer = 1; } } }"</f>
+        <v>public void button21(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 1) return; else { game1[2][1] = currentPlayer; currentGame=4; button21.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button21.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button21.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button22(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 1) return; else { game1[2][2] = currentPlayer; currentGame=5; button22.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button22.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button22.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button23(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 1) return; else { game1[2][3] = currentPlayer; currentGame=6; button23.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button23.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button23.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button24(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 2) return; else { game2[2][1] = currentPlayer; currentGame=4; button24.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button24.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button24.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button25(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 2) return; else { game2[2][2] = currentPlayer; currentGame=5; button25.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button25.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button25.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button26(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 2) return; else { game2[2][3] = currentPlayer; currentGame=6; button26.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button26.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button26.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button27(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 3) return; else { game3[2][1] = currentPlayer; currentGame=4; button27.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button27.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button27.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R23" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button28(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 3) return; else { game3[2][2] = currentPlayer; currentGame=5; button28.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button28.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button28.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S23" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button29(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 3) return; else { game3[2][3] = currentPlayer; currentGame=6; button29.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button29.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button29.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="24" spans="1:19">
       <c r="A24">
@@ -4324,6 +5044,42 @@
       <c r="I24">
         <v>33</v>
       </c>
+      <c r="K24" t="str">
+        <f t="shared" si="13"/>
+        <v>public void button31(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 1) return; else { game1[3][1] = currentPlayer; currentGame=7; button31.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button31.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button31.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button32(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 1) return; else { game1[3][2] = currentPlayer; currentGame=8; button32.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button32.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button32.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button33(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 1) return; else { game1[3][3] = currentPlayer; currentGame=9; button33.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button33.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button33.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button34(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 2) return; else { game2[3][1] = currentPlayer; currentGame=7; button34.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button34.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button34.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button35(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 2) return; else { game2[3][2] = currentPlayer; currentGame=8; button35.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button35.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button35.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button36(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 2) return; else { game2[3][3] = currentPlayer; currentGame=9; button36.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button36.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button36.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button37(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 3) return; else { game3[3][1] = currentPlayer; currentGame=7; button37.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button37.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button37.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R24" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button38(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 3) return; else { game3[3][2] = currentPlayer; currentGame=8; button38.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button38.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button38.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button39(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 3) return; else { game3[3][3] = currentPlayer; currentGame=9; button39.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button39.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button39.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="25" spans="1:19">
       <c r="A25">
@@ -4353,6 +5109,42 @@
       <c r="I25">
         <v>13</v>
       </c>
+      <c r="K25" t="str">
+        <f t="shared" si="13"/>
+        <v>public void button41(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 4) return; else { game4[1][1] = currentPlayer; currentGame=1; button41.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button41.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button41.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button42(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 4) return; else { game4[1][2] = currentPlayer; currentGame=2; button42.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button42.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button42.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button43(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 4) return; else { game4[1][3] = currentPlayer; currentGame=3; button43.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button43.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button43.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button44(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 5) return; else { game5[1][1] = currentPlayer; currentGame=1; button44.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button44.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button44.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button45(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 5) return; else { game5[1][2] = currentPlayer; currentGame=2; button45.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button45.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button45.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button46(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 5) return; else { game5[1][3] = currentPlayer; currentGame=3; button46.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button46.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button46.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button47(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 6) return; else { game6[1][1] = currentPlayer; currentGame=1; button47.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button47.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button47.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R25" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button48(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 6) return; else { game6[1][2] = currentPlayer; currentGame=2; button48.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button48.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button48.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button49(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 6) return; else { game6[1][3] = currentPlayer; currentGame=3; button49.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button49.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button49.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26">
@@ -4382,6 +5174,42 @@
       <c r="I26">
         <v>23</v>
       </c>
+      <c r="K26" t="str">
+        <f t="shared" si="13"/>
+        <v>public void button51(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[2][1] = currentPlayer; currentGame=4; button51.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button51.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button51.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button52(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 4) return; else { game4[2][2] = currentPlayer; currentGame=5; button52.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button52.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button52.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button53(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 4) return; else { game4[2][3] = currentPlayer; currentGame=6; button53.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button53.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button53.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button54(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 5) return; else { game5[2][1] = currentPlayer; currentGame=4; button54.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button54.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button54.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button55(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[2][2] = currentPlayer; currentGame=5; button55.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button55.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button55.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button56(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 5) return; else { game5[2][3] = currentPlayer; currentGame=6; button56.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button56.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button56.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button57(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 6) return; else { game6[2][1] = currentPlayer; currentGame=4; button57.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button57.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button57.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R26" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button58(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 6) return; else { game6[2][2] = currentPlayer; currentGame=5; button58.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button58.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button58.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button59(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[2][3] = currentPlayer; currentGame=6; button59.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button59.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button59.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27">
@@ -4411,6 +5239,42 @@
       <c r="I27">
         <v>33</v>
       </c>
+      <c r="K27" t="str">
+        <f t="shared" si="13"/>
+        <v>public void button61(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 4) return; else { game4[3][1] = currentPlayer; currentGame=7; button61.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button61.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button61.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button62(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 4) return; else { game4[3][2] = currentPlayer; currentGame=8; button62.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button62.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button62.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button63(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 4) return; else { game4[3][3] = currentPlayer; currentGame=9; button63.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button63.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button63.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button64(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 5) return; else { game5[3][1] = currentPlayer; currentGame=7; button64.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button64.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button64.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button65(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 5) return; else { game5[3][2] = currentPlayer; currentGame=8; button65.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button65.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button65.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button66(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 5) return; else { game5[3][3] = currentPlayer; currentGame=9; button66.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button66.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button66.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button67(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 6) return; else { game6[3][1] = currentPlayer; currentGame=7; button67.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button67.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button67.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R27" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button68(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 6) return; else { game6[3][2] = currentPlayer; currentGame=8; button68.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button68.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button68.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S27" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button69(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 6) return; else { game6[3][3] = currentPlayer; currentGame=9; button69.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button69.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button69.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28">
@@ -4440,6 +5304,42 @@
       <c r="I28">
         <v>13</v>
       </c>
+      <c r="K28" t="str">
+        <f t="shared" si="13"/>
+        <v>public void button71(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 7) return; else { game7[1][1] = currentPlayer; currentGame=1; button71.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button71.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button71.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button72(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 7) return; else { game7[1][2] = currentPlayer; currentGame=2; button72.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button72.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button72.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button73(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 7) return; else { game7[1][3] = currentPlayer; currentGame=3; button73.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button73.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button73.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button74(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 8) return; else { game8[1][1] = currentPlayer; currentGame=1; button74.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button74.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button74.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button75(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 8) return; else { game8[1][2] = currentPlayer; currentGame=2; button75.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button75.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button75.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button76(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 8) return; else { game8[1][3] = currentPlayer; currentGame=3; button76.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button76.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button76.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button77(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 9) return; else { game9[1][1] = currentPlayer; currentGame=1; button77.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button77.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button77.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R28" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button78(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 9) return; else { game9[1][2] = currentPlayer; currentGame=2; button78.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button78.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button78.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S28" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button79(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 9) return; else { game9[1][3] = currentPlayer; currentGame=3; button79.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button79.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button79.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="29" spans="1:19">
       <c r="A29">
@@ -4469,6 +5369,42 @@
       <c r="I29">
         <v>23</v>
       </c>
+      <c r="K29" t="str">
+        <f t="shared" si="13"/>
+        <v>public void button81(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 7) return; else { game7[2][1] = currentPlayer; currentGame=4; button81.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button81.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button81.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button82(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 7) return; else { game7[2][2] = currentPlayer; currentGame=5; button82.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button82.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button82.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button83(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 7) return; else { game7[2][3] = currentPlayer; currentGame=6; button83.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button83.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button83.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button84(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 8) return; else { game8[2][1] = currentPlayer; currentGame=4; button84.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button84.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button84.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button85(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 8) return; else { game8[2][2] = currentPlayer; currentGame=5; button85.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button85.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button85.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button86(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 8) return; else { game8[2][3] = currentPlayer; currentGame=6; button86.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button86.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button86.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button87(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 9) return; else { game9[2][1] = currentPlayer; currentGame=4; button87.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button87.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button87.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R29" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button88(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 9) return; else { game9[2][2] = currentPlayer; currentGame=5; button88.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button88.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button88.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S29" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button89(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 9) return; else { game9[2][3] = currentPlayer; currentGame=6; button89.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button89.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button89.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30">
@@ -4498,6 +5434,42 @@
       <c r="I30">
         <v>33</v>
       </c>
+      <c r="K30" t="str">
+        <f t="shared" si="13"/>
+        <v>public void button91(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[3][1] = currentPlayer; currentGame=7; button91.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button91.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button91.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button92(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 7) return; else { game7[3][2] = currentPlayer; currentGame=8; button92.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button92.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button92.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button93(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 7) return; else { game7[3][3] = currentPlayer; currentGame=9; button93.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button93.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button93.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button94(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 8) return; else { game8[3][1] = currentPlayer; currentGame=7; button94.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button94.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button94.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button95(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[3][2] = currentPlayer; currentGame=8; button95.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button95.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button95.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button96(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 8) return; else { game8[3][3] = currentPlayer; currentGame=9; button96.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button96.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button96.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button97(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 9) return; else { game9[3][1] = currentPlayer; currentGame=7; button97.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button97.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button97.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="R30" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button98(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 9) return; else { game9[3][2] = currentPlayer; currentGame=8; button98.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button98.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button98.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" si="12"/>
+        <v>public void button99(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[3][3] = currentPlayer; currentGame=9; button99.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button99.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button99.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+      </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32">
@@ -4527,8 +5499,44 @@
       <c r="I32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="K32" t="str">
+        <f>"button"&amp;A12&amp;".setEnabled(false);"</f>
+        <v>button11.setEnabled(false);</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" ref="L32:S40" si="14">"button"&amp;B12&amp;".setEnabled(false);"</f>
+        <v>button12.setEnabled(false);</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="14"/>
+        <v>button13.setEnabled(false);</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="14"/>
+        <v>button14.setEnabled(false);</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="14"/>
+        <v>button15.setEnabled(false);</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="14"/>
+        <v>button16.setEnabled(false);</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="14"/>
+        <v>button17.setEnabled(false);</v>
+      </c>
+      <c r="R32" t="str">
+        <f t="shared" si="14"/>
+        <v>button18.setEnabled(false);</v>
+      </c>
+      <c r="S32" t="str">
+        <f t="shared" si="14"/>
+        <v>button19.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>4</v>
       </c>
@@ -4556,8 +5564,44 @@
       <c r="I33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="K33" t="str">
+        <f t="shared" ref="K33:K40" si="15">"button"&amp;A13&amp;".setEnabled(false);"</f>
+        <v>button21.setEnabled(false);</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="14"/>
+        <v>button22.setEnabled(false);</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="14"/>
+        <v>button23.setEnabled(false);</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="14"/>
+        <v>button24.setEnabled(false);</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="14"/>
+        <v>button25.setEnabled(false);</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="14"/>
+        <v>button26.setEnabled(false);</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="14"/>
+        <v>button27.setEnabled(false);</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="14"/>
+        <v>button28.setEnabled(false);</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="14"/>
+        <v>button29.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>7</v>
       </c>
@@ -4585,8 +5629,44 @@
       <c r="I34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="K34" t="str">
+        <f t="shared" si="15"/>
+        <v>button31.setEnabled(false);</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="14"/>
+        <v>button32.setEnabled(false);</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="14"/>
+        <v>button33.setEnabled(false);</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="14"/>
+        <v>button34.setEnabled(false);</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="14"/>
+        <v>button35.setEnabled(false);</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="14"/>
+        <v>button36.setEnabled(false);</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="14"/>
+        <v>button37.setEnabled(false);</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="14"/>
+        <v>button38.setEnabled(false);</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="14"/>
+        <v>button39.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>1</v>
       </c>
@@ -4614,8 +5694,44 @@
       <c r="I35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="K35" t="str">
+        <f t="shared" si="15"/>
+        <v>button41.setEnabled(false);</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="14"/>
+        <v>button42.setEnabled(false);</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="14"/>
+        <v>button43.setEnabled(false);</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="14"/>
+        <v>button44.setEnabled(false);</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="14"/>
+        <v>button45.setEnabled(false);</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="14"/>
+        <v>button46.setEnabled(false);</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="14"/>
+        <v>button47.setEnabled(false);</v>
+      </c>
+      <c r="R35" t="str">
+        <f t="shared" si="14"/>
+        <v>button48.setEnabled(false);</v>
+      </c>
+      <c r="S35" t="str">
+        <f t="shared" si="14"/>
+        <v>button49.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>4</v>
       </c>
@@ -4643,8 +5759,44 @@
       <c r="I36">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="K36" t="str">
+        <f t="shared" si="15"/>
+        <v>button51.setEnabled(false);</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="14"/>
+        <v>button52.setEnabled(false);</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="14"/>
+        <v>button53.setEnabled(false);</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="14"/>
+        <v>button54.setEnabled(false);</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="14"/>
+        <v>button55.setEnabled(false);</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="14"/>
+        <v>button56.setEnabled(false);</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" si="14"/>
+        <v>button57.setEnabled(false);</v>
+      </c>
+      <c r="R36" t="str">
+        <f t="shared" si="14"/>
+        <v>button58.setEnabled(false);</v>
+      </c>
+      <c r="S36" t="str">
+        <f t="shared" si="14"/>
+        <v>button59.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37">
         <v>7</v>
       </c>
@@ -4672,8 +5824,44 @@
       <c r="I37">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="K37" t="str">
+        <f t="shared" si="15"/>
+        <v>button61.setEnabled(false);</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="14"/>
+        <v>button62.setEnabled(false);</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="14"/>
+        <v>button63.setEnabled(false);</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="14"/>
+        <v>button64.setEnabled(false);</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="14"/>
+        <v>button65.setEnabled(false);</v>
+      </c>
+      <c r="P37" t="str">
+        <f t="shared" si="14"/>
+        <v>button66.setEnabled(false);</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" si="14"/>
+        <v>button67.setEnabled(false);</v>
+      </c>
+      <c r="R37" t="str">
+        <f t="shared" si="14"/>
+        <v>button68.setEnabled(false);</v>
+      </c>
+      <c r="S37" t="str">
+        <f t="shared" si="14"/>
+        <v>button69.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38">
         <v>1</v>
       </c>
@@ -4701,8 +5889,44 @@
       <c r="I38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="K38" t="str">
+        <f t="shared" si="15"/>
+        <v>button71.setEnabled(false);</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="14"/>
+        <v>button72.setEnabled(false);</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="14"/>
+        <v>button73.setEnabled(false);</v>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="14"/>
+        <v>button74.setEnabled(false);</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="14"/>
+        <v>button75.setEnabled(false);</v>
+      </c>
+      <c r="P38" t="str">
+        <f t="shared" si="14"/>
+        <v>button76.setEnabled(false);</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="14"/>
+        <v>button77.setEnabled(false);</v>
+      </c>
+      <c r="R38" t="str">
+        <f t="shared" si="14"/>
+        <v>button78.setEnabled(false);</v>
+      </c>
+      <c r="S38" t="str">
+        <f t="shared" si="14"/>
+        <v>button79.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39">
         <v>4</v>
       </c>
@@ -4730,8 +5954,44 @@
       <c r="I39">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="K39" t="str">
+        <f t="shared" si="15"/>
+        <v>button81.setEnabled(false);</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="14"/>
+        <v>button82.setEnabled(false);</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="14"/>
+        <v>button83.setEnabled(false);</v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="14"/>
+        <v>button84.setEnabled(false);</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="14"/>
+        <v>button85.setEnabled(false);</v>
+      </c>
+      <c r="P39" t="str">
+        <f t="shared" si="14"/>
+        <v>button86.setEnabled(false);</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="14"/>
+        <v>button87.setEnabled(false);</v>
+      </c>
+      <c r="R39" t="str">
+        <f t="shared" si="14"/>
+        <v>button88.setEnabled(false);</v>
+      </c>
+      <c r="S39" t="str">
+        <f t="shared" si="14"/>
+        <v>button89.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40">
         <v>7</v>
       </c>
@@ -4758,6 +6018,384 @@
       </c>
       <c r="I40">
         <v>9</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="15"/>
+        <v>button91.setEnabled(false);</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="14"/>
+        <v>button92.setEnabled(false);</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="14"/>
+        <v>button93.setEnabled(false);</v>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="14"/>
+        <v>button94.setEnabled(false);</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="14"/>
+        <v>button95.setEnabled(false);</v>
+      </c>
+      <c r="P40" t="str">
+        <f t="shared" si="14"/>
+        <v>button96.setEnabled(false);</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="14"/>
+        <v>button97.setEnabled(false);</v>
+      </c>
+      <c r="R40" t="str">
+        <f t="shared" si="14"/>
+        <v>button98.setEnabled(false);</v>
+      </c>
+      <c r="S40" t="str">
+        <f t="shared" si="14"/>
+        <v>button99.setEnabled(false);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="K42" t="str">
+        <f>"button"&amp;A12&amp;".getBackground().setColorFilter(null);"</f>
+        <v>button11.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" ref="L42:S50" si="16">"button"&amp;B12&amp;".getBackground().setColorFilter(null);"</f>
+        <v>button12.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="16"/>
+        <v>button13.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N42" t="str">
+        <f t="shared" si="16"/>
+        <v>button14.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="16"/>
+        <v>button15.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P42" t="str">
+        <f t="shared" si="16"/>
+        <v>button16.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q42" t="str">
+        <f t="shared" si="16"/>
+        <v>button17.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R42" t="str">
+        <f t="shared" si="16"/>
+        <v>button18.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S42" t="str">
+        <f t="shared" si="16"/>
+        <v>button19.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="K43" t="str">
+        <f t="shared" ref="K43:K50" si="17">"button"&amp;A13&amp;".getBackground().setColorFilter(null);"</f>
+        <v>button21.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="16"/>
+        <v>button22.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="16"/>
+        <v>button23.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="16"/>
+        <v>button24.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="16"/>
+        <v>button25.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P43" t="str">
+        <f t="shared" si="16"/>
+        <v>button26.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q43" t="str">
+        <f t="shared" si="16"/>
+        <v>button27.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R43" t="str">
+        <f t="shared" si="16"/>
+        <v>button28.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S43" t="str">
+        <f t="shared" si="16"/>
+        <v>button29.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="K44" t="str">
+        <f t="shared" si="17"/>
+        <v>button31.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="16"/>
+        <v>button32.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="16"/>
+        <v>button33.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="16"/>
+        <v>button34.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" si="16"/>
+        <v>button35.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P44" t="str">
+        <f t="shared" si="16"/>
+        <v>button36.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q44" t="str">
+        <f t="shared" si="16"/>
+        <v>button37.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R44" t="str">
+        <f t="shared" si="16"/>
+        <v>button38.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S44" t="str">
+        <f t="shared" si="16"/>
+        <v>button39.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="K45" t="str">
+        <f t="shared" si="17"/>
+        <v>button41.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="16"/>
+        <v>button42.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="16"/>
+        <v>button43.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="16"/>
+        <v>button44.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O45" t="str">
+        <f t="shared" si="16"/>
+        <v>button45.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P45" t="str">
+        <f t="shared" si="16"/>
+        <v>button46.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q45" t="str">
+        <f t="shared" si="16"/>
+        <v>button47.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R45" t="str">
+        <f t="shared" si="16"/>
+        <v>button48.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S45" t="str">
+        <f t="shared" si="16"/>
+        <v>button49.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="K46" t="str">
+        <f t="shared" si="17"/>
+        <v>button51.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="16"/>
+        <v>button52.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="16"/>
+        <v>button53.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="16"/>
+        <v>button54.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O46" t="str">
+        <f t="shared" si="16"/>
+        <v>button55.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P46" t="str">
+        <f t="shared" si="16"/>
+        <v>button56.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q46" t="str">
+        <f t="shared" si="16"/>
+        <v>button57.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R46" t="str">
+        <f t="shared" si="16"/>
+        <v>button58.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S46" t="str">
+        <f t="shared" si="16"/>
+        <v>button59.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="K47" t="str">
+        <f t="shared" si="17"/>
+        <v>button61.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="16"/>
+        <v>button62.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="16"/>
+        <v>button63.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="16"/>
+        <v>button64.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O47" t="str">
+        <f t="shared" si="16"/>
+        <v>button65.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P47" t="str">
+        <f t="shared" si="16"/>
+        <v>button66.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q47" t="str">
+        <f t="shared" si="16"/>
+        <v>button67.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R47" t="str">
+        <f t="shared" si="16"/>
+        <v>button68.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S47" t="str">
+        <f t="shared" si="16"/>
+        <v>button69.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="K48" t="str">
+        <f t="shared" si="17"/>
+        <v>button71.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="16"/>
+        <v>button72.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="16"/>
+        <v>button73.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="16"/>
+        <v>button74.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O48" t="str">
+        <f t="shared" si="16"/>
+        <v>button75.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P48" t="str">
+        <f t="shared" si="16"/>
+        <v>button76.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q48" t="str">
+        <f t="shared" si="16"/>
+        <v>button77.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R48" t="str">
+        <f t="shared" si="16"/>
+        <v>button78.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S48" t="str">
+        <f t="shared" si="16"/>
+        <v>button79.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="49" spans="11:19">
+      <c r="K49" t="str">
+        <f t="shared" si="17"/>
+        <v>button81.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="16"/>
+        <v>button82.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M49" t="str">
+        <f t="shared" si="16"/>
+        <v>button83.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N49" t="str">
+        <f t="shared" si="16"/>
+        <v>button84.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O49" t="str">
+        <f t="shared" si="16"/>
+        <v>button85.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P49" t="str">
+        <f t="shared" si="16"/>
+        <v>button86.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q49" t="str">
+        <f t="shared" si="16"/>
+        <v>button87.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R49" t="str">
+        <f t="shared" si="16"/>
+        <v>button88.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S49" t="str">
+        <f t="shared" si="16"/>
+        <v>button89.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="50" spans="11:19">
+      <c r="K50" t="str">
+        <f t="shared" si="17"/>
+        <v>button91.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="16"/>
+        <v>button92.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" si="16"/>
+        <v>button93.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="N50" t="str">
+        <f t="shared" si="16"/>
+        <v>button94.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="O50" t="str">
+        <f t="shared" si="16"/>
+        <v>button95.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="P50" t="str">
+        <f t="shared" si="16"/>
+        <v>button96.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="Q50" t="str">
+        <f t="shared" si="16"/>
+        <v>button97.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="R50" t="str">
+        <f t="shared" si="16"/>
+        <v>button98.getBackground().setColorFilter(null);</v>
+      </c>
+      <c r="S50" t="str">
+        <f t="shared" si="16"/>
+        <v>button99.getBackground().setColorFilter(null);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolve selection bug and improve reset function
</commit_message>
<xml_diff>
--- a/_DESIGN/Book4b.xlsx
+++ b/_DESIGN/Book4b.xlsx
@@ -1634,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F81"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1646,7 +1646,7 @@
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1670,8 +1670,12 @@
         <f>A1&amp;".setEnabled(false);"</f>
         <v>button11.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="str">
+        <f>A1&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;");"</f>
+        <v>button11.setText("");</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1695,8 +1699,12 @@
         <f t="shared" ref="F2:F65" si="4">A2&amp;".setEnabled(false);"</f>
         <v>button12.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G65" si="5">A2&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;");"</f>
+        <v>button12.setText("");</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1720,8 +1728,12 @@
         <f t="shared" si="4"/>
         <v>button13.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="str">
+        <f t="shared" si="5"/>
+        <v>button13.setText("");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1745,8 +1757,12 @@
         <f t="shared" si="4"/>
         <v>button14.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="str">
+        <f t="shared" si="5"/>
+        <v>button14.setText("");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1770,8 +1786,12 @@
         <f t="shared" si="4"/>
         <v>button15.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="str">
+        <f t="shared" si="5"/>
+        <v>button15.setText("");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1795,8 +1815,12 @@
         <f t="shared" si="4"/>
         <v>button16.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="str">
+        <f t="shared" si="5"/>
+        <v>button16.setText("");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1820,8 +1844,12 @@
         <f t="shared" si="4"/>
         <v>button17.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="str">
+        <f t="shared" si="5"/>
+        <v>button17.setText("");</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1845,8 +1873,12 @@
         <f t="shared" si="4"/>
         <v>button18.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="str">
+        <f t="shared" si="5"/>
+        <v>button18.setText("");</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1870,8 +1902,12 @@
         <f t="shared" si="4"/>
         <v>button19.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="str">
+        <f t="shared" si="5"/>
+        <v>button19.setText("");</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1895,8 +1931,12 @@
         <f t="shared" si="4"/>
         <v>button21.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="str">
+        <f t="shared" si="5"/>
+        <v>button21.setText("");</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1920,8 +1960,12 @@
         <f t="shared" si="4"/>
         <v>button22.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="str">
+        <f t="shared" si="5"/>
+        <v>button22.setText("");</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1945,8 +1989,12 @@
         <f t="shared" si="4"/>
         <v>button23.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="str">
+        <f t="shared" si="5"/>
+        <v>button23.setText("");</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1970,8 +2018,12 @@
         <f t="shared" si="4"/>
         <v>button24.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="str">
+        <f t="shared" si="5"/>
+        <v>button24.setText("");</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1995,8 +2047,12 @@
         <f t="shared" si="4"/>
         <v>button25.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="str">
+        <f t="shared" si="5"/>
+        <v>button25.setText("");</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2020,8 +2076,12 @@
         <f t="shared" si="4"/>
         <v>button26.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" t="str">
+        <f t="shared" si="5"/>
+        <v>button26.setText("");</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2045,8 +2105,12 @@
         <f t="shared" si="4"/>
         <v>button27.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" t="str">
+        <f t="shared" si="5"/>
+        <v>button27.setText("");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2070,8 +2134,12 @@
         <f t="shared" si="4"/>
         <v>button28.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" t="str">
+        <f t="shared" si="5"/>
+        <v>button28.setText("");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2095,8 +2163,12 @@
         <f t="shared" si="4"/>
         <v>button29.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="str">
+        <f t="shared" si="5"/>
+        <v>button29.setText("");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2120,8 +2192,12 @@
         <f t="shared" si="4"/>
         <v>button31.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="str">
+        <f t="shared" si="5"/>
+        <v>button31.setText("");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2145,8 +2221,12 @@
         <f t="shared" si="4"/>
         <v>button32.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" t="str">
+        <f t="shared" si="5"/>
+        <v>button32.setText("");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2170,8 +2250,12 @@
         <f t="shared" si="4"/>
         <v>button33.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" t="str">
+        <f t="shared" si="5"/>
+        <v>button33.setText("");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2195,8 +2279,12 @@
         <f t="shared" si="4"/>
         <v>button34.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" t="str">
+        <f t="shared" si="5"/>
+        <v>button34.setText("");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2220,8 +2308,12 @@
         <f t="shared" si="4"/>
         <v>button35.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" t="str">
+        <f t="shared" si="5"/>
+        <v>button35.setText("");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2245,8 +2337,12 @@
         <f t="shared" si="4"/>
         <v>button36.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" t="str">
+        <f t="shared" si="5"/>
+        <v>button36.setText("");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2270,8 +2366,12 @@
         <f t="shared" si="4"/>
         <v>button37.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" t="str">
+        <f t="shared" si="5"/>
+        <v>button37.setText("");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2295,8 +2395,12 @@
         <f t="shared" si="4"/>
         <v>button38.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" t="str">
+        <f t="shared" si="5"/>
+        <v>button38.setText("");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2320,8 +2424,12 @@
         <f t="shared" si="4"/>
         <v>button39.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" t="str">
+        <f t="shared" si="5"/>
+        <v>button39.setText("");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2345,8 +2453,12 @@
         <f t="shared" si="4"/>
         <v>button41.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" t="str">
+        <f t="shared" si="5"/>
+        <v>button41.setText("");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2370,8 +2482,12 @@
         <f t="shared" si="4"/>
         <v>button42.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" t="str">
+        <f t="shared" si="5"/>
+        <v>button42.setText("");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2395,8 +2511,12 @@
         <f t="shared" si="4"/>
         <v>button43.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" t="str">
+        <f t="shared" si="5"/>
+        <v>button43.setText("");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2420,8 +2540,12 @@
         <f t="shared" si="4"/>
         <v>button44.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" t="str">
+        <f t="shared" si="5"/>
+        <v>button44.setText("");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2445,8 +2569,12 @@
         <f t="shared" si="4"/>
         <v>button45.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" t="str">
+        <f t="shared" si="5"/>
+        <v>button45.setText("");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2470,8 +2598,12 @@
         <f t="shared" si="4"/>
         <v>button46.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" t="str">
+        <f t="shared" si="5"/>
+        <v>button46.setText("");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2495,8 +2627,12 @@
         <f t="shared" si="4"/>
         <v>button47.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" t="str">
+        <f t="shared" si="5"/>
+        <v>button47.setText("");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2520,8 +2656,12 @@
         <f t="shared" si="4"/>
         <v>button48.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" t="str">
+        <f t="shared" si="5"/>
+        <v>button48.setText("");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2545,8 +2685,12 @@
         <f t="shared" si="4"/>
         <v>button49.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" t="str">
+        <f t="shared" si="5"/>
+        <v>button49.setText("");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2570,8 +2714,12 @@
         <f t="shared" si="4"/>
         <v>button51.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" t="str">
+        <f t="shared" si="5"/>
+        <v>button51.setText("");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2595,8 +2743,12 @@
         <f t="shared" si="4"/>
         <v>button52.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" t="str">
+        <f t="shared" si="5"/>
+        <v>button52.setText("");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2620,8 +2772,12 @@
         <f t="shared" si="4"/>
         <v>button53.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39" t="str">
+        <f t="shared" si="5"/>
+        <v>button53.setText("");</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2645,8 +2801,12 @@
         <f t="shared" si="4"/>
         <v>button54.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40" t="str">
+        <f t="shared" si="5"/>
+        <v>button54.setText("");</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2670,8 +2830,12 @@
         <f t="shared" si="4"/>
         <v>button55.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" t="str">
+        <f t="shared" si="5"/>
+        <v>button55.setText("");</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2695,8 +2859,12 @@
         <f t="shared" si="4"/>
         <v>button56.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42" t="str">
+        <f t="shared" si="5"/>
+        <v>button56.setText("");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2720,8 +2888,12 @@
         <f t="shared" si="4"/>
         <v>button57.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43" t="str">
+        <f t="shared" si="5"/>
+        <v>button57.setText("");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2745,8 +2917,12 @@
         <f t="shared" si="4"/>
         <v>button58.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" t="str">
+        <f t="shared" si="5"/>
+        <v>button58.setText("");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2770,8 +2946,12 @@
         <f t="shared" si="4"/>
         <v>button59.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45" t="str">
+        <f t="shared" si="5"/>
+        <v>button59.setText("");</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2795,8 +2975,12 @@
         <f t="shared" si="4"/>
         <v>button61.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46" t="str">
+        <f t="shared" si="5"/>
+        <v>button61.setText("");</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2820,8 +3004,12 @@
         <f t="shared" si="4"/>
         <v>button62.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47" t="str">
+        <f t="shared" si="5"/>
+        <v>button62.setText("");</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2845,8 +3033,12 @@
         <f t="shared" si="4"/>
         <v>button63.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" t="str">
+        <f t="shared" si="5"/>
+        <v>button63.setText("");</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2870,8 +3062,12 @@
         <f t="shared" si="4"/>
         <v>button64.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49" t="str">
+        <f t="shared" si="5"/>
+        <v>button64.setText("");</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2895,8 +3091,12 @@
         <f t="shared" si="4"/>
         <v>button65.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50" t="str">
+        <f t="shared" si="5"/>
+        <v>button65.setText("");</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2920,8 +3120,12 @@
         <f t="shared" si="4"/>
         <v>button66.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" t="str">
+        <f t="shared" si="5"/>
+        <v>button66.setText("");</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2945,8 +3149,12 @@
         <f t="shared" si="4"/>
         <v>button67.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52" t="str">
+        <f t="shared" si="5"/>
+        <v>button67.setText("");</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2970,8 +3178,12 @@
         <f t="shared" si="4"/>
         <v>button68.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53" t="str">
+        <f t="shared" si="5"/>
+        <v>button68.setText("");</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2995,8 +3207,12 @@
         <f t="shared" si="4"/>
         <v>button69.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54" t="str">
+        <f t="shared" si="5"/>
+        <v>button69.setText("");</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -3020,8 +3236,12 @@
         <f t="shared" si="4"/>
         <v>button71.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55" t="str">
+        <f t="shared" si="5"/>
+        <v>button71.setText("");</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -3045,8 +3265,12 @@
         <f t="shared" si="4"/>
         <v>button72.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56" t="str">
+        <f t="shared" si="5"/>
+        <v>button72.setText("");</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -3070,8 +3294,12 @@
         <f t="shared" si="4"/>
         <v>button73.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57" t="str">
+        <f t="shared" si="5"/>
+        <v>button73.setText("");</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3095,8 +3323,12 @@
         <f t="shared" si="4"/>
         <v>button74.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58" t="str">
+        <f t="shared" si="5"/>
+        <v>button74.setText("");</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -3120,8 +3352,12 @@
         <f t="shared" si="4"/>
         <v>button75.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59" t="str">
+        <f t="shared" si="5"/>
+        <v>button75.setText("");</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -3145,8 +3381,12 @@
         <f t="shared" si="4"/>
         <v>button76.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60" t="str">
+        <f t="shared" si="5"/>
+        <v>button76.setText("");</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -3170,8 +3410,12 @@
         <f t="shared" si="4"/>
         <v>button77.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61" t="str">
+        <f t="shared" si="5"/>
+        <v>button77.setText("");</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -3195,8 +3439,12 @@
         <f t="shared" si="4"/>
         <v>button78.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62" t="str">
+        <f t="shared" si="5"/>
+        <v>button78.setText("");</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -3220,8 +3468,12 @@
         <f t="shared" si="4"/>
         <v>button79.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63" t="str">
+        <f t="shared" si="5"/>
+        <v>button79.setText("");</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -3245,8 +3497,12 @@
         <f t="shared" si="4"/>
         <v>button81.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64" t="str">
+        <f t="shared" si="5"/>
+        <v>button81.setText("");</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -3270,405 +3526,473 @@
         <f t="shared" si="4"/>
         <v>button82.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65" t="str">
+        <f t="shared" si="5"/>
+        <v>button82.setText("");</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B81" si="5">"Button "&amp;A66&amp;";"</f>
+        <f t="shared" ref="B66:B81" si="6">"Button "&amp;A66&amp;";"</f>
         <v>Button button83;</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C81" si="6">A66&amp;" = findViewById(R.id."&amp;A66&amp;");"</f>
+        <f t="shared" ref="C66:C81" si="7">A66&amp;" = findViewById(R.id."&amp;A66&amp;");"</f>
         <v>button83 = findViewById(R.id.button83);</v>
       </c>
       <c r="D66" s="9" t="str">
-        <f t="shared" ref="D66:D81" si="7">A66&amp;".getBackground().setColorFilter(null);"</f>
+        <f t="shared" ref="D66:D81" si="8">A66&amp;".getBackground().setColorFilter(null);"</f>
         <v>button83.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E81" si="8">A66&amp;".setEnabled(true);"</f>
+        <f t="shared" ref="E66:E81" si="9">A66&amp;".setEnabled(true);"</f>
         <v>button83.setEnabled(true);</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ref="F66:F81" si="9">A66&amp;".setEnabled(false);"</f>
+        <f t="shared" ref="F66:F81" si="10">A66&amp;".setEnabled(false);"</f>
         <v>button83.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66" t="str">
+        <f t="shared" ref="G66:G81" si="11">A66&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;");"</f>
+        <v>button83.setText("");</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>66</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button84;</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button84 = findViewById(R.id.button84);</v>
       </c>
       <c r="D67" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button84.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button84.setEnabled(true);</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button84.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67" t="str">
+        <f t="shared" si="11"/>
+        <v>button84.setText("");</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>67</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button85;</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button85 = findViewById(R.id.button85);</v>
       </c>
       <c r="D68" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button85.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button85.setEnabled(true);</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button85.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68" t="str">
+        <f t="shared" si="11"/>
+        <v>button85.setText("");</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>68</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button86;</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button86 = findViewById(R.id.button86);</v>
       </c>
       <c r="D69" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button86.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button86.setEnabled(true);</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button86.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69" t="str">
+        <f t="shared" si="11"/>
+        <v>button86.setText("");</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>69</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button87;</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button87 = findViewById(R.id.button87);</v>
       </c>
       <c r="D70" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button87.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button87.setEnabled(true);</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button87.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70" t="str">
+        <f t="shared" si="11"/>
+        <v>button87.setText("");</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>70</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button88;</v>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button88 = findViewById(R.id.button88);</v>
       </c>
       <c r="D71" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button88.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button88.setEnabled(true);</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button88.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71" t="str">
+        <f t="shared" si="11"/>
+        <v>button88.setText("");</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>71</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button89;</v>
       </c>
       <c r="C72" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button89 = findViewById(R.id.button89);</v>
       </c>
       <c r="D72" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button89.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button89.setEnabled(true);</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button89.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72" t="str">
+        <f t="shared" si="11"/>
+        <v>button89.setText("");</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>72</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button91;</v>
       </c>
       <c r="C73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button91 = findViewById(R.id.button91);</v>
       </c>
       <c r="D73" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button91.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button91.setEnabled(true);</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button91.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73" t="str">
+        <f t="shared" si="11"/>
+        <v>button91.setText("");</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>73</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button92;</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button92 = findViewById(R.id.button92);</v>
       </c>
       <c r="D74" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button92.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button92.setEnabled(true);</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button92.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74" t="str">
+        <f t="shared" si="11"/>
+        <v>button92.setText("");</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>74</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button93;</v>
       </c>
       <c r="C75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button93 = findViewById(R.id.button93);</v>
       </c>
       <c r="D75" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button93.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button93.setEnabled(true);</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button93.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75" t="str">
+        <f t="shared" si="11"/>
+        <v>button93.setText("");</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>75</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button94;</v>
       </c>
       <c r="C76" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button94 = findViewById(R.id.button94);</v>
       </c>
       <c r="D76" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button94.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button94.setEnabled(true);</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button94.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76" t="str">
+        <f t="shared" si="11"/>
+        <v>button94.setText("");</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>76</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button95;</v>
       </c>
       <c r="C77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button95 = findViewById(R.id.button95);</v>
       </c>
       <c r="D77" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button95.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button95.setEnabled(true);</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button95.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77" t="str">
+        <f t="shared" si="11"/>
+        <v>button95.setText("");</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>77</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button96;</v>
       </c>
       <c r="C78" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button96 = findViewById(R.id.button96);</v>
       </c>
       <c r="D78" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button96.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button96.setEnabled(true);</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button96.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78" t="str">
+        <f t="shared" si="11"/>
+        <v>button96.setText("");</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>78</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button97;</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button97 = findViewById(R.id.button97);</v>
       </c>
       <c r="D79" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button97.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button97.setEnabled(true);</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button97.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79" t="str">
+        <f t="shared" si="11"/>
+        <v>button97.setText("");</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>79</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button98;</v>
       </c>
       <c r="C80" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button98 = findViewById(R.id.button98);</v>
       </c>
       <c r="D80" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button98.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button98.setEnabled(true);</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button98.setEnabled(false);</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80" t="str">
+        <f t="shared" si="11"/>
+        <v>button98.setText("");</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>80</v>
       </c>
       <c r="B81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Button button99;</v>
       </c>
       <c r="C81" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>button99 = findViewById(R.id.button99);</v>
       </c>
       <c r="D81" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>button99.getBackground().setColorFilter(null);</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>button99.setEnabled(true);</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>button99.setEnabled(false);</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="11"/>
+        <v>button99.setText("");</v>
       </c>
     </row>
   </sheetData>
@@ -3681,8 +4005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O10" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4915,20 +5239,20 @@
         <v>13</v>
       </c>
       <c r="K22" t="str">
-        <f>"public void button"&amp;A12&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;A32&amp;"; if (currentGame != "&amp;A2&amp;") return; else { game"&amp;A2&amp;"["&amp;LEFT(A22,1)&amp;"]["&amp;RIGHT(A22,1)&amp;"] = currentPlayer; currentGame="&amp;A32&amp;"; button"&amp;A12&amp;".setEnabled(false); activeGame"&amp;A32&amp;"(); if (currentPlayer == 1) { button"&amp;A12&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;A2&amp;"Win(); currentPlayer = 2; } else { button"&amp;A12&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;A2&amp;"Win(); currentPlayer = 1; } } }"</f>
+        <f>"public void button"&amp;A12&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;A2&amp;"; if (currentGame != "&amp;A2&amp;") return; else { game"&amp;A2&amp;"["&amp;LEFT(A22,1)&amp;"]["&amp;RIGHT(A22,1)&amp;"] = currentPlayer; currentGame="&amp;A32&amp;"; button"&amp;A12&amp;".setEnabled(false); activeGame"&amp;A32&amp;"(); if (currentPlayer == 1) { button"&amp;A12&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;A2&amp;"Win(); currentPlayer = 2; } else { button"&amp;A12&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;A2&amp;"Win(); currentPlayer = 1; } } }"</f>
         <v>public void button11(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[1][1] = currentPlayer; currentGame=1; button11.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button11.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button11.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" ref="L22:S30" si="12">"public void button"&amp;B12&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;B32&amp;"; if (currentGame != "&amp;B2&amp;") return; else { game"&amp;B2&amp;"["&amp;LEFT(B22,1)&amp;"]["&amp;RIGHT(B22,1)&amp;"] = currentPlayer; currentGame="&amp;B32&amp;"; button"&amp;B12&amp;".setEnabled(false); activeGame"&amp;B32&amp;"(); if (currentPlayer == 1) { button"&amp;B12&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;B2&amp;"Win(); currentPlayer = 2; } else { button"&amp;B12&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;B2&amp;"Win(); currentPlayer = 1; } } }"</f>
-        <v>public void button12(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 1) return; else { game1[1][2] = currentPlayer; currentGame=2; button12.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button12.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button12.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+        <f t="shared" ref="L22:S30" si="12">"public void button"&amp;B12&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;B2&amp;"; if (currentGame != "&amp;B2&amp;") return; else { game"&amp;B2&amp;"["&amp;LEFT(B22,1)&amp;"]["&amp;RIGHT(B22,1)&amp;"] = currentPlayer; currentGame="&amp;B32&amp;"; button"&amp;B12&amp;".setEnabled(false); activeGame"&amp;B32&amp;"(); if (currentPlayer == 1) { button"&amp;B12&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;B2&amp;"Win(); currentPlayer = 2; } else { button"&amp;B12&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;B2&amp;"Win(); currentPlayer = 1; } } }"</f>
+        <v>public void button12(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[1][2] = currentPlayer; currentGame=2; button12.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button12.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button12.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="12"/>
-        <v>public void button13(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 1) return; else { game1[1][3] = currentPlayer; currentGame=3; button13.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button13.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button13.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+        <v>public void button13(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[1][3] = currentPlayer; currentGame=3; button13.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button13.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button13.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="12"/>
-        <v>public void button14(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 2) return; else { game2[1][1] = currentPlayer; currentGame=1; button14.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button14.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button14.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+        <v>public void button14(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[1][1] = currentPlayer; currentGame=1; button14.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button14.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button14.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="12"/>
@@ -4936,15 +5260,15 @@
       </c>
       <c r="P22" t="str">
         <f t="shared" si="12"/>
-        <v>public void button16(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 2) return; else { game2[1][3] = currentPlayer; currentGame=3; button16.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button16.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button16.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+        <v>public void button16(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[1][3] = currentPlayer; currentGame=3; button16.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button16.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button16.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="12"/>
-        <v>public void button17(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 3) return; else { game3[1][1] = currentPlayer; currentGame=1; button17.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button17.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button17.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+        <v>public void button17(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[1][1] = currentPlayer; currentGame=1; button17.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button17.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button17.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R22" t="str">
         <f t="shared" si="12"/>
-        <v>public void button18(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 3) return; else { game3[1][2] = currentPlayer; currentGame=2; button18.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button18.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button18.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+        <v>public void button18(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[1][2] = currentPlayer; currentGame=2; button18.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button18.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button18.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S22" t="str">
         <f t="shared" si="12"/>
@@ -4980,40 +5304,40 @@
         <v>23</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" ref="K23:K30" si="13">"public void button"&amp;A13&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;A33&amp;"; if (currentGame != "&amp;A3&amp;") return; else { game"&amp;A3&amp;"["&amp;LEFT(A23,1)&amp;"]["&amp;RIGHT(A23,1)&amp;"] = currentPlayer; currentGame="&amp;A33&amp;"; button"&amp;A13&amp;".setEnabled(false); activeGame"&amp;A33&amp;"(); if (currentPlayer == 1) { button"&amp;A13&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;A3&amp;"Win(); currentPlayer = 2; } else { button"&amp;A13&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;A3&amp;"Win(); currentPlayer = 1; } } }"</f>
-        <v>public void button21(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 1) return; else { game1[2][1] = currentPlayer; currentGame=4; button21.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button21.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button21.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+        <f t="shared" ref="K23:K30" si="13">"public void button"&amp;A13&amp;"(View view) { if (currentGame == 0) currentGame = "&amp;A3&amp;"; if (currentGame != "&amp;A3&amp;") return; else { game"&amp;A3&amp;"["&amp;LEFT(A23,1)&amp;"]["&amp;RIGHT(A23,1)&amp;"] = currentPlayer; currentGame="&amp;A33&amp;"; button"&amp;A13&amp;".setEnabled(false); activeGame"&amp;A33&amp;"(); if (currentPlayer == 1) { button"&amp;A13&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); checkGame"&amp;A3&amp;"Win(); currentPlayer = 2; } else { button"&amp;A13&amp;".setText("&amp;CHAR(34)&amp;"O"&amp;CHAR(34)&amp;"); checkGame"&amp;A3&amp;"Win(); currentPlayer = 1; } } }"</f>
+        <v>public void button21(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[2][1] = currentPlayer; currentGame=4; button21.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button21.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button21.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="12"/>
-        <v>public void button22(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 1) return; else { game1[2][2] = currentPlayer; currentGame=5; button22.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button22.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button22.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+        <v>public void button22(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[2][2] = currentPlayer; currentGame=5; button22.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button22.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button22.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="12"/>
-        <v>public void button23(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 1) return; else { game1[2][3] = currentPlayer; currentGame=6; button23.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button23.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button23.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+        <v>public void button23(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[2][3] = currentPlayer; currentGame=6; button23.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button23.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button23.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="12"/>
-        <v>public void button24(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 2) return; else { game2[2][1] = currentPlayer; currentGame=4; button24.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button24.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button24.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+        <v>public void button24(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[2][1] = currentPlayer; currentGame=4; button24.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button24.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button24.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="12"/>
-        <v>public void button25(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 2) return; else { game2[2][2] = currentPlayer; currentGame=5; button25.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button25.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button25.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+        <v>public void button25(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[2][2] = currentPlayer; currentGame=5; button25.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button25.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button25.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="P23" t="str">
         <f t="shared" si="12"/>
-        <v>public void button26(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 2) return; else { game2[2][3] = currentPlayer; currentGame=6; button26.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button26.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button26.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+        <v>public void button26(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[2][3] = currentPlayer; currentGame=6; button26.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button26.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button26.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="12"/>
-        <v>public void button27(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 3) return; else { game3[2][1] = currentPlayer; currentGame=4; button27.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button27.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button27.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+        <v>public void button27(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[2][1] = currentPlayer; currentGame=4; button27.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button27.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button27.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R23" t="str">
         <f t="shared" si="12"/>
-        <v>public void button28(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 3) return; else { game3[2][2] = currentPlayer; currentGame=5; button28.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button28.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button28.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+        <v>public void button28(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[2][2] = currentPlayer; currentGame=5; button28.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button28.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button28.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" si="12"/>
-        <v>public void button29(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 3) return; else { game3[2][3] = currentPlayer; currentGame=6; button29.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button29.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button29.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+        <v>public void button29(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[2][3] = currentPlayer; currentGame=6; button29.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button29.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button29.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -5046,39 +5370,39 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="13"/>
-        <v>public void button31(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 1) return; else { game1[3][1] = currentPlayer; currentGame=7; button31.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button31.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button31.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+        <v>public void button31(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[3][1] = currentPlayer; currentGame=7; button31.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button31.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button31.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="12"/>
-        <v>public void button32(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 1) return; else { game1[3][2] = currentPlayer; currentGame=8; button32.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button32.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button32.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+        <v>public void button32(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[3][2] = currentPlayer; currentGame=8; button32.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button32.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button32.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="12"/>
-        <v>public void button33(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 1) return; else { game1[3][3] = currentPlayer; currentGame=9; button33.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button33.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button33.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
+        <v>public void button33(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 1) return; else { game1[3][3] = currentPlayer; currentGame=9; button33.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button33.setText("X"); checkGame1Win(); currentPlayer = 2; } else { button33.setText("O"); checkGame1Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="12"/>
-        <v>public void button34(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 2) return; else { game2[3][1] = currentPlayer; currentGame=7; button34.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button34.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button34.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+        <v>public void button34(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[3][1] = currentPlayer; currentGame=7; button34.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button34.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button34.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="12"/>
-        <v>public void button35(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 2) return; else { game2[3][2] = currentPlayer; currentGame=8; button35.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button35.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button35.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+        <v>public void button35(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[3][2] = currentPlayer; currentGame=8; button35.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button35.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button35.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="P24" t="str">
         <f t="shared" si="12"/>
-        <v>public void button36(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 2) return; else { game2[3][3] = currentPlayer; currentGame=9; button36.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button36.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button36.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
+        <v>public void button36(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 2) return; else { game2[3][3] = currentPlayer; currentGame=9; button36.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button36.setText("X"); checkGame2Win(); currentPlayer = 2; } else { button36.setText("O"); checkGame2Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="12"/>
-        <v>public void button37(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 3) return; else { game3[3][1] = currentPlayer; currentGame=7; button37.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button37.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button37.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+        <v>public void button37(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[3][1] = currentPlayer; currentGame=7; button37.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button37.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button37.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R24" t="str">
         <f t="shared" si="12"/>
-        <v>public void button38(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 3) return; else { game3[3][2] = currentPlayer; currentGame=8; button38.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button38.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button38.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+        <v>public void button38(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[3][2] = currentPlayer; currentGame=8; button38.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button38.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button38.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" si="12"/>
-        <v>public void button39(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 3) return; else { game3[3][3] = currentPlayer; currentGame=9; button39.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button39.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button39.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
+        <v>public void button39(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 3) return; else { game3[3][3] = currentPlayer; currentGame=9; button39.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button39.setText("X"); checkGame3Win(); currentPlayer = 2; } else { button39.setText("O"); checkGame3Win(); currentPlayer = 1; } } }</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -5111,39 +5435,39 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="13"/>
-        <v>public void button41(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 4) return; else { game4[1][1] = currentPlayer; currentGame=1; button41.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button41.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button41.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+        <v>public void button41(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[1][1] = currentPlayer; currentGame=1; button41.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button41.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button41.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="12"/>
-        <v>public void button42(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 4) return; else { game4[1][2] = currentPlayer; currentGame=2; button42.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button42.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button42.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+        <v>public void button42(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[1][2] = currentPlayer; currentGame=2; button42.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button42.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button42.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="12"/>
-        <v>public void button43(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 4) return; else { game4[1][3] = currentPlayer; currentGame=3; button43.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button43.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button43.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+        <v>public void button43(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[1][3] = currentPlayer; currentGame=3; button43.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button43.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button43.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="12"/>
-        <v>public void button44(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 5) return; else { game5[1][1] = currentPlayer; currentGame=1; button44.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button44.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button44.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+        <v>public void button44(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[1][1] = currentPlayer; currentGame=1; button44.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button44.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button44.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="12"/>
-        <v>public void button45(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 5) return; else { game5[1][2] = currentPlayer; currentGame=2; button45.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button45.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button45.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+        <v>public void button45(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[1][2] = currentPlayer; currentGame=2; button45.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button45.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button45.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="P25" t="str">
         <f t="shared" si="12"/>
-        <v>public void button46(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 5) return; else { game5[1][3] = currentPlayer; currentGame=3; button46.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button46.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button46.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+        <v>public void button46(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[1][3] = currentPlayer; currentGame=3; button46.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button46.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button46.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="12"/>
-        <v>public void button47(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 6) return; else { game6[1][1] = currentPlayer; currentGame=1; button47.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button47.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button47.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+        <v>public void button47(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[1][1] = currentPlayer; currentGame=1; button47.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button47.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button47.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R25" t="str">
         <f t="shared" si="12"/>
-        <v>public void button48(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 6) return; else { game6[1][2] = currentPlayer; currentGame=2; button48.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button48.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button48.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+        <v>public void button48(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[1][2] = currentPlayer; currentGame=2; button48.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button48.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button48.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S25" t="str">
         <f t="shared" si="12"/>
-        <v>public void button49(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 6) return; else { game6[1][3] = currentPlayer; currentGame=3; button49.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button49.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button49.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+        <v>public void button49(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[1][3] = currentPlayer; currentGame=3; button49.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button49.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button49.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -5180,15 +5504,15 @@
       </c>
       <c r="L26" t="str">
         <f t="shared" si="12"/>
-        <v>public void button52(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 4) return; else { game4[2][2] = currentPlayer; currentGame=5; button52.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button52.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button52.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+        <v>public void button52(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[2][2] = currentPlayer; currentGame=5; button52.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button52.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button52.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="12"/>
-        <v>public void button53(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 4) return; else { game4[2][3] = currentPlayer; currentGame=6; button53.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button53.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button53.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+        <v>public void button53(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[2][3] = currentPlayer; currentGame=6; button53.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button53.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button53.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="12"/>
-        <v>public void button54(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 5) return; else { game5[2][1] = currentPlayer; currentGame=4; button54.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button54.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button54.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+        <v>public void button54(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[2][1] = currentPlayer; currentGame=4; button54.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button54.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button54.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="12"/>
@@ -5196,15 +5520,15 @@
       </c>
       <c r="P26" t="str">
         <f t="shared" si="12"/>
-        <v>public void button56(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 5) return; else { game5[2][3] = currentPlayer; currentGame=6; button56.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button56.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button56.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+        <v>public void button56(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[2][3] = currentPlayer; currentGame=6; button56.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button56.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button56.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="12"/>
-        <v>public void button57(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 6) return; else { game6[2][1] = currentPlayer; currentGame=4; button57.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button57.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button57.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+        <v>public void button57(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[2][1] = currentPlayer; currentGame=4; button57.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button57.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button57.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R26" t="str">
         <f t="shared" si="12"/>
-        <v>public void button58(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 6) return; else { game6[2][2] = currentPlayer; currentGame=5; button58.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button58.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button58.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+        <v>public void button58(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[2][2] = currentPlayer; currentGame=5; button58.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button58.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button58.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S26" t="str">
         <f t="shared" si="12"/>
@@ -5241,39 +5565,39 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="13"/>
-        <v>public void button61(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 4) return; else { game4[3][1] = currentPlayer; currentGame=7; button61.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button61.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button61.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+        <v>public void button61(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[3][1] = currentPlayer; currentGame=7; button61.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button61.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button61.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="12"/>
-        <v>public void button62(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 4) return; else { game4[3][2] = currentPlayer; currentGame=8; button62.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button62.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button62.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+        <v>public void button62(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[3][2] = currentPlayer; currentGame=8; button62.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button62.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button62.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="12"/>
-        <v>public void button63(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 4) return; else { game4[3][3] = currentPlayer; currentGame=9; button63.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button63.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button63.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
+        <v>public void button63(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 4) return; else { game4[3][3] = currentPlayer; currentGame=9; button63.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button63.setText("X"); checkGame4Win(); currentPlayer = 2; } else { button63.setText("O"); checkGame4Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="12"/>
-        <v>public void button64(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 5) return; else { game5[3][1] = currentPlayer; currentGame=7; button64.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button64.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button64.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+        <v>public void button64(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[3][1] = currentPlayer; currentGame=7; button64.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button64.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button64.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="12"/>
-        <v>public void button65(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 5) return; else { game5[3][2] = currentPlayer; currentGame=8; button65.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button65.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button65.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+        <v>public void button65(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[3][2] = currentPlayer; currentGame=8; button65.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button65.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button65.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="P27" t="str">
         <f t="shared" si="12"/>
-        <v>public void button66(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 5) return; else { game5[3][3] = currentPlayer; currentGame=9; button66.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button66.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button66.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
+        <v>public void button66(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 5) return; else { game5[3][3] = currentPlayer; currentGame=9; button66.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button66.setText("X"); checkGame5Win(); currentPlayer = 2; } else { button66.setText("O"); checkGame5Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="12"/>
-        <v>public void button67(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 6) return; else { game6[3][1] = currentPlayer; currentGame=7; button67.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button67.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button67.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+        <v>public void button67(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[3][1] = currentPlayer; currentGame=7; button67.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button67.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button67.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R27" t="str">
         <f t="shared" si="12"/>
-        <v>public void button68(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 6) return; else { game6[3][2] = currentPlayer; currentGame=8; button68.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button68.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button68.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+        <v>public void button68(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[3][2] = currentPlayer; currentGame=8; button68.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button68.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button68.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S27" t="str">
         <f t="shared" si="12"/>
-        <v>public void button69(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 6) return; else { game6[3][3] = currentPlayer; currentGame=9; button69.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button69.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button69.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
+        <v>public void button69(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 6) return; else { game6[3][3] = currentPlayer; currentGame=9; button69.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button69.setText("X"); checkGame6Win(); currentPlayer = 2; } else { button69.setText("O"); checkGame6Win(); currentPlayer = 1; } } }</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -5306,39 +5630,39 @@
       </c>
       <c r="K28" t="str">
         <f t="shared" si="13"/>
-        <v>public void button71(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 7) return; else { game7[1][1] = currentPlayer; currentGame=1; button71.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button71.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button71.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+        <v>public void button71(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[1][1] = currentPlayer; currentGame=1; button71.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button71.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button71.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="12"/>
-        <v>public void button72(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 7) return; else { game7[1][2] = currentPlayer; currentGame=2; button72.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button72.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button72.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+        <v>public void button72(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[1][2] = currentPlayer; currentGame=2; button72.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button72.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button72.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="12"/>
-        <v>public void button73(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 7) return; else { game7[1][3] = currentPlayer; currentGame=3; button73.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button73.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button73.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+        <v>public void button73(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[1][3] = currentPlayer; currentGame=3; button73.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button73.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button73.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="12"/>
-        <v>public void button74(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 8) return; else { game8[1][1] = currentPlayer; currentGame=1; button74.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button74.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button74.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+        <v>public void button74(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[1][1] = currentPlayer; currentGame=1; button74.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button74.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button74.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="12"/>
-        <v>public void button75(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 8) return; else { game8[1][2] = currentPlayer; currentGame=2; button75.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button75.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button75.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+        <v>public void button75(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[1][2] = currentPlayer; currentGame=2; button75.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button75.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button75.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="P28" t="str">
         <f t="shared" si="12"/>
-        <v>public void button76(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 8) return; else { game8[1][3] = currentPlayer; currentGame=3; button76.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button76.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button76.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+        <v>public void button76(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[1][3] = currentPlayer; currentGame=3; button76.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button76.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button76.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="12"/>
-        <v>public void button77(View view) { if (currentGame == 0) currentGame = 1; if (currentGame != 9) return; else { game9[1][1] = currentPlayer; currentGame=1; button77.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button77.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button77.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+        <v>public void button77(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[1][1] = currentPlayer; currentGame=1; button77.setEnabled(false); activeGame1(); if (currentPlayer == 1) { button77.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button77.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R28" t="str">
         <f t="shared" si="12"/>
-        <v>public void button78(View view) { if (currentGame == 0) currentGame = 2; if (currentGame != 9) return; else { game9[1][2] = currentPlayer; currentGame=2; button78.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button78.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button78.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+        <v>public void button78(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[1][2] = currentPlayer; currentGame=2; button78.setEnabled(false); activeGame2(); if (currentPlayer == 1) { button78.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button78.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S28" t="str">
         <f t="shared" si="12"/>
-        <v>public void button79(View view) { if (currentGame == 0) currentGame = 3; if (currentGame != 9) return; else { game9[1][3] = currentPlayer; currentGame=3; button79.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button79.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button79.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+        <v>public void button79(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[1][3] = currentPlayer; currentGame=3; button79.setEnabled(false); activeGame3(); if (currentPlayer == 1) { button79.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button79.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -5371,39 +5695,39 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="13"/>
-        <v>public void button81(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 7) return; else { game7[2][1] = currentPlayer; currentGame=4; button81.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button81.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button81.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+        <v>public void button81(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[2][1] = currentPlayer; currentGame=4; button81.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button81.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button81.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="12"/>
-        <v>public void button82(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 7) return; else { game7[2][2] = currentPlayer; currentGame=5; button82.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button82.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button82.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+        <v>public void button82(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[2][2] = currentPlayer; currentGame=5; button82.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button82.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button82.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="12"/>
-        <v>public void button83(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 7) return; else { game7[2][3] = currentPlayer; currentGame=6; button83.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button83.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button83.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+        <v>public void button83(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[2][3] = currentPlayer; currentGame=6; button83.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button83.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button83.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="12"/>
-        <v>public void button84(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 8) return; else { game8[2][1] = currentPlayer; currentGame=4; button84.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button84.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button84.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+        <v>public void button84(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[2][1] = currentPlayer; currentGame=4; button84.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button84.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button84.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="12"/>
-        <v>public void button85(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 8) return; else { game8[2][2] = currentPlayer; currentGame=5; button85.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button85.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button85.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+        <v>public void button85(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[2][2] = currentPlayer; currentGame=5; button85.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button85.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button85.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="P29" t="str">
         <f t="shared" si="12"/>
-        <v>public void button86(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 8) return; else { game8[2][3] = currentPlayer; currentGame=6; button86.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button86.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button86.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+        <v>public void button86(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[2][3] = currentPlayer; currentGame=6; button86.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button86.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button86.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q29" t="str">
         <f t="shared" si="12"/>
-        <v>public void button87(View view) { if (currentGame == 0) currentGame = 4; if (currentGame != 9) return; else { game9[2][1] = currentPlayer; currentGame=4; button87.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button87.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button87.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+        <v>public void button87(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[2][1] = currentPlayer; currentGame=4; button87.setEnabled(false); activeGame4(); if (currentPlayer == 1) { button87.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button87.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R29" t="str">
         <f t="shared" si="12"/>
-        <v>public void button88(View view) { if (currentGame == 0) currentGame = 5; if (currentGame != 9) return; else { game9[2][2] = currentPlayer; currentGame=5; button88.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button88.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button88.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+        <v>public void button88(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[2][2] = currentPlayer; currentGame=5; button88.setEnabled(false); activeGame5(); if (currentPlayer == 1) { button88.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button88.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S29" t="str">
         <f t="shared" si="12"/>
-        <v>public void button89(View view) { if (currentGame == 0) currentGame = 6; if (currentGame != 9) return; else { game9[2][3] = currentPlayer; currentGame=6; button89.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button89.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button89.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+        <v>public void button89(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[2][3] = currentPlayer; currentGame=6; button89.setEnabled(false); activeGame6(); if (currentPlayer == 1) { button89.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button89.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -5440,15 +5764,15 @@
       </c>
       <c r="L30" t="str">
         <f t="shared" si="12"/>
-        <v>public void button92(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 7) return; else { game7[3][2] = currentPlayer; currentGame=8; button92.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button92.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button92.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+        <v>public void button92(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[3][2] = currentPlayer; currentGame=8; button92.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button92.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button92.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="12"/>
-        <v>public void button93(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 7) return; else { game7[3][3] = currentPlayer; currentGame=9; button93.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button93.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button93.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
+        <v>public void button93(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 7) return; else { game7[3][3] = currentPlayer; currentGame=9; button93.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button93.setText("X"); checkGame7Win(); currentPlayer = 2; } else { button93.setText("O"); checkGame7Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="12"/>
-        <v>public void button94(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 8) return; else { game8[3][1] = currentPlayer; currentGame=7; button94.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button94.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button94.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+        <v>public void button94(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[3][1] = currentPlayer; currentGame=7; button94.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button94.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button94.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" si="12"/>
@@ -5456,15 +5780,15 @@
       </c>
       <c r="P30" t="str">
         <f t="shared" si="12"/>
-        <v>public void button96(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 8) return; else { game8[3][3] = currentPlayer; currentGame=9; button96.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button96.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button96.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
+        <v>public void button96(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 8) return; else { game8[3][3] = currentPlayer; currentGame=9; button96.setEnabled(false); activeGame9(); if (currentPlayer == 1) { button96.setText("X"); checkGame8Win(); currentPlayer = 2; } else { button96.setText("O"); checkGame8Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" si="12"/>
-        <v>public void button97(View view) { if (currentGame == 0) currentGame = 7; if (currentGame != 9) return; else { game9[3][1] = currentPlayer; currentGame=7; button97.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button97.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button97.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+        <v>public void button97(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[3][1] = currentPlayer; currentGame=7; button97.setEnabled(false); activeGame7(); if (currentPlayer == 1) { button97.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button97.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="R30" t="str">
         <f t="shared" si="12"/>
-        <v>public void button98(View view) { if (currentGame == 0) currentGame = 8; if (currentGame != 9) return; else { game9[3][2] = currentPlayer; currentGame=8; button98.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button98.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button98.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
+        <v>public void button98(View view) { if (currentGame == 0) currentGame = 9; if (currentGame != 9) return; else { game9[3][2] = currentPlayer; currentGame=8; button98.setEnabled(false); activeGame8(); if (currentPlayer == 1) { button98.setText("X"); checkGame9Win(); currentPlayer = 2; } else { button98.setText("O"); checkGame9Win(); currentPlayer = 1; } } }</v>
       </c>
       <c r="S30" t="str">
         <f t="shared" si="12"/>

</xml_diff>

<commit_message>
Add game win mechanism and highlighting
</commit_message>
<xml_diff>
--- a/_DESIGN/Book4b.xlsx
+++ b/_DESIGN/Book4b.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uibc\Desktop\SuperTicTacToe\_DESIGN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TREE\Google Drive\_ANDROID\_PROJECTS\Super-Tic-Tac-Toe\_DESIGN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="165">
   <si>
     <t>button11</t>
   </si>
@@ -275,6 +275,252 @@
   </si>
   <si>
     <t>position</t>
+  </si>
+  <si>
+    <t>button11.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button12.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button13.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button14.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button15.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button16.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button17.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button18.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button19.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button21.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button22.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button23.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button24.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button25.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button26.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button27.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button28.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button29.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button31.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button32.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button33.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button34.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button35.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button36.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button37.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button38.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button39.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button41.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button42.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button43.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button44.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button45.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button46.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button47.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button48.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button49.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button51.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button52.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button53.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button54.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button55.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button56.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button57.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button58.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button59.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button61.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button62.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button63.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button64.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button65.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button66.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button67.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button68.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button69.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button71.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button72.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button73.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button74.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button75.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button76.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button77.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button78.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button79.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button81.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button82.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button83.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button84.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button85.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button86.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button87.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button88.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button89.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button91.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button92.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button93.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button94.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button95.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button96.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button97.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button98.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t>button99.getBackground().setColorFilter(new LightingColorFilter(0xff4CAF50, 0x000000));</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -345,7 +591,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -353,11 +599,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -373,6 +668,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4003,10 +4304,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="Q52" sqref="Q52:S60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6646,7 +6947,7 @@
         <v>button79.getBackground().setColorFilter(null);</v>
       </c>
     </row>
-    <row r="49" spans="11:19">
+    <row r="49" spans="11:20">
       <c r="K49" t="str">
         <f t="shared" si="17"/>
         <v>button81.getBackground().setColorFilter(null);</v>
@@ -6684,7 +6985,7 @@
         <v>button89.getBackground().setColorFilter(null);</v>
       </c>
     </row>
-    <row r="50" spans="11:19">
+    <row r="50" spans="11:20">
       <c r="K50" t="str">
         <f t="shared" si="17"/>
         <v>button91.getBackground().setColorFilter(null);</v>
@@ -6720,6 +7021,294 @@
       <c r="S50" t="str">
         <f t="shared" si="16"/>
         <v>button99.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="52" spans="11:20">
+      <c r="K52" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="N52" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="O52" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="P52" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q52" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="R52" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="S52" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="T52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="11:20">
+      <c r="K53" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="L53" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="M53" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="N53" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="O53" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="P53" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q53" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="R53" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="S53" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="T53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="11:20">
+      <c r="K54" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L54" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="M54" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="N54" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="O54" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="P54" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q54" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="R54" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="S54" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="T54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="11:20">
+      <c r="K55" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="L55" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="M55" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N55" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="O55" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="P55" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q55" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="R55" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="S55" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="T55" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="11:20">
+      <c r="K56" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L56" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="M56" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="N56" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="O56" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="P56" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q56" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="R56" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="S56" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="T56" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="11:20">
+      <c r="K57" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="L57" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="M57" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="N57" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="O57" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="P57" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q57" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="R57" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="S57" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="T57" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="11:20">
+      <c r="K58" t="s">
+        <v>137</v>
+      </c>
+      <c r="L58" t="s">
+        <v>138</v>
+      </c>
+      <c r="M58" t="s">
+        <v>139</v>
+      </c>
+      <c r="N58" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="O58" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="P58" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>143</v>
+      </c>
+      <c r="R58" t="s">
+        <v>144</v>
+      </c>
+      <c r="S58" t="s">
+        <v>145</v>
+      </c>
+      <c r="T58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="11:20">
+      <c r="K59" t="s">
+        <v>146</v>
+      </c>
+      <c r="L59" t="s">
+        <v>147</v>
+      </c>
+      <c r="M59" t="s">
+        <v>148</v>
+      </c>
+      <c r="N59" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="O59" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="P59" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>152</v>
+      </c>
+      <c r="R59" t="s">
+        <v>153</v>
+      </c>
+      <c r="S59" t="s">
+        <v>154</v>
+      </c>
+      <c r="T59" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="11:20">
+      <c r="K60" t="s">
+        <v>155</v>
+      </c>
+      <c r="L60" t="s">
+        <v>156</v>
+      </c>
+      <c r="M60" t="s">
+        <v>157</v>
+      </c>
+      <c r="N60" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="O60" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="P60" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>161</v>
+      </c>
+      <c r="R60" t="s">
+        <v>162</v>
+      </c>
+      <c r="S60" t="s">
+        <v>163</v>
+      </c>
+      <c r="T60" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add draw detection for main Game
</commit_message>
<xml_diff>
--- a/_DESIGN/Book4b.xlsx
+++ b/_DESIGN/Book4b.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="246">
   <si>
     <t>button11</t>
   </si>
@@ -521,6 +521,249 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>button11.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button12.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button13.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button14.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button15.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button16.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button17.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button18.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button19.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button21.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button22.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button23.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button24.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button25.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button26.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button27.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button28.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button29.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button31.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button32.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button33.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button34.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button35.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button36.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button37.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button38.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button39.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button41.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button42.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button43.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button44.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button45.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button46.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button47.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button48.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button49.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button51.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button52.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button53.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button54.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button55.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button56.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button57.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button58.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button59.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button61.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button62.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button63.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button64.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button65.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button66.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button67.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button68.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button69.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button71.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button72.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button73.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button74.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button75.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button76.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button77.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button78.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button79.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button81.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button82.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button83.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button84.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button85.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button86.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button87.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button88.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button89.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button91.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button92.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button93.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button94.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button95.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button96.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button97.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button98.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
+  </si>
+  <si>
+    <t>button99.getBackground().setColorFilter(new LightingColorFilter(0xff00BCD4, 0x000000));</t>
   </si>
 </sst>
 </file>
@@ -665,15 +908,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4304,10 +4547,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:T70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52:S60"/>
+      <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4316,17 +4559,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2">
@@ -4914,17 +5157,17 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12">
@@ -7024,31 +7267,31 @@
       </c>
     </row>
     <row r="52" spans="11:20">
-      <c r="K52" s="11" t="s">
+      <c r="K52" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="L52" s="11" t="s">
+      <c r="L52" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="M52" s="11" t="s">
+      <c r="M52" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="N52" s="13" t="s">
+      <c r="N52" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="O52" s="11" t="s">
+      <c r="O52" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="P52" s="15" t="s">
+      <c r="P52" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Q52" s="11" t="s">
+      <c r="Q52" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="R52" s="11" t="s">
+      <c r="R52" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="S52" s="11" t="s">
+      <c r="S52" s="10" t="s">
         <v>91</v>
       </c>
       <c r="T52" t="s">
@@ -7056,31 +7299,31 @@
       </c>
     </row>
     <row r="53" spans="11:20">
-      <c r="K53" s="11" t="s">
+      <c r="K53" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="L53" s="11" t="s">
+      <c r="L53" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="M53" s="11" t="s">
+      <c r="M53" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="N53" s="13" t="s">
+      <c r="N53" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="O53" s="11" t="s">
+      <c r="O53" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="P53" s="15" t="s">
+      <c r="P53" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="Q53" s="11" t="s">
+      <c r="Q53" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="R53" s="11" t="s">
+      <c r="R53" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="S53" s="11" t="s">
+      <c r="S53" s="10" t="s">
         <v>100</v>
       </c>
       <c r="T53" t="s">
@@ -7088,31 +7331,31 @@
       </c>
     </row>
     <row r="54" spans="11:20">
-      <c r="K54" s="12" t="s">
+      <c r="K54" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="L54" s="12" t="s">
+      <c r="L54" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="M54" s="12" t="s">
+      <c r="M54" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="N54" s="14" t="s">
+      <c r="N54" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="O54" s="12" t="s">
+      <c r="O54" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="P54" s="16" t="s">
+      <c r="P54" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="Q54" s="12" t="s">
+      <c r="Q54" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="R54" s="12" t="s">
+      <c r="R54" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="S54" s="12" t="s">
+      <c r="S54" s="11" t="s">
         <v>109</v>
       </c>
       <c r="T54" t="s">
@@ -7120,98 +7363,98 @@
       </c>
     </row>
     <row r="55" spans="11:20">
-      <c r="K55" s="11" t="s">
+      <c r="K55" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="L55" s="11" t="s">
+      <c r="L55" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="M55" s="11" t="s">
+      <c r="M55" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="N55" s="13" t="s">
+      <c r="N55" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="O55" s="11" t="s">
+      <c r="O55" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="P55" s="15" t="s">
+      <c r="P55" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="Q55" s="11" t="s">
+      <c r="Q55" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="R55" s="11" t="s">
+      <c r="R55" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="S55" s="11" t="s">
+      <c r="S55" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="T55" s="11" t="s">
+      <c r="T55" s="10" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="56" spans="11:20">
-      <c r="K56" s="11" t="s">
+      <c r="K56" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="L56" s="11" t="s">
+      <c r="L56" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="M56" s="11" t="s">
+      <c r="M56" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="N56" s="13" t="s">
+      <c r="N56" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="O56" s="11" t="s">
+      <c r="O56" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="P56" s="15" t="s">
+      <c r="P56" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="Q56" s="11" t="s">
+      <c r="Q56" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="R56" s="11" t="s">
+      <c r="R56" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="S56" s="11" t="s">
+      <c r="S56" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="T56" s="11" t="s">
+      <c r="T56" s="10" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="57" spans="11:20">
-      <c r="K57" s="12" t="s">
+      <c r="K57" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="L57" s="12" t="s">
+      <c r="L57" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="M57" s="12" t="s">
+      <c r="M57" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="N57" s="14" t="s">
+      <c r="N57" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="O57" s="12" t="s">
+      <c r="O57" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="P57" s="16" t="s">
+      <c r="P57" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="Q57" s="12" t="s">
+      <c r="Q57" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="R57" s="12" t="s">
+      <c r="R57" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="S57" s="12" t="s">
+      <c r="S57" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="T57" s="11" t="s">
+      <c r="T57" s="10" t="s">
         <v>164</v>
       </c>
     </row>
@@ -7225,13 +7468,13 @@
       <c r="M58" t="s">
         <v>139</v>
       </c>
-      <c r="N58" s="13" t="s">
+      <c r="N58" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="O58" s="11" t="s">
+      <c r="O58" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="P58" s="15" t="s">
+      <c r="P58" s="14" t="s">
         <v>142</v>
       </c>
       <c r="Q58" t="s">
@@ -7257,13 +7500,13 @@
       <c r="M59" t="s">
         <v>148</v>
       </c>
-      <c r="N59" s="13" t="s">
+      <c r="N59" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="O59" s="11" t="s">
+      <c r="O59" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="P59" s="15" t="s">
+      <c r="P59" s="14" t="s">
         <v>151</v>
       </c>
       <c r="Q59" t="s">
@@ -7289,13 +7532,13 @@
       <c r="M60" t="s">
         <v>157</v>
       </c>
-      <c r="N60" s="13" t="s">
+      <c r="N60" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="O60" s="11" t="s">
+      <c r="O60" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="P60" s="15" t="s">
+      <c r="P60" s="14" t="s">
         <v>160</v>
       </c>
       <c r="Q60" t="s">
@@ -7308,6 +7551,294 @@
         <v>163</v>
       </c>
       <c r="T60" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="11:20">
+      <c r="K62" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="L62" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="M62" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="N62" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="O62" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="P62" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q62" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="R62" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="S62" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="T62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="11:20">
+      <c r="K63" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="L63" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="M63" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="N63" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="O63" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="P63" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q63" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="R63" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="S63" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="T63" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="64" spans="11:20">
+      <c r="K64" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L64" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="M64" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="N64" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O64" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="P64" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q64" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="R64" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="S64" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="T64" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="11:20">
+      <c r="K65" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="L65" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="M65" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="N65" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="O65" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="P65" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q65" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="R65" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="S65" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="T65" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="11:20">
+      <c r="K66" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="L66" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M66" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="N66" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="O66" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="P66" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q66" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="R66" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="S66" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="T66" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="11:20">
+      <c r="K67" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="L67" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="M67" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="N67" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="O67" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="P67" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q67" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="R67" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="S67" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="T67" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="11:20">
+      <c r="K68" t="s">
+        <v>219</v>
+      </c>
+      <c r="L68" t="s">
+        <v>220</v>
+      </c>
+      <c r="M68" t="s">
+        <v>221</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="O68" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="P68" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>225</v>
+      </c>
+      <c r="R68" t="s">
+        <v>226</v>
+      </c>
+      <c r="S68" t="s">
+        <v>227</v>
+      </c>
+      <c r="T68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="11:20">
+      <c r="K69" t="s">
+        <v>228</v>
+      </c>
+      <c r="L69" t="s">
+        <v>229</v>
+      </c>
+      <c r="M69" t="s">
+        <v>230</v>
+      </c>
+      <c r="N69" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="O69" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="P69" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>234</v>
+      </c>
+      <c r="R69" t="s">
+        <v>235</v>
+      </c>
+      <c r="S69" t="s">
+        <v>236</v>
+      </c>
+      <c r="T69" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="11:20">
+      <c r="K70" t="s">
+        <v>237</v>
+      </c>
+      <c r="L70" t="s">
+        <v>238</v>
+      </c>
+      <c r="M70" t="s">
+        <v>239</v>
+      </c>
+      <c r="N70" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="O70" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="P70" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>243</v>
+      </c>
+      <c r="R70" t="s">
+        <v>244</v>
+      </c>
+      <c r="S70" t="s">
+        <v>245</v>
+      </c>
+      <c r="T70" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify Excel colours for Medium article
</commit_message>
<xml_diff>
--- a/_DESIGN/Book4b.xlsx
+++ b/_DESIGN/Book4b.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -784,7 +784,7 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -794,12 +794,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -895,16 +889,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -932,6 +925,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C66B89F-100F-4DF3-869A-6E12098422CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4381500"/>
+          <a:ext cx="7820025" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1233,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="A1:I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1275,35 +1334,35 @@
         <f>"button"&amp;A1</f>
         <v>button11</v>
       </c>
-      <c r="L1" s="2" t="str">
+      <c r="L1" s="4" t="str">
         <f t="shared" ref="L1:S1" si="0">"button"&amp;B1</f>
         <v>button12</v>
       </c>
-      <c r="M1" s="2" t="str">
+      <c r="M1" s="4" t="str">
         <f t="shared" si="0"/>
         <v>button13</v>
       </c>
-      <c r="N1" s="2" t="str">
+      <c r="N1" s="4" t="str">
         <f t="shared" si="0"/>
         <v>button14</v>
       </c>
-      <c r="O1" s="2" t="str">
+      <c r="O1" s="4" t="str">
         <f t="shared" si="0"/>
         <v>button15</v>
       </c>
-      <c r="P1" s="2" t="str">
+      <c r="P1" s="4" t="str">
         <f t="shared" si="0"/>
         <v>button16</v>
       </c>
-      <c r="Q1" s="2" t="str">
+      <c r="Q1" s="4" t="str">
         <f t="shared" si="0"/>
         <v>button17</v>
       </c>
-      <c r="R1" s="2" t="str">
+      <c r="R1" s="4" t="str">
         <f t="shared" si="0"/>
         <v>button18</v>
       </c>
-      <c r="S1" s="1" t="str">
+      <c r="S1" s="6" t="str">
         <f t="shared" si="0"/>
         <v>button19</v>
       </c>
@@ -1336,39 +1395,39 @@
       <c r="I2">
         <v>29</v>
       </c>
-      <c r="K2" s="2" t="str">
+      <c r="K2" s="3" t="str">
         <f t="shared" ref="K2:K9" si="1">"button"&amp;A2</f>
         <v>button21</v>
       </c>
-      <c r="L2" t="str">
+      <c r="L2" s="5" t="str">
         <f t="shared" ref="L2:L9" si="2">"button"&amp;B2</f>
         <v>button22</v>
       </c>
-      <c r="M2" t="str">
+      <c r="M2" s="5" t="str">
         <f t="shared" ref="M2:M9" si="3">"button"&amp;C2</f>
         <v>button23</v>
       </c>
-      <c r="N2" t="str">
+      <c r="N2" s="5" t="str">
         <f t="shared" ref="N2:N9" si="4">"button"&amp;D2</f>
         <v>button24</v>
       </c>
-      <c r="O2" t="str">
+      <c r="O2" s="5" t="str">
         <f t="shared" ref="O2:O9" si="5">"button"&amp;E2</f>
         <v>button25</v>
       </c>
-      <c r="P2" t="str">
+      <c r="P2" s="5" t="str">
         <f t="shared" ref="P2:P9" si="6">"button"&amp;F2</f>
         <v>button26</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="Q2" s="5" t="str">
         <f t="shared" ref="Q2:Q9" si="7">"button"&amp;G2</f>
         <v>button27</v>
       </c>
-      <c r="R2" t="str">
+      <c r="R2" s="5" t="str">
         <f t="shared" ref="R2:R9" si="8">"button"&amp;H2</f>
         <v>button28</v>
       </c>
-      <c r="S2" s="2" t="str">
+      <c r="S2" s="7" t="str">
         <f t="shared" ref="S2:S9" si="9">"button"&amp;I2</f>
         <v>button29</v>
       </c>
@@ -1401,39 +1460,39 @@
       <c r="I3">
         <v>39</v>
       </c>
-      <c r="K3" s="2" t="str">
+      <c r="K3" s="3" t="str">
         <f t="shared" si="1"/>
         <v>button31</v>
       </c>
-      <c r="L3" t="str">
+      <c r="L3" s="5" t="str">
         <f t="shared" si="2"/>
         <v>button32</v>
       </c>
-      <c r="M3" t="str">
+      <c r="M3" s="5" t="str">
         <f t="shared" si="3"/>
         <v>button33</v>
       </c>
-      <c r="N3" t="str">
+      <c r="N3" s="5" t="str">
         <f t="shared" si="4"/>
         <v>button34</v>
       </c>
-      <c r="O3" t="str">
+      <c r="O3" s="5" t="str">
         <f t="shared" si="5"/>
         <v>button35</v>
       </c>
-      <c r="P3" t="str">
+      <c r="P3" s="5" t="str">
         <f t="shared" si="6"/>
         <v>button36</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="Q3" s="5" t="str">
         <f t="shared" si="7"/>
         <v>button37</v>
       </c>
-      <c r="R3" t="str">
+      <c r="R3" s="5" t="str">
         <f t="shared" si="8"/>
         <v>button38</v>
       </c>
-      <c r="S3" s="2" t="str">
+      <c r="S3" s="7" t="str">
         <f t="shared" si="9"/>
         <v>button39</v>
       </c>
@@ -1466,39 +1525,39 @@
       <c r="I4">
         <v>49</v>
       </c>
-      <c r="K4" s="2" t="str">
+      <c r="K4" s="3" t="str">
         <f t="shared" si="1"/>
         <v>button41</v>
       </c>
-      <c r="L4" t="str">
+      <c r="L4" s="5" t="str">
         <f t="shared" si="2"/>
         <v>button42</v>
       </c>
-      <c r="M4" t="str">
+      <c r="M4" s="5" t="str">
         <f t="shared" si="3"/>
         <v>button43</v>
       </c>
-      <c r="N4" t="str">
+      <c r="N4" s="5" t="str">
         <f t="shared" si="4"/>
         <v>button44</v>
       </c>
-      <c r="O4" t="str">
+      <c r="O4" s="5" t="str">
         <f t="shared" si="5"/>
         <v>button45</v>
       </c>
-      <c r="P4" t="str">
+      <c r="P4" s="5" t="str">
         <f t="shared" si="6"/>
         <v>button46</v>
       </c>
-      <c r="Q4" t="str">
+      <c r="Q4" s="5" t="str">
         <f t="shared" si="7"/>
         <v>button47</v>
       </c>
-      <c r="R4" t="str">
+      <c r="R4" s="5" t="str">
         <f t="shared" si="8"/>
         <v>button48</v>
       </c>
-      <c r="S4" s="2" t="str">
+      <c r="S4" s="7" t="str">
         <f t="shared" si="9"/>
         <v>button49</v>
       </c>
@@ -1531,39 +1590,39 @@
       <c r="I5">
         <v>59</v>
       </c>
-      <c r="K5" s="2" t="str">
+      <c r="K5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>button51</v>
       </c>
-      <c r="L5" t="str">
+      <c r="L5" s="5" t="str">
         <f t="shared" si="2"/>
         <v>button52</v>
       </c>
-      <c r="M5" t="str">
+      <c r="M5" s="5" t="str">
         <f t="shared" si="3"/>
         <v>button53</v>
       </c>
-      <c r="N5" t="str">
+      <c r="N5" s="5" t="str">
         <f t="shared" si="4"/>
         <v>button54</v>
       </c>
-      <c r="O5" t="str">
+      <c r="O5" s="5" t="str">
         <f t="shared" si="5"/>
         <v>button55</v>
       </c>
-      <c r="P5" t="str">
+      <c r="P5" s="5" t="str">
         <f t="shared" si="6"/>
         <v>button56</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="Q5" s="5" t="str">
         <f t="shared" si="7"/>
         <v>button57</v>
       </c>
-      <c r="R5" t="str">
+      <c r="R5" s="5" t="str">
         <f t="shared" si="8"/>
         <v>button58</v>
       </c>
-      <c r="S5" s="2" t="str">
+      <c r="S5" s="7" t="str">
         <f t="shared" si="9"/>
         <v>button59</v>
       </c>
@@ -1596,39 +1655,39 @@
       <c r="I6">
         <v>69</v>
       </c>
-      <c r="K6" s="2" t="str">
+      <c r="K6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>button61</v>
       </c>
-      <c r="L6" t="str">
+      <c r="L6" s="5" t="str">
         <f t="shared" si="2"/>
         <v>button62</v>
       </c>
-      <c r="M6" t="str">
+      <c r="M6" s="5" t="str">
         <f t="shared" si="3"/>
         <v>button63</v>
       </c>
-      <c r="N6" t="str">
+      <c r="N6" s="5" t="str">
         <f t="shared" si="4"/>
         <v>button64</v>
       </c>
-      <c r="O6" t="str">
+      <c r="O6" s="5" t="str">
         <f t="shared" si="5"/>
         <v>button65</v>
       </c>
-      <c r="P6" t="str">
+      <c r="P6" s="5" t="str">
         <f t="shared" si="6"/>
         <v>button66</v>
       </c>
-      <c r="Q6" t="str">
+      <c r="Q6" s="5" t="str">
         <f t="shared" si="7"/>
         <v>button67</v>
       </c>
-      <c r="R6" t="str">
+      <c r="R6" s="5" t="str">
         <f t="shared" si="8"/>
         <v>button68</v>
       </c>
-      <c r="S6" s="2" t="str">
+      <c r="S6" s="7" t="str">
         <f t="shared" si="9"/>
         <v>button69</v>
       </c>
@@ -1661,39 +1720,39 @@
       <c r="I7">
         <v>79</v>
       </c>
-      <c r="K7" s="2" t="str">
+      <c r="K7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>button71</v>
       </c>
-      <c r="L7" t="str">
+      <c r="L7" s="5" t="str">
         <f t="shared" si="2"/>
         <v>button72</v>
       </c>
-      <c r="M7" t="str">
+      <c r="M7" s="5" t="str">
         <f t="shared" si="3"/>
         <v>button73</v>
       </c>
-      <c r="N7" t="str">
+      <c r="N7" s="5" t="str">
         <f t="shared" si="4"/>
         <v>button74</v>
       </c>
-      <c r="O7" t="str">
+      <c r="O7" s="5" t="str">
         <f t="shared" si="5"/>
         <v>button75</v>
       </c>
-      <c r="P7" t="str">
+      <c r="P7" s="5" t="str">
         <f t="shared" si="6"/>
         <v>button76</v>
       </c>
-      <c r="Q7" t="str">
+      <c r="Q7" s="5" t="str">
         <f t="shared" si="7"/>
         <v>button77</v>
       </c>
-      <c r="R7" t="str">
+      <c r="R7" s="5" t="str">
         <f t="shared" si="8"/>
         <v>button78</v>
       </c>
-      <c r="S7" s="2" t="str">
+      <c r="S7" s="7" t="str">
         <f t="shared" si="9"/>
         <v>button79</v>
       </c>
@@ -1726,39 +1785,39 @@
       <c r="I8">
         <v>89</v>
       </c>
-      <c r="K8" s="2" t="str">
+      <c r="K8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>button81</v>
       </c>
-      <c r="L8" t="str">
+      <c r="L8" s="5" t="str">
         <f t="shared" si="2"/>
         <v>button82</v>
       </c>
-      <c r="M8" t="str">
+      <c r="M8" s="5" t="str">
         <f t="shared" si="3"/>
         <v>button83</v>
       </c>
-      <c r="N8" t="str">
+      <c r="N8" s="5" t="str">
         <f t="shared" si="4"/>
         <v>button84</v>
       </c>
-      <c r="O8" t="str">
+      <c r="O8" s="5" t="str">
         <f t="shared" si="5"/>
         <v>button85</v>
       </c>
-      <c r="P8" t="str">
+      <c r="P8" s="5" t="str">
         <f t="shared" si="6"/>
         <v>button86</v>
       </c>
-      <c r="Q8" t="str">
+      <c r="Q8" s="5" t="str">
         <f t="shared" si="7"/>
         <v>button87</v>
       </c>
-      <c r="R8" t="str">
+      <c r="R8" s="5" t="str">
         <f t="shared" si="8"/>
         <v>button88</v>
       </c>
-      <c r="S8" s="2" t="str">
+      <c r="S8" s="7" t="str">
         <f t="shared" si="9"/>
         <v>button89</v>
       </c>
@@ -1791,39 +1850,39 @@
       <c r="I9">
         <v>99</v>
       </c>
-      <c r="K9" s="2" t="str">
+      <c r="K9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>button91</v>
       </c>
-      <c r="L9" s="3" t="str">
+      <c r="L9" s="5" t="str">
         <f t="shared" si="2"/>
         <v>button92</v>
       </c>
-      <c r="M9" s="3" t="str">
+      <c r="M9" s="5" t="str">
         <f t="shared" si="3"/>
         <v>button93</v>
       </c>
-      <c r="N9" s="3" t="str">
+      <c r="N9" s="5" t="str">
         <f t="shared" si="4"/>
         <v>button94</v>
       </c>
-      <c r="O9" s="3" t="str">
+      <c r="O9" s="5" t="str">
         <f t="shared" si="5"/>
         <v>button95</v>
       </c>
-      <c r="P9" s="3" t="str">
+      <c r="P9" s="5" t="str">
         <f t="shared" si="6"/>
         <v>button96</v>
       </c>
-      <c r="Q9" s="3" t="str">
+      <c r="Q9" s="5" t="str">
         <f t="shared" si="7"/>
         <v>button97</v>
       </c>
-      <c r="R9" s="3" t="str">
+      <c r="R9" s="5" t="str">
         <f t="shared" si="8"/>
         <v>button98</v>
       </c>
-      <c r="S9" s="2" t="str">
+      <c r="S9" s="7" t="str">
         <f t="shared" si="9"/>
         <v>button99</v>
       </c>
@@ -1833,339 +1892,339 @@
         <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/button12"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button11" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button11" app:layout_constraintEnd_toStartOf="@id/button12" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
-      <c r="L11" s="5" t="str">
+      <c r="L11" s="4" t="str">
         <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;L1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M1&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button12" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button12" app:layout_constraintEnd_toStartOf="@id/button13" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button11" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
-      <c r="M11" s="5" t="str">
+      <c r="M11" s="4" t="str">
         <f t="shared" ref="M11:R11" si="10">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;M1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;M1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;N1&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;L1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button13" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button13" app:layout_constraintEnd_toStartOf="@id/button14" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button12" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
-      <c r="N11" s="5" t="str">
+      <c r="N11" s="4" t="str">
         <f t="shared" si="10"/>
         <v>&lt;Button android:id="@+id/button14" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button14" app:layout_constraintEnd_toStartOf="@id/button15" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button13" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
-      <c r="O11" s="5" t="str">
+      <c r="O11" s="4" t="str">
         <f t="shared" si="10"/>
         <v>&lt;Button android:id="@+id/button15" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button15" app:layout_constraintEnd_toStartOf="@id/button16" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button14" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
-      <c r="P11" s="5" t="str">
+      <c r="P11" s="4" t="str">
         <f t="shared" si="10"/>
         <v>&lt;Button android:id="@+id/button16" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button16" app:layout_constraintEnd_toStartOf="@id/button17" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button15" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
-      <c r="Q11" s="5" t="str">
+      <c r="Q11" s="4" t="str">
         <f t="shared" si="10"/>
         <v>&lt;Button android:id="@+id/button17" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button17" app:layout_constraintEnd_toStartOf="@id/button18" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button16" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
-      <c r="R11" s="5" t="str">
+      <c r="R11" s="4" t="str">
         <f t="shared" si="10"/>
         <v>&lt;Button android:id="@+id/button18" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button18" app:layout_constraintEnd_toStartOf="@id/button19" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button17" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
-      <c r="S11" s="7" t="str">
+      <c r="S11" s="6" t="str">
         <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S1&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;S1&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R1&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/imageView"&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button19" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button19" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button18" app:layout_constraintTop_toBottomOf="@id/imageView" /&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="K12" s="4" t="str">
+      <c r="K12" s="3" t="str">
         <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;K1&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button21" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button21" app:layout_constraintEnd_toStartOf="@id/button22" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button11" /&gt;</v>
       </c>
-      <c r="L12" s="6" t="str">
+      <c r="L12" s="5" t="str">
         <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L1&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button22" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button22" app:layout_constraintEnd_toStartOf="@id/button23" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button21" app:layout_constraintTop_toBottomOf="@id/button12" /&gt;</v>
       </c>
-      <c r="M12" s="6" t="str">
+      <c r="M12" s="5" t="str">
         <f t="shared" ref="M12:R12" si="11">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;M2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;M2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;N2&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;L2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;M1&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button23" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button23" app:layout_constraintEnd_toStartOf="@id/button24" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button22" app:layout_constraintTop_toBottomOf="@id/button13" /&gt;</v>
       </c>
-      <c r="N12" s="6" t="str">
+      <c r="N12" s="5" t="str">
         <f t="shared" si="11"/>
         <v>&lt;Button android:id="@+id/button24" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button24" app:layout_constraintEnd_toStartOf="@id/button25" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button23" app:layout_constraintTop_toBottomOf="@id/button14" /&gt;</v>
       </c>
-      <c r="O12" s="6" t="str">
+      <c r="O12" s="5" t="str">
         <f t="shared" si="11"/>
         <v>&lt;Button android:id="@+id/button25" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button25" app:layout_constraintEnd_toStartOf="@id/button26" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button24" app:layout_constraintTop_toBottomOf="@id/button15" /&gt;</v>
       </c>
-      <c r="P12" s="6" t="str">
+      <c r="P12" s="5" t="str">
         <f t="shared" si="11"/>
         <v>&lt;Button android:id="@+id/button26" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button26" app:layout_constraintEnd_toStartOf="@id/button27" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button25" app:layout_constraintTop_toBottomOf="@id/button16" /&gt;</v>
       </c>
-      <c r="Q12" s="6" t="str">
+      <c r="Q12" s="5" t="str">
         <f t="shared" si="11"/>
         <v>&lt;Button android:id="@+id/button27" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button27" app:layout_constraintEnd_toStartOf="@id/button28" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button26" app:layout_constraintTop_toBottomOf="@id/button17" /&gt;</v>
       </c>
-      <c r="R12" s="6" t="str">
+      <c r="R12" s="5" t="str">
         <f t="shared" si="11"/>
         <v>&lt;Button android:id="@+id/button28" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button28" app:layout_constraintEnd_toStartOf="@id/button29" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button27" app:layout_constraintTop_toBottomOf="@id/button18" /&gt;</v>
       </c>
-      <c r="S12" s="8" t="str">
+      <c r="S12" s="7" t="str">
         <f>"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S2&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;S2&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R2&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;S1&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button29" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button29" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button28" app:layout_constraintTop_toBottomOf="@id/button19" /&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="K13" s="4" t="str">
+      <c r="K13" s="3" t="str">
         <f t="shared" ref="K13:K19" si="12">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;K3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginLeft="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginStart="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;K3&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;L3&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toStartOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;K2&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button31" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button31" app:layout_constraintEnd_toStartOf="@id/button32" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button21" /&gt;</v>
       </c>
-      <c r="L13" s="6" t="str">
+      <c r="L13" s="5" t="str">
         <f t="shared" ref="L13:R19" si="13">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;L3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;L3&amp;CHAR(34)&amp;" app:layout_constraintEnd_toStartOf="&amp;CHAR(34)&amp;"@id/"&amp;M3&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@+id/"&amp;K3&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;L2&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button32" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button32" app:layout_constraintEnd_toStartOf="@id/button33" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button31" app:layout_constraintTop_toBottomOf="@id/button22" /&gt;</v>
       </c>
-      <c r="M13" s="6" t="str">
+      <c r="M13" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button33" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button33" app:layout_constraintEnd_toStartOf="@id/button34" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button32" app:layout_constraintTop_toBottomOf="@id/button23" /&gt;</v>
       </c>
-      <c r="N13" s="6" t="str">
+      <c r="N13" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button34" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button34" app:layout_constraintEnd_toStartOf="@id/button35" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button33" app:layout_constraintTop_toBottomOf="@id/button24" /&gt;</v>
       </c>
-      <c r="O13" s="6" t="str">
+      <c r="O13" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button35" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button35" app:layout_constraintEnd_toStartOf="@id/button36" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button34" app:layout_constraintTop_toBottomOf="@id/button25" /&gt;</v>
       </c>
-      <c r="P13" s="6" t="str">
+      <c r="P13" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button36" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button36" app:layout_constraintEnd_toStartOf="@id/button37" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button35" app:layout_constraintTop_toBottomOf="@id/button26" /&gt;</v>
       </c>
-      <c r="Q13" s="6" t="str">
+      <c r="Q13" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button37" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button37" app:layout_constraintEnd_toStartOf="@id/button38" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button36" app:layout_constraintTop_toBottomOf="@id/button27" /&gt;</v>
       </c>
-      <c r="R13" s="6" t="str">
+      <c r="R13" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button38" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button38" app:layout_constraintEnd_toStartOf="@id/button39" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button37" app:layout_constraintTop_toBottomOf="@id/button28" /&gt;</v>
       </c>
-      <c r="S13" s="8" t="str">
+      <c r="S13" s="7" t="str">
         <f t="shared" ref="S13:S19" si="14">"&lt;Button android:id="&amp;CHAR(34)&amp;"@+id/"&amp;S3&amp;CHAR(34)&amp;" android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;" android:layout_marginEnd="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:layout_marginRight="&amp;CHAR(34)&amp;"8dp"&amp;CHAR(34)&amp;" android:minWidth="&amp;CHAR(34)&amp;"40dp"&amp;CHAR(34)&amp;" android:onClick="&amp;CHAR(34)&amp;S3&amp;CHAR(34)&amp;" app:layout_constraintEnd_toEndOf="&amp;CHAR(34)&amp;"parent"&amp;CHAR(34)&amp;" app:layout_constraintHorizontal_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" app:layout_constraintStart_toEndOf="&amp;CHAR(34)&amp;"@id/"&amp;R3&amp;CHAR(34)&amp;" app:layout_constraintTop_toBottomOf="&amp;CHAR(34)&amp;"@id/"&amp;S2&amp;CHAR(34)&amp;" /&gt;"</f>
         <v>&lt;Button android:id="@+id/button39" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button39" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button38" app:layout_constraintTop_toBottomOf="@id/button29" /&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="K14" s="4" t="str">
+      <c r="K14" s="3" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button41" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button41" app:layout_constraintEnd_toStartOf="@id/button42" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button31" /&gt;</v>
       </c>
-      <c r="L14" s="6" t="str">
+      <c r="L14" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button42" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button42" app:layout_constraintEnd_toStartOf="@id/button43" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button41" app:layout_constraintTop_toBottomOf="@id/button32" /&gt;</v>
       </c>
-      <c r="M14" s="6" t="str">
+      <c r="M14" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button43" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button43" app:layout_constraintEnd_toStartOf="@id/button44" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button42" app:layout_constraintTop_toBottomOf="@id/button33" /&gt;</v>
       </c>
-      <c r="N14" s="6" t="str">
+      <c r="N14" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button44" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button44" app:layout_constraintEnd_toStartOf="@id/button45" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button43" app:layout_constraintTop_toBottomOf="@id/button34" /&gt;</v>
       </c>
-      <c r="O14" s="6" t="str">
+      <c r="O14" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button45" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button45" app:layout_constraintEnd_toStartOf="@id/button46" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button44" app:layout_constraintTop_toBottomOf="@id/button35" /&gt;</v>
       </c>
-      <c r="P14" s="6" t="str">
+      <c r="P14" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button46" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button46" app:layout_constraintEnd_toStartOf="@id/button47" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button45" app:layout_constraintTop_toBottomOf="@id/button36" /&gt;</v>
       </c>
-      <c r="Q14" s="6" t="str">
+      <c r="Q14" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button47" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button47" app:layout_constraintEnd_toStartOf="@id/button48" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button46" app:layout_constraintTop_toBottomOf="@id/button37" /&gt;</v>
       </c>
-      <c r="R14" s="6" t="str">
+      <c r="R14" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button48" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button48" app:layout_constraintEnd_toStartOf="@id/button49" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button47" app:layout_constraintTop_toBottomOf="@id/button38" /&gt;</v>
       </c>
-      <c r="S14" s="8" t="str">
+      <c r="S14" s="7" t="str">
         <f t="shared" si="14"/>
         <v>&lt;Button android:id="@+id/button49" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button49" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button48" app:layout_constraintTop_toBottomOf="@id/button39" /&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="K15" s="4" t="str">
+      <c r="K15" s="3" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button51" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button51" app:layout_constraintEnd_toStartOf="@id/button52" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button41" /&gt;</v>
       </c>
-      <c r="L15" s="6" t="str">
+      <c r="L15" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button52" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button52" app:layout_constraintEnd_toStartOf="@id/button53" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button51" app:layout_constraintTop_toBottomOf="@id/button42" /&gt;</v>
       </c>
-      <c r="M15" s="6" t="str">
+      <c r="M15" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button53" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button53" app:layout_constraintEnd_toStartOf="@id/button54" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button52" app:layout_constraintTop_toBottomOf="@id/button43" /&gt;</v>
       </c>
-      <c r="N15" s="6" t="str">
+      <c r="N15" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button54" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button54" app:layout_constraintEnd_toStartOf="@id/button55" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button53" app:layout_constraintTop_toBottomOf="@id/button44" /&gt;</v>
       </c>
-      <c r="O15" s="6" t="str">
+      <c r="O15" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button55" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button55" app:layout_constraintEnd_toStartOf="@id/button56" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button54" app:layout_constraintTop_toBottomOf="@id/button45" /&gt;</v>
       </c>
-      <c r="P15" s="6" t="str">
+      <c r="P15" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button56" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button56" app:layout_constraintEnd_toStartOf="@id/button57" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button55" app:layout_constraintTop_toBottomOf="@id/button46" /&gt;</v>
       </c>
-      <c r="Q15" s="6" t="str">
+      <c r="Q15" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button57" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button57" app:layout_constraintEnd_toStartOf="@id/button58" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button56" app:layout_constraintTop_toBottomOf="@id/button47" /&gt;</v>
       </c>
-      <c r="R15" s="6" t="str">
+      <c r="R15" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button58" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button58" app:layout_constraintEnd_toStartOf="@id/button59" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button57" app:layout_constraintTop_toBottomOf="@id/button48" /&gt;</v>
       </c>
-      <c r="S15" s="8" t="str">
+      <c r="S15" s="7" t="str">
         <f t="shared" si="14"/>
         <v>&lt;Button android:id="@+id/button59" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button59" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button58" app:layout_constraintTop_toBottomOf="@id/button49" /&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="K16" s="4" t="str">
+      <c r="K16" s="3" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button61" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button61" app:layout_constraintEnd_toStartOf="@id/button62" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button51" /&gt;</v>
       </c>
-      <c r="L16" s="6" t="str">
+      <c r="L16" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button62" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button62" app:layout_constraintEnd_toStartOf="@id/button63" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button61" app:layout_constraintTop_toBottomOf="@id/button52" /&gt;</v>
       </c>
-      <c r="M16" s="6" t="str">
+      <c r="M16" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button63" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button63" app:layout_constraintEnd_toStartOf="@id/button64" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button62" app:layout_constraintTop_toBottomOf="@id/button53" /&gt;</v>
       </c>
-      <c r="N16" s="6" t="str">
+      <c r="N16" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button64" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button64" app:layout_constraintEnd_toStartOf="@id/button65" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button63" app:layout_constraintTop_toBottomOf="@id/button54" /&gt;</v>
       </c>
-      <c r="O16" s="6" t="str">
+      <c r="O16" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button65" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button65" app:layout_constraintEnd_toStartOf="@id/button66" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button64" app:layout_constraintTop_toBottomOf="@id/button55" /&gt;</v>
       </c>
-      <c r="P16" s="6" t="str">
+      <c r="P16" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button66" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button66" app:layout_constraintEnd_toStartOf="@id/button67" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button65" app:layout_constraintTop_toBottomOf="@id/button56" /&gt;</v>
       </c>
-      <c r="Q16" s="6" t="str">
+      <c r="Q16" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button67" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button67" app:layout_constraintEnd_toStartOf="@id/button68" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button66" app:layout_constraintTop_toBottomOf="@id/button57" /&gt;</v>
       </c>
-      <c r="R16" s="6" t="str">
+      <c r="R16" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button68" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button68" app:layout_constraintEnd_toStartOf="@id/button69" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button67" app:layout_constraintTop_toBottomOf="@id/button58" /&gt;</v>
       </c>
-      <c r="S16" s="8" t="str">
+      <c r="S16" s="7" t="str">
         <f t="shared" si="14"/>
         <v>&lt;Button android:id="@+id/button69" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button69" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button68" app:layout_constraintTop_toBottomOf="@id/button59" /&gt;</v>
       </c>
     </row>
     <row r="17" spans="11:19">
-      <c r="K17" s="4" t="str">
+      <c r="K17" s="3" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button71" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button71" app:layout_constraintEnd_toStartOf="@id/button72" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button61" /&gt;</v>
       </c>
-      <c r="L17" s="6" t="str">
+      <c r="L17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button72" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button72" app:layout_constraintEnd_toStartOf="@id/button73" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button71" app:layout_constraintTop_toBottomOf="@id/button62" /&gt;</v>
       </c>
-      <c r="M17" s="6" t="str">
+      <c r="M17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button73" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button73" app:layout_constraintEnd_toStartOf="@id/button74" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button72" app:layout_constraintTop_toBottomOf="@id/button63" /&gt;</v>
       </c>
-      <c r="N17" s="6" t="str">
+      <c r="N17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button74" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button74" app:layout_constraintEnd_toStartOf="@id/button75" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button73" app:layout_constraintTop_toBottomOf="@id/button64" /&gt;</v>
       </c>
-      <c r="O17" s="6" t="str">
+      <c r="O17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button75" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button75" app:layout_constraintEnd_toStartOf="@id/button76" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button74" app:layout_constraintTop_toBottomOf="@id/button65" /&gt;</v>
       </c>
-      <c r="P17" s="6" t="str">
+      <c r="P17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button76" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button76" app:layout_constraintEnd_toStartOf="@id/button77" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button75" app:layout_constraintTop_toBottomOf="@id/button66" /&gt;</v>
       </c>
-      <c r="Q17" s="6" t="str">
+      <c r="Q17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button77" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button77" app:layout_constraintEnd_toStartOf="@id/button78" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button76" app:layout_constraintTop_toBottomOf="@id/button67" /&gt;</v>
       </c>
-      <c r="R17" s="6" t="str">
+      <c r="R17" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button78" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button78" app:layout_constraintEnd_toStartOf="@id/button79" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button77" app:layout_constraintTop_toBottomOf="@id/button68" /&gt;</v>
       </c>
-      <c r="S17" s="8" t="str">
+      <c r="S17" s="7" t="str">
         <f t="shared" si="14"/>
         <v>&lt;Button android:id="@+id/button79" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button79" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button78" app:layout_constraintTop_toBottomOf="@id/button69" /&gt;</v>
       </c>
     </row>
     <row r="18" spans="11:19">
-      <c r="K18" s="4" t="str">
+      <c r="K18" s="3" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button81" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button81" app:layout_constraintEnd_toStartOf="@id/button82" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button71" /&gt;</v>
       </c>
-      <c r="L18" s="6" t="str">
+      <c r="L18" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button82" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button82" app:layout_constraintEnd_toStartOf="@id/button83" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button81" app:layout_constraintTop_toBottomOf="@id/button72" /&gt;</v>
       </c>
-      <c r="M18" s="6" t="str">
+      <c r="M18" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button83" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button83" app:layout_constraintEnd_toStartOf="@id/button84" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button82" app:layout_constraintTop_toBottomOf="@id/button73" /&gt;</v>
       </c>
-      <c r="N18" s="6" t="str">
+      <c r="N18" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button84" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button84" app:layout_constraintEnd_toStartOf="@id/button85" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button83" app:layout_constraintTop_toBottomOf="@id/button74" /&gt;</v>
       </c>
-      <c r="O18" s="6" t="str">
+      <c r="O18" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button85" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button85" app:layout_constraintEnd_toStartOf="@id/button86" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button84" app:layout_constraintTop_toBottomOf="@id/button75" /&gt;</v>
       </c>
-      <c r="P18" s="6" t="str">
+      <c r="P18" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button86" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button86" app:layout_constraintEnd_toStartOf="@id/button87" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button85" app:layout_constraintTop_toBottomOf="@id/button76" /&gt;</v>
       </c>
-      <c r="Q18" s="6" t="str">
+      <c r="Q18" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button87" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button87" app:layout_constraintEnd_toStartOf="@id/button88" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button86" app:layout_constraintTop_toBottomOf="@id/button77" /&gt;</v>
       </c>
-      <c r="R18" s="6" t="str">
+      <c r="R18" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button88" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button88" app:layout_constraintEnd_toStartOf="@id/button89" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button87" app:layout_constraintTop_toBottomOf="@id/button78" /&gt;</v>
       </c>
-      <c r="S18" s="8" t="str">
+      <c r="S18" s="7" t="str">
         <f t="shared" si="14"/>
         <v>&lt;Button android:id="@+id/button89" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button89" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button88" app:layout_constraintTop_toBottomOf="@id/button79" /&gt;</v>
       </c>
     </row>
     <row r="19" spans="11:19">
-      <c r="K19" s="4" t="str">
+      <c r="K19" s="3" t="str">
         <f t="shared" si="12"/>
         <v>&lt;Button android:id="@+id/button91" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginLeft="8dp" android:layout_marginStart="8dp" android:minWidth="40dp" android:onClick="button91" app:layout_constraintEnd_toStartOf="@id/button92" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toStartOf="parent" app:layout_constraintTop_toBottomOf="@id/button81" /&gt;</v>
       </c>
-      <c r="L19" s="6" t="str">
+      <c r="L19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button92" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button92" app:layout_constraintEnd_toStartOf="@id/button93" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button91" app:layout_constraintTop_toBottomOf="@id/button82" /&gt;</v>
       </c>
-      <c r="M19" s="6" t="str">
+      <c r="M19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button93" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button93" app:layout_constraintEnd_toStartOf="@id/button94" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button92" app:layout_constraintTop_toBottomOf="@id/button83" /&gt;</v>
       </c>
-      <c r="N19" s="6" t="str">
+      <c r="N19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button94" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button94" app:layout_constraintEnd_toStartOf="@id/button95" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button93" app:layout_constraintTop_toBottomOf="@id/button84" /&gt;</v>
       </c>
-      <c r="O19" s="6" t="str">
+      <c r="O19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button95" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button95" app:layout_constraintEnd_toStartOf="@id/button96" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button94" app:layout_constraintTop_toBottomOf="@id/button85" /&gt;</v>
       </c>
-      <c r="P19" s="6" t="str">
+      <c r="P19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button96" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button96" app:layout_constraintEnd_toStartOf="@id/button97" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button95" app:layout_constraintTop_toBottomOf="@id/button86" /&gt;</v>
       </c>
-      <c r="Q19" s="6" t="str">
+      <c r="Q19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button97" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button97" app:layout_constraintEnd_toStartOf="@id/button98" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button96" app:layout_constraintTop_toBottomOf="@id/button87" /&gt;</v>
       </c>
-      <c r="R19" s="6" t="str">
+      <c r="R19" s="5" t="str">
         <f t="shared" si="13"/>
         <v>&lt;Button android:id="@+id/button98" android:layout_width="wrap_content" android:layout_height="wrap_content" android:minWidth="40dp" android:onClick="button98" app:layout_constraintEnd_toStartOf="@id/button99" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@+id/button97" app:layout_constraintTop_toBottomOf="@id/button88" /&gt;</v>
       </c>
-      <c r="S19" s="8" t="str">
+      <c r="S19" s="7" t="str">
         <f t="shared" si="14"/>
         <v>&lt;Button android:id="@+id/button99" android:layout_width="wrap_content" android:layout_height="wrap_content" android:layout_marginEnd="8dp" android:layout_marginRight="8dp" android:minWidth="40dp" android:onClick="button99" app:layout_constraintEnd_toEndOf="parent" app:layout_constraintHorizontal_weight="1" app:layout_constraintStart_toEndOf="@id/button98" app:layout_constraintTop_toBottomOf="@id/button89" /&gt;</v>
       </c>
@@ -2173,6 +2232,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2202,7 +2262,7 @@
         <f>A1&amp;" = findViewById(R.id."&amp;A1&amp;");"</f>
         <v>button11 = findViewById(R.id.button11);</v>
       </c>
-      <c r="D1" s="9" t="str">
+      <c r="D1" s="8" t="str">
         <f>A1&amp;".getBackground().setColorFilter(null);"</f>
         <v>button11.getBackground().setColorFilter(null);</v>
       </c>
@@ -2231,7 +2291,7 @@
         <f t="shared" ref="C2:C65" si="1">A2&amp;" = findViewById(R.id."&amp;A2&amp;");"</f>
         <v>button12 = findViewById(R.id.button12);</v>
       </c>
-      <c r="D2" s="9" t="str">
+      <c r="D2" s="8" t="str">
         <f t="shared" ref="D2:D65" si="2">A2&amp;".getBackground().setColorFilter(null);"</f>
         <v>button12.getBackground().setColorFilter(null);</v>
       </c>
@@ -2260,7 +2320,7 @@
         <f t="shared" si="1"/>
         <v>button13 = findViewById(R.id.button13);</v>
       </c>
-      <c r="D3" s="9" t="str">
+      <c r="D3" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button13.getBackground().setColorFilter(null);</v>
       </c>
@@ -2289,7 +2349,7 @@
         <f t="shared" si="1"/>
         <v>button14 = findViewById(R.id.button14);</v>
       </c>
-      <c r="D4" s="9" t="str">
+      <c r="D4" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button14.getBackground().setColorFilter(null);</v>
       </c>
@@ -2318,7 +2378,7 @@
         <f t="shared" si="1"/>
         <v>button15 = findViewById(R.id.button15);</v>
       </c>
-      <c r="D5" s="9" t="str">
+      <c r="D5" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button15.getBackground().setColorFilter(null);</v>
       </c>
@@ -2347,7 +2407,7 @@
         <f t="shared" si="1"/>
         <v>button16 = findViewById(R.id.button16);</v>
       </c>
-      <c r="D6" s="9" t="str">
+      <c r="D6" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button16.getBackground().setColorFilter(null);</v>
       </c>
@@ -2376,7 +2436,7 @@
         <f t="shared" si="1"/>
         <v>button17 = findViewById(R.id.button17);</v>
       </c>
-      <c r="D7" s="9" t="str">
+      <c r="D7" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button17.getBackground().setColorFilter(null);</v>
       </c>
@@ -2405,7 +2465,7 @@
         <f t="shared" si="1"/>
         <v>button18 = findViewById(R.id.button18);</v>
       </c>
-      <c r="D8" s="9" t="str">
+      <c r="D8" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button18.getBackground().setColorFilter(null);</v>
       </c>
@@ -2434,7 +2494,7 @@
         <f t="shared" si="1"/>
         <v>button19 = findViewById(R.id.button19);</v>
       </c>
-      <c r="D9" s="9" t="str">
+      <c r="D9" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button19.getBackground().setColorFilter(null);</v>
       </c>
@@ -2463,7 +2523,7 @@
         <f t="shared" si="1"/>
         <v>button21 = findViewById(R.id.button21);</v>
       </c>
-      <c r="D10" s="9" t="str">
+      <c r="D10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button21.getBackground().setColorFilter(null);</v>
       </c>
@@ -2492,7 +2552,7 @@
         <f t="shared" si="1"/>
         <v>button22 = findViewById(R.id.button22);</v>
       </c>
-      <c r="D11" s="9" t="str">
+      <c r="D11" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button22.getBackground().setColorFilter(null);</v>
       </c>
@@ -2521,7 +2581,7 @@
         <f t="shared" si="1"/>
         <v>button23 = findViewById(R.id.button23);</v>
       </c>
-      <c r="D12" s="9" t="str">
+      <c r="D12" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button23.getBackground().setColorFilter(null);</v>
       </c>
@@ -2550,7 +2610,7 @@
         <f t="shared" si="1"/>
         <v>button24 = findViewById(R.id.button24);</v>
       </c>
-      <c r="D13" s="9" t="str">
+      <c r="D13" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button24.getBackground().setColorFilter(null);</v>
       </c>
@@ -2579,7 +2639,7 @@
         <f t="shared" si="1"/>
         <v>button25 = findViewById(R.id.button25);</v>
       </c>
-      <c r="D14" s="9" t="str">
+      <c r="D14" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button25.getBackground().setColorFilter(null);</v>
       </c>
@@ -2608,7 +2668,7 @@
         <f t="shared" si="1"/>
         <v>button26 = findViewById(R.id.button26);</v>
       </c>
-      <c r="D15" s="9" t="str">
+      <c r="D15" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button26.getBackground().setColorFilter(null);</v>
       </c>
@@ -2637,7 +2697,7 @@
         <f t="shared" si="1"/>
         <v>button27 = findViewById(R.id.button27);</v>
       </c>
-      <c r="D16" s="9" t="str">
+      <c r="D16" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button27.getBackground().setColorFilter(null);</v>
       </c>
@@ -2666,7 +2726,7 @@
         <f t="shared" si="1"/>
         <v>button28 = findViewById(R.id.button28);</v>
       </c>
-      <c r="D17" s="9" t="str">
+      <c r="D17" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button28.getBackground().setColorFilter(null);</v>
       </c>
@@ -2695,7 +2755,7 @@
         <f t="shared" si="1"/>
         <v>button29 = findViewById(R.id.button29);</v>
       </c>
-      <c r="D18" s="9" t="str">
+      <c r="D18" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button29.getBackground().setColorFilter(null);</v>
       </c>
@@ -2724,7 +2784,7 @@
         <f t="shared" si="1"/>
         <v>button31 = findViewById(R.id.button31);</v>
       </c>
-      <c r="D19" s="9" t="str">
+      <c r="D19" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button31.getBackground().setColorFilter(null);</v>
       </c>
@@ -2753,7 +2813,7 @@
         <f t="shared" si="1"/>
         <v>button32 = findViewById(R.id.button32);</v>
       </c>
-      <c r="D20" s="9" t="str">
+      <c r="D20" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button32.getBackground().setColorFilter(null);</v>
       </c>
@@ -2782,7 +2842,7 @@
         <f t="shared" si="1"/>
         <v>button33 = findViewById(R.id.button33);</v>
       </c>
-      <c r="D21" s="9" t="str">
+      <c r="D21" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button33.getBackground().setColorFilter(null);</v>
       </c>
@@ -2811,7 +2871,7 @@
         <f t="shared" si="1"/>
         <v>button34 = findViewById(R.id.button34);</v>
       </c>
-      <c r="D22" s="9" t="str">
+      <c r="D22" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button34.getBackground().setColorFilter(null);</v>
       </c>
@@ -2840,7 +2900,7 @@
         <f t="shared" si="1"/>
         <v>button35 = findViewById(R.id.button35);</v>
       </c>
-      <c r="D23" s="9" t="str">
+      <c r="D23" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button35.getBackground().setColorFilter(null);</v>
       </c>
@@ -2869,7 +2929,7 @@
         <f t="shared" si="1"/>
         <v>button36 = findViewById(R.id.button36);</v>
       </c>
-      <c r="D24" s="9" t="str">
+      <c r="D24" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button36.getBackground().setColorFilter(null);</v>
       </c>
@@ -2898,7 +2958,7 @@
         <f t="shared" si="1"/>
         <v>button37 = findViewById(R.id.button37);</v>
       </c>
-      <c r="D25" s="9" t="str">
+      <c r="D25" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button37.getBackground().setColorFilter(null);</v>
       </c>
@@ -2927,7 +2987,7 @@
         <f t="shared" si="1"/>
         <v>button38 = findViewById(R.id.button38);</v>
       </c>
-      <c r="D26" s="9" t="str">
+      <c r="D26" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button38.getBackground().setColorFilter(null);</v>
       </c>
@@ -2956,7 +3016,7 @@
         <f t="shared" si="1"/>
         <v>button39 = findViewById(R.id.button39);</v>
       </c>
-      <c r="D27" s="9" t="str">
+      <c r="D27" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button39.getBackground().setColorFilter(null);</v>
       </c>
@@ -2985,7 +3045,7 @@
         <f t="shared" si="1"/>
         <v>button41 = findViewById(R.id.button41);</v>
       </c>
-      <c r="D28" s="9" t="str">
+      <c r="D28" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button41.getBackground().setColorFilter(null);</v>
       </c>
@@ -3014,7 +3074,7 @@
         <f t="shared" si="1"/>
         <v>button42 = findViewById(R.id.button42);</v>
       </c>
-      <c r="D29" s="9" t="str">
+      <c r="D29" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button42.getBackground().setColorFilter(null);</v>
       </c>
@@ -3043,7 +3103,7 @@
         <f t="shared" si="1"/>
         <v>button43 = findViewById(R.id.button43);</v>
       </c>
-      <c r="D30" s="9" t="str">
+      <c r="D30" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button43.getBackground().setColorFilter(null);</v>
       </c>
@@ -3072,7 +3132,7 @@
         <f t="shared" si="1"/>
         <v>button44 = findViewById(R.id.button44);</v>
       </c>
-      <c r="D31" s="9" t="str">
+      <c r="D31" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button44.getBackground().setColorFilter(null);</v>
       </c>
@@ -3101,7 +3161,7 @@
         <f t="shared" si="1"/>
         <v>button45 = findViewById(R.id.button45);</v>
       </c>
-      <c r="D32" s="9" t="str">
+      <c r="D32" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button45.getBackground().setColorFilter(null);</v>
       </c>
@@ -3130,7 +3190,7 @@
         <f t="shared" si="1"/>
         <v>button46 = findViewById(R.id.button46);</v>
       </c>
-      <c r="D33" s="9" t="str">
+      <c r="D33" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button46.getBackground().setColorFilter(null);</v>
       </c>
@@ -3159,7 +3219,7 @@
         <f t="shared" si="1"/>
         <v>button47 = findViewById(R.id.button47);</v>
       </c>
-      <c r="D34" s="9" t="str">
+      <c r="D34" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button47.getBackground().setColorFilter(null);</v>
       </c>
@@ -3188,7 +3248,7 @@
         <f t="shared" si="1"/>
         <v>button48 = findViewById(R.id.button48);</v>
       </c>
-      <c r="D35" s="9" t="str">
+      <c r="D35" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button48.getBackground().setColorFilter(null);</v>
       </c>
@@ -3217,7 +3277,7 @@
         <f t="shared" si="1"/>
         <v>button49 = findViewById(R.id.button49);</v>
       </c>
-      <c r="D36" s="9" t="str">
+      <c r="D36" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button49.getBackground().setColorFilter(null);</v>
       </c>
@@ -3246,7 +3306,7 @@
         <f t="shared" si="1"/>
         <v>button51 = findViewById(R.id.button51);</v>
       </c>
-      <c r="D37" s="9" t="str">
+      <c r="D37" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button51.getBackground().setColorFilter(null);</v>
       </c>
@@ -3275,7 +3335,7 @@
         <f t="shared" si="1"/>
         <v>button52 = findViewById(R.id.button52);</v>
       </c>
-      <c r="D38" s="9" t="str">
+      <c r="D38" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button52.getBackground().setColorFilter(null);</v>
       </c>
@@ -3304,7 +3364,7 @@
         <f t="shared" si="1"/>
         <v>button53 = findViewById(R.id.button53);</v>
       </c>
-      <c r="D39" s="9" t="str">
+      <c r="D39" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button53.getBackground().setColorFilter(null);</v>
       </c>
@@ -3333,7 +3393,7 @@
         <f t="shared" si="1"/>
         <v>button54 = findViewById(R.id.button54);</v>
       </c>
-      <c r="D40" s="9" t="str">
+      <c r="D40" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button54.getBackground().setColorFilter(null);</v>
       </c>
@@ -3362,7 +3422,7 @@
         <f t="shared" si="1"/>
         <v>button55 = findViewById(R.id.button55);</v>
       </c>
-      <c r="D41" s="9" t="str">
+      <c r="D41" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button55.getBackground().setColorFilter(null);</v>
       </c>
@@ -3391,7 +3451,7 @@
         <f t="shared" si="1"/>
         <v>button56 = findViewById(R.id.button56);</v>
       </c>
-      <c r="D42" s="9" t="str">
+      <c r="D42" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button56.getBackground().setColorFilter(null);</v>
       </c>
@@ -3420,7 +3480,7 @@
         <f t="shared" si="1"/>
         <v>button57 = findViewById(R.id.button57);</v>
       </c>
-      <c r="D43" s="9" t="str">
+      <c r="D43" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button57.getBackground().setColorFilter(null);</v>
       </c>
@@ -3449,7 +3509,7 @@
         <f t="shared" si="1"/>
         <v>button58 = findViewById(R.id.button58);</v>
       </c>
-      <c r="D44" s="9" t="str">
+      <c r="D44" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button58.getBackground().setColorFilter(null);</v>
       </c>
@@ -3478,7 +3538,7 @@
         <f t="shared" si="1"/>
         <v>button59 = findViewById(R.id.button59);</v>
       </c>
-      <c r="D45" s="9" t="str">
+      <c r="D45" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button59.getBackground().setColorFilter(null);</v>
       </c>
@@ -3507,7 +3567,7 @@
         <f t="shared" si="1"/>
         <v>button61 = findViewById(R.id.button61);</v>
       </c>
-      <c r="D46" s="9" t="str">
+      <c r="D46" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button61.getBackground().setColorFilter(null);</v>
       </c>
@@ -3536,7 +3596,7 @@
         <f t="shared" si="1"/>
         <v>button62 = findViewById(R.id.button62);</v>
       </c>
-      <c r="D47" s="9" t="str">
+      <c r="D47" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button62.getBackground().setColorFilter(null);</v>
       </c>
@@ -3565,7 +3625,7 @@
         <f t="shared" si="1"/>
         <v>button63 = findViewById(R.id.button63);</v>
       </c>
-      <c r="D48" s="9" t="str">
+      <c r="D48" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button63.getBackground().setColorFilter(null);</v>
       </c>
@@ -3594,7 +3654,7 @@
         <f t="shared" si="1"/>
         <v>button64 = findViewById(R.id.button64);</v>
       </c>
-      <c r="D49" s="9" t="str">
+      <c r="D49" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button64.getBackground().setColorFilter(null);</v>
       </c>
@@ -3623,7 +3683,7 @@
         <f t="shared" si="1"/>
         <v>button65 = findViewById(R.id.button65);</v>
       </c>
-      <c r="D50" s="9" t="str">
+      <c r="D50" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button65.getBackground().setColorFilter(null);</v>
       </c>
@@ -3652,7 +3712,7 @@
         <f t="shared" si="1"/>
         <v>button66 = findViewById(R.id.button66);</v>
       </c>
-      <c r="D51" s="9" t="str">
+      <c r="D51" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button66.getBackground().setColorFilter(null);</v>
       </c>
@@ -3681,7 +3741,7 @@
         <f t="shared" si="1"/>
         <v>button67 = findViewById(R.id.button67);</v>
       </c>
-      <c r="D52" s="9" t="str">
+      <c r="D52" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button67.getBackground().setColorFilter(null);</v>
       </c>
@@ -3710,7 +3770,7 @@
         <f t="shared" si="1"/>
         <v>button68 = findViewById(R.id.button68);</v>
       </c>
-      <c r="D53" s="9" t="str">
+      <c r="D53" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button68.getBackground().setColorFilter(null);</v>
       </c>
@@ -3739,7 +3799,7 @@
         <f t="shared" si="1"/>
         <v>button69 = findViewById(R.id.button69);</v>
       </c>
-      <c r="D54" s="9" t="str">
+      <c r="D54" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button69.getBackground().setColorFilter(null);</v>
       </c>
@@ -3768,7 +3828,7 @@
         <f t="shared" si="1"/>
         <v>button71 = findViewById(R.id.button71);</v>
       </c>
-      <c r="D55" s="9" t="str">
+      <c r="D55" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button71.getBackground().setColorFilter(null);</v>
       </c>
@@ -3797,7 +3857,7 @@
         <f t="shared" si="1"/>
         <v>button72 = findViewById(R.id.button72);</v>
       </c>
-      <c r="D56" s="9" t="str">
+      <c r="D56" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button72.getBackground().setColorFilter(null);</v>
       </c>
@@ -3826,7 +3886,7 @@
         <f t="shared" si="1"/>
         <v>button73 = findViewById(R.id.button73);</v>
       </c>
-      <c r="D57" s="9" t="str">
+      <c r="D57" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button73.getBackground().setColorFilter(null);</v>
       </c>
@@ -3855,7 +3915,7 @@
         <f t="shared" si="1"/>
         <v>button74 = findViewById(R.id.button74);</v>
       </c>
-      <c r="D58" s="9" t="str">
+      <c r="D58" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button74.getBackground().setColorFilter(null);</v>
       </c>
@@ -3884,7 +3944,7 @@
         <f t="shared" si="1"/>
         <v>button75 = findViewById(R.id.button75);</v>
       </c>
-      <c r="D59" s="9" t="str">
+      <c r="D59" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button75.getBackground().setColorFilter(null);</v>
       </c>
@@ -3913,7 +3973,7 @@
         <f t="shared" si="1"/>
         <v>button76 = findViewById(R.id.button76);</v>
       </c>
-      <c r="D60" s="9" t="str">
+      <c r="D60" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button76.getBackground().setColorFilter(null);</v>
       </c>
@@ -3942,7 +4002,7 @@
         <f t="shared" si="1"/>
         <v>button77 = findViewById(R.id.button77);</v>
       </c>
-      <c r="D61" s="9" t="str">
+      <c r="D61" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button77.getBackground().setColorFilter(null);</v>
       </c>
@@ -3971,7 +4031,7 @@
         <f t="shared" si="1"/>
         <v>button78 = findViewById(R.id.button78);</v>
       </c>
-      <c r="D62" s="9" t="str">
+      <c r="D62" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button78.getBackground().setColorFilter(null);</v>
       </c>
@@ -4000,7 +4060,7 @@
         <f t="shared" si="1"/>
         <v>button79 = findViewById(R.id.button79);</v>
       </c>
-      <c r="D63" s="9" t="str">
+      <c r="D63" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button79.getBackground().setColorFilter(null);</v>
       </c>
@@ -4029,7 +4089,7 @@
         <f t="shared" si="1"/>
         <v>button81 = findViewById(R.id.button81);</v>
       </c>
-      <c r="D64" s="9" t="str">
+      <c r="D64" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button81.getBackground().setColorFilter(null);</v>
       </c>
@@ -4058,7 +4118,7 @@
         <f t="shared" si="1"/>
         <v>button82 = findViewById(R.id.button82);</v>
       </c>
-      <c r="D65" s="9" t="str">
+      <c r="D65" s="8" t="str">
         <f t="shared" si="2"/>
         <v>button82.getBackground().setColorFilter(null);</v>
       </c>
@@ -4087,7 +4147,7 @@
         <f t="shared" ref="C66:C81" si="7">A66&amp;" = findViewById(R.id."&amp;A66&amp;");"</f>
         <v>button83 = findViewById(R.id.button83);</v>
       </c>
-      <c r="D66" s="9" t="str">
+      <c r="D66" s="8" t="str">
         <f t="shared" ref="D66:D81" si="8">A66&amp;".getBackground().setColorFilter(null);"</f>
         <v>button83.getBackground().setColorFilter(null);</v>
       </c>
@@ -4116,7 +4176,7 @@
         <f t="shared" si="7"/>
         <v>button84 = findViewById(R.id.button84);</v>
       </c>
-      <c r="D67" s="9" t="str">
+      <c r="D67" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button84.getBackground().setColorFilter(null);</v>
       </c>
@@ -4145,7 +4205,7 @@
         <f t="shared" si="7"/>
         <v>button85 = findViewById(R.id.button85);</v>
       </c>
-      <c r="D68" s="9" t="str">
+      <c r="D68" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button85.getBackground().setColorFilter(null);</v>
       </c>
@@ -4174,7 +4234,7 @@
         <f t="shared" si="7"/>
         <v>button86 = findViewById(R.id.button86);</v>
       </c>
-      <c r="D69" s="9" t="str">
+      <c r="D69" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button86.getBackground().setColorFilter(null);</v>
       </c>
@@ -4203,7 +4263,7 @@
         <f t="shared" si="7"/>
         <v>button87 = findViewById(R.id.button87);</v>
       </c>
-      <c r="D70" s="9" t="str">
+      <c r="D70" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button87.getBackground().setColorFilter(null);</v>
       </c>
@@ -4232,7 +4292,7 @@
         <f t="shared" si="7"/>
         <v>button88 = findViewById(R.id.button88);</v>
       </c>
-      <c r="D71" s="9" t="str">
+      <c r="D71" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button88.getBackground().setColorFilter(null);</v>
       </c>
@@ -4261,7 +4321,7 @@
         <f t="shared" si="7"/>
         <v>button89 = findViewById(R.id.button89);</v>
       </c>
-      <c r="D72" s="9" t="str">
+      <c r="D72" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button89.getBackground().setColorFilter(null);</v>
       </c>
@@ -4290,7 +4350,7 @@
         <f t="shared" si="7"/>
         <v>button91 = findViewById(R.id.button91);</v>
       </c>
-      <c r="D73" s="9" t="str">
+      <c r="D73" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button91.getBackground().setColorFilter(null);</v>
       </c>
@@ -4319,7 +4379,7 @@
         <f t="shared" si="7"/>
         <v>button92 = findViewById(R.id.button92);</v>
       </c>
-      <c r="D74" s="9" t="str">
+      <c r="D74" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button92.getBackground().setColorFilter(null);</v>
       </c>
@@ -4348,7 +4408,7 @@
         <f t="shared" si="7"/>
         <v>button93 = findViewById(R.id.button93);</v>
       </c>
-      <c r="D75" s="9" t="str">
+      <c r="D75" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button93.getBackground().setColorFilter(null);</v>
       </c>
@@ -4377,7 +4437,7 @@
         <f t="shared" si="7"/>
         <v>button94 = findViewById(R.id.button94);</v>
       </c>
-      <c r="D76" s="9" t="str">
+      <c r="D76" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button94.getBackground().setColorFilter(null);</v>
       </c>
@@ -4406,7 +4466,7 @@
         <f t="shared" si="7"/>
         <v>button95 = findViewById(R.id.button95);</v>
       </c>
-      <c r="D77" s="9" t="str">
+      <c r="D77" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button95.getBackground().setColorFilter(null);</v>
       </c>
@@ -4435,7 +4495,7 @@
         <f t="shared" si="7"/>
         <v>button96 = findViewById(R.id.button96);</v>
       </c>
-      <c r="D78" s="9" t="str">
+      <c r="D78" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button96.getBackground().setColorFilter(null);</v>
       </c>
@@ -4464,7 +4524,7 @@
         <f t="shared" si="7"/>
         <v>button97 = findViewById(R.id.button97);</v>
       </c>
-      <c r="D79" s="9" t="str">
+      <c r="D79" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button97.getBackground().setColorFilter(null);</v>
       </c>
@@ -4493,7 +4553,7 @@
         <f t="shared" si="7"/>
         <v>button98 = findViewById(R.id.button98);</v>
       </c>
-      <c r="D80" s="9" t="str">
+      <c r="D80" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button98.getBackground().setColorFilter(null);</v>
       </c>
@@ -4522,7 +4582,7 @@
         <f t="shared" si="7"/>
         <v>button99 = findViewById(R.id.button99);</v>
       </c>
-      <c r="D81" s="9" t="str">
+      <c r="D81" s="8" t="str">
         <f t="shared" si="8"/>
         <v>button99.getBackground().setColorFilter(null);</v>
       </c>
@@ -4549,7 +4609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
@@ -4559,17 +4619,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2">
@@ -5157,17 +5217,17 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12">
@@ -5197,39 +5257,39 @@
       <c r="I12">
         <v>19</v>
       </c>
-      <c r="K12" s="3" t="str">
+      <c r="K12" s="2" t="str">
         <f>"button"&amp;A12&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button11.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L12" s="3" t="str">
+      <c r="L12" s="2" t="str">
         <f t="shared" ref="L12:S12" si="2">"button"&amp;B12&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button12.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M12" s="3" t="str">
+      <c r="M12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>button13.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N12" s="3" t="str">
+      <c r="N12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>button14.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O12" s="3" t="str">
+      <c r="O12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>button15.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P12" s="3" t="str">
+      <c r="P12" s="2" t="str">
         <f>"button"&amp;F12&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button16.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q12" s="3" t="str">
+      <c r="Q12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>button17.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R12" s="3" t="str">
+      <c r="R12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>button18.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S12" s="3" t="str">
+      <c r="S12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>button19.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -5262,39 +5322,39 @@
       <c r="I13">
         <v>29</v>
       </c>
-      <c r="K13" s="3" t="str">
+      <c r="K13" s="2" t="str">
         <f t="shared" ref="K13:K20" si="3">"button"&amp;A13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button21.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L13" s="3" t="str">
+      <c r="L13" s="2" t="str">
         <f t="shared" ref="L13:L20" si="4">"button"&amp;B13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button22.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M13" s="3" t="str">
+      <c r="M13" s="2" t="str">
         <f t="shared" ref="M13:M20" si="5">"button"&amp;C13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button23.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N13" s="3" t="str">
+      <c r="N13" s="2" t="str">
         <f t="shared" ref="N13:N20" si="6">"button"&amp;D13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button24.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O13" s="3" t="str">
+      <c r="O13" s="2" t="str">
         <f t="shared" ref="O13:O20" si="7">"button"&amp;E13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button25.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P13" s="3" t="str">
+      <c r="P13" s="2" t="str">
         <f t="shared" ref="P13:P20" si="8">"button"&amp;F13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button26.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q13" s="3" t="str">
+      <c r="Q13" s="2" t="str">
         <f t="shared" ref="Q13:Q20" si="9">"button"&amp;G13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button27.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R13" s="3" t="str">
+      <c r="R13" s="2" t="str">
         <f t="shared" ref="R13:R20" si="10">"button"&amp;H13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button28.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S13" s="3" t="str">
+      <c r="S13" s="2" t="str">
         <f t="shared" ref="S13:S20" si="11">"button"&amp;I13&amp;".getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));"</f>
         <v>button29.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -5327,39 +5387,39 @@
       <c r="I14">
         <v>39</v>
       </c>
-      <c r="K14" s="3" t="str">
+      <c r="K14" s="2" t="str">
         <f t="shared" si="3"/>
         <v>button31.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L14" s="3" t="str">
+      <c r="L14" s="2" t="str">
         <f t="shared" si="4"/>
         <v>button32.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M14" s="3" t="str">
+      <c r="M14" s="2" t="str">
         <f t="shared" si="5"/>
         <v>button33.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N14" s="3" t="str">
+      <c r="N14" s="2" t="str">
         <f t="shared" si="6"/>
         <v>button34.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O14" s="3" t="str">
+      <c r="O14" s="2" t="str">
         <f t="shared" si="7"/>
         <v>button35.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P14" s="3" t="str">
+      <c r="P14" s="2" t="str">
         <f t="shared" si="8"/>
         <v>button36.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q14" s="3" t="str">
+      <c r="Q14" s="2" t="str">
         <f t="shared" si="9"/>
         <v>button37.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R14" s="3" t="str">
+      <c r="R14" s="2" t="str">
         <f t="shared" si="10"/>
         <v>button38.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S14" s="3" t="str">
+      <c r="S14" s="2" t="str">
         <f t="shared" si="11"/>
         <v>button39.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -5392,39 +5452,39 @@
       <c r="I15">
         <v>49</v>
       </c>
-      <c r="K15" s="3" t="str">
+      <c r="K15" s="2" t="str">
         <f t="shared" si="3"/>
         <v>button41.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L15" s="3" t="str">
+      <c r="L15" s="2" t="str">
         <f t="shared" si="4"/>
         <v>button42.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M15" s="3" t="str">
+      <c r="M15" s="2" t="str">
         <f t="shared" si="5"/>
         <v>button43.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N15" s="3" t="str">
+      <c r="N15" s="2" t="str">
         <f t="shared" si="6"/>
         <v>button44.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O15" s="3" t="str">
+      <c r="O15" s="2" t="str">
         <f t="shared" si="7"/>
         <v>button45.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P15" s="3" t="str">
+      <c r="P15" s="2" t="str">
         <f t="shared" si="8"/>
         <v>button46.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q15" s="3" t="str">
+      <c r="Q15" s="2" t="str">
         <f t="shared" si="9"/>
         <v>button47.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R15" s="3" t="str">
+      <c r="R15" s="2" t="str">
         <f t="shared" si="10"/>
         <v>button48.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S15" s="3" t="str">
+      <c r="S15" s="2" t="str">
         <f t="shared" si="11"/>
         <v>button49.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -5457,39 +5517,39 @@
       <c r="I16">
         <v>59</v>
       </c>
-      <c r="K16" s="3" t="str">
+      <c r="K16" s="2" t="str">
         <f t="shared" si="3"/>
         <v>button51.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L16" s="3" t="str">
+      <c r="L16" s="2" t="str">
         <f t="shared" si="4"/>
         <v>button52.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M16" s="3" t="str">
+      <c r="M16" s="2" t="str">
         <f t="shared" si="5"/>
         <v>button53.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N16" s="3" t="str">
+      <c r="N16" s="2" t="str">
         <f t="shared" si="6"/>
         <v>button54.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O16" s="3" t="str">
+      <c r="O16" s="2" t="str">
         <f t="shared" si="7"/>
         <v>button55.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P16" s="3" t="str">
+      <c r="P16" s="2" t="str">
         <f t="shared" si="8"/>
         <v>button56.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q16" s="3" t="str">
+      <c r="Q16" s="2" t="str">
         <f t="shared" si="9"/>
         <v>button57.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R16" s="3" t="str">
+      <c r="R16" s="2" t="str">
         <f t="shared" si="10"/>
         <v>button58.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S16" s="3" t="str">
+      <c r="S16" s="2" t="str">
         <f t="shared" si="11"/>
         <v>button59.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -5522,39 +5582,39 @@
       <c r="I17">
         <v>69</v>
       </c>
-      <c r="K17" s="3" t="str">
+      <c r="K17" s="2" t="str">
         <f t="shared" si="3"/>
         <v>button61.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L17" s="3" t="str">
+      <c r="L17" s="2" t="str">
         <f t="shared" si="4"/>
         <v>button62.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M17" s="3" t="str">
+      <c r="M17" s="2" t="str">
         <f t="shared" si="5"/>
         <v>button63.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N17" s="3" t="str">
+      <c r="N17" s="2" t="str">
         <f t="shared" si="6"/>
         <v>button64.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O17" s="3" t="str">
+      <c r="O17" s="2" t="str">
         <f t="shared" si="7"/>
         <v>button65.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P17" s="3" t="str">
+      <c r="P17" s="2" t="str">
         <f t="shared" si="8"/>
         <v>button66.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q17" s="3" t="str">
+      <c r="Q17" s="2" t="str">
         <f t="shared" si="9"/>
         <v>button67.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R17" s="3" t="str">
+      <c r="R17" s="2" t="str">
         <f t="shared" si="10"/>
         <v>button68.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S17" s="3" t="str">
+      <c r="S17" s="2" t="str">
         <f t="shared" si="11"/>
         <v>button69.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -5587,39 +5647,39 @@
       <c r="I18">
         <v>79</v>
       </c>
-      <c r="K18" s="3" t="str">
+      <c r="K18" s="2" t="str">
         <f t="shared" si="3"/>
         <v>button71.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L18" s="3" t="str">
+      <c r="L18" s="2" t="str">
         <f t="shared" si="4"/>
         <v>button72.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M18" s="3" t="str">
+      <c r="M18" s="2" t="str">
         <f t="shared" si="5"/>
         <v>button73.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N18" s="3" t="str">
+      <c r="N18" s="2" t="str">
         <f t="shared" si="6"/>
         <v>button74.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O18" s="3" t="str">
+      <c r="O18" s="2" t="str">
         <f t="shared" si="7"/>
         <v>button75.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P18" s="3" t="str">
+      <c r="P18" s="2" t="str">
         <f t="shared" si="8"/>
         <v>button76.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q18" s="3" t="str">
+      <c r="Q18" s="2" t="str">
         <f t="shared" si="9"/>
         <v>button77.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R18" s="3" t="str">
+      <c r="R18" s="2" t="str">
         <f t="shared" si="10"/>
         <v>button78.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S18" s="3" t="str">
+      <c r="S18" s="2" t="str">
         <f t="shared" si="11"/>
         <v>button79.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -5652,39 +5712,39 @@
       <c r="I19">
         <v>89</v>
       </c>
-      <c r="K19" s="3" t="str">
+      <c r="K19" s="2" t="str">
         <f t="shared" si="3"/>
         <v>button81.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L19" s="3" t="str">
+      <c r="L19" s="2" t="str">
         <f t="shared" si="4"/>
         <v>button82.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M19" s="3" t="str">
+      <c r="M19" s="2" t="str">
         <f t="shared" si="5"/>
         <v>button83.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N19" s="3" t="str">
+      <c r="N19" s="2" t="str">
         <f t="shared" si="6"/>
         <v>button84.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O19" s="3" t="str">
+      <c r="O19" s="2" t="str">
         <f t="shared" si="7"/>
         <v>button85.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P19" s="3" t="str">
+      <c r="P19" s="2" t="str">
         <f t="shared" si="8"/>
         <v>button86.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q19" s="3" t="str">
+      <c r="Q19" s="2" t="str">
         <f t="shared" si="9"/>
         <v>button87.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R19" s="3" t="str">
+      <c r="R19" s="2" t="str">
         <f t="shared" si="10"/>
         <v>button88.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S19" s="3" t="str">
+      <c r="S19" s="2" t="str">
         <f t="shared" si="11"/>
         <v>button89.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -5717,39 +5777,39 @@
       <c r="I20">
         <v>99</v>
       </c>
-      <c r="K20" s="3" t="str">
+      <c r="K20" s="2" t="str">
         <f t="shared" si="3"/>
         <v>button91.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="L20" s="3" t="str">
+      <c r="L20" s="2" t="str">
         <f t="shared" si="4"/>
         <v>button92.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="M20" s="3" t="str">
+      <c r="M20" s="2" t="str">
         <f t="shared" si="5"/>
         <v>button93.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="N20" s="3" t="str">
+      <c r="N20" s="2" t="str">
         <f t="shared" si="6"/>
         <v>button94.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="O20" s="3" t="str">
+      <c r="O20" s="2" t="str">
         <f t="shared" si="7"/>
         <v>button95.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="P20" s="3" t="str">
+      <c r="P20" s="2" t="str">
         <f t="shared" si="8"/>
         <v>button96.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="Q20" s="3" t="str">
+      <c r="Q20" s="2" t="str">
         <f t="shared" si="9"/>
         <v>button97.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="R20" s="3" t="str">
+      <c r="R20" s="2" t="str">
         <f t="shared" si="10"/>
         <v>button98.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
-      <c r="S20" s="3" t="str">
+      <c r="S20" s="2" t="str">
         <f t="shared" si="11"/>
         <v>button99.getBackground().setColorFilter(new LightingColorFilter(0xffC5E1A5, 0x000000));</v>
       </c>
@@ -7267,31 +7327,31 @@
       </c>
     </row>
     <row r="52" spans="11:20">
-      <c r="K52" s="10" t="s">
+      <c r="K52" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="L52" s="10" t="s">
+      <c r="L52" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="M52" s="10" t="s">
+      <c r="M52" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N52" s="12" t="s">
+      <c r="N52" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="O52" s="10" t="s">
+      <c r="O52" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="P52" s="14" t="s">
+      <c r="P52" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="Q52" s="10" t="s">
+      <c r="Q52" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="R52" s="10" t="s">
+      <c r="R52" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="S52" s="10" t="s">
+      <c r="S52" s="9" t="s">
         <v>91</v>
       </c>
       <c r="T52" t="s">
@@ -7299,31 +7359,31 @@
       </c>
     </row>
     <row r="53" spans="11:20">
-      <c r="K53" s="10" t="s">
+      <c r="K53" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="L53" s="10" t="s">
+      <c r="L53" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="M53" s="10" t="s">
+      <c r="M53" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="N53" s="12" t="s">
+      <c r="N53" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="O53" s="10" t="s">
+      <c r="O53" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="P53" s="14" t="s">
+      <c r="P53" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Q53" s="10" t="s">
+      <c r="Q53" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="R53" s="10" t="s">
+      <c r="R53" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="S53" s="10" t="s">
+      <c r="S53" s="9" t="s">
         <v>100</v>
       </c>
       <c r="T53" t="s">
@@ -7331,31 +7391,31 @@
       </c>
     </row>
     <row r="54" spans="11:20">
-      <c r="K54" s="11" t="s">
+      <c r="K54" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="L54" s="11" t="s">
+      <c r="L54" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="M54" s="11" t="s">
+      <c r="M54" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="N54" s="13" t="s">
+      <c r="N54" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="O54" s="11" t="s">
+      <c r="O54" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="P54" s="15" t="s">
+      <c r="P54" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="Q54" s="11" t="s">
+      <c r="Q54" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="R54" s="11" t="s">
+      <c r="R54" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="S54" s="11" t="s">
+      <c r="S54" s="10" t="s">
         <v>109</v>
       </c>
       <c r="T54" t="s">
@@ -7363,98 +7423,98 @@
       </c>
     </row>
     <row r="55" spans="11:20">
-      <c r="K55" s="10" t="s">
+      <c r="K55" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="L55" s="10" t="s">
+      <c r="L55" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="M55" s="10" t="s">
+      <c r="M55" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="N55" s="12" t="s">
+      <c r="N55" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="O55" s="10" t="s">
+      <c r="O55" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="P55" s="14" t="s">
+      <c r="P55" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="Q55" s="10" t="s">
+      <c r="Q55" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="R55" s="10" t="s">
+      <c r="R55" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="S55" s="10" t="s">
+      <c r="S55" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="T55" s="10" t="s">
+      <c r="T55" s="9" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="56" spans="11:20">
-      <c r="K56" s="10" t="s">
+      <c r="K56" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="L56" s="10" t="s">
+      <c r="L56" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="M56" s="10" t="s">
+      <c r="M56" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="N56" s="12" t="s">
+      <c r="N56" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="O56" s="10" t="s">
+      <c r="O56" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="P56" s="14" t="s">
+      <c r="P56" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="Q56" s="10" t="s">
+      <c r="Q56" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="R56" s="10" t="s">
+      <c r="R56" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="S56" s="10" t="s">
+      <c r="S56" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="T56" s="10" t="s">
+      <c r="T56" s="9" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="57" spans="11:20">
-      <c r="K57" s="11" t="s">
+      <c r="K57" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="L57" s="11" t="s">
+      <c r="L57" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="M57" s="11" t="s">
+      <c r="M57" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="N57" s="13" t="s">
+      <c r="N57" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="O57" s="11" t="s">
+      <c r="O57" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="P57" s="15" t="s">
+      <c r="P57" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="Q57" s="11" t="s">
+      <c r="Q57" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="R57" s="11" t="s">
+      <c r="R57" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="S57" s="11" t="s">
+      <c r="S57" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="T57" s="10" t="s">
+      <c r="T57" s="9" t="s">
         <v>164</v>
       </c>
     </row>
@@ -7468,13 +7528,13 @@
       <c r="M58" t="s">
         <v>139</v>
       </c>
-      <c r="N58" s="12" t="s">
+      <c r="N58" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="O58" s="10" t="s">
+      <c r="O58" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="P58" s="14" t="s">
+      <c r="P58" s="13" t="s">
         <v>142</v>
       </c>
       <c r="Q58" t="s">
@@ -7500,13 +7560,13 @@
       <c r="M59" t="s">
         <v>148</v>
       </c>
-      <c r="N59" s="12" t="s">
+      <c r="N59" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="O59" s="10" t="s">
+      <c r="O59" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="P59" s="14" t="s">
+      <c r="P59" s="13" t="s">
         <v>151</v>
       </c>
       <c r="Q59" t="s">
@@ -7532,13 +7592,13 @@
       <c r="M60" t="s">
         <v>157</v>
       </c>
-      <c r="N60" s="12" t="s">
+      <c r="N60" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="O60" s="10" t="s">
+      <c r="O60" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="P60" s="14" t="s">
+      <c r="P60" s="13" t="s">
         <v>160</v>
       </c>
       <c r="Q60" t="s">
@@ -7555,31 +7615,31 @@
       </c>
     </row>
     <row r="62" spans="11:20">
-      <c r="K62" s="10" t="s">
+      <c r="K62" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="L62" s="10" t="s">
+      <c r="L62" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="M62" s="10" t="s">
+      <c r="M62" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="N62" s="12" t="s">
+      <c r="N62" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="O62" s="10" t="s">
+      <c r="O62" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="P62" s="14" t="s">
+      <c r="P62" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="Q62" s="10" t="s">
+      <c r="Q62" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="R62" s="10" t="s">
+      <c r="R62" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="S62" s="10" t="s">
+      <c r="S62" s="9" t="s">
         <v>173</v>
       </c>
       <c r="T62" t="s">
@@ -7587,31 +7647,31 @@
       </c>
     </row>
     <row r="63" spans="11:20">
-      <c r="K63" s="10" t="s">
+      <c r="K63" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="L63" s="10" t="s">
+      <c r="L63" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="M63" s="10" t="s">
+      <c r="M63" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="N63" s="12" t="s">
+      <c r="N63" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="O63" s="10" t="s">
+      <c r="O63" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="P63" s="14" t="s">
+      <c r="P63" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="Q63" s="10" t="s">
+      <c r="Q63" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="R63" s="10" t="s">
+      <c r="R63" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="S63" s="10" t="s">
+      <c r="S63" s="9" t="s">
         <v>182</v>
       </c>
       <c r="T63" t="s">
@@ -7619,31 +7679,31 @@
       </c>
     </row>
     <row r="64" spans="11:20">
-      <c r="K64" s="11" t="s">
+      <c r="K64" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="L64" s="11" t="s">
+      <c r="L64" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="M64" s="11" t="s">
+      <c r="M64" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="N64" s="13" t="s">
+      <c r="N64" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="O64" s="11" t="s">
+      <c r="O64" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="P64" s="15" t="s">
+      <c r="P64" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="Q64" s="11" t="s">
+      <c r="Q64" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="R64" s="11" t="s">
+      <c r="R64" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="S64" s="11" t="s">
+      <c r="S64" s="10" t="s">
         <v>191</v>
       </c>
       <c r="T64" t="s">
@@ -7651,98 +7711,98 @@
       </c>
     </row>
     <row r="65" spans="11:20">
-      <c r="K65" s="10" t="s">
+      <c r="K65" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="L65" s="10" t="s">
+      <c r="L65" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="M65" s="10" t="s">
+      <c r="M65" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="N65" s="12" t="s">
+      <c r="N65" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="O65" s="10" t="s">
+      <c r="O65" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="P65" s="14" t="s">
+      <c r="P65" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="Q65" s="10" t="s">
+      <c r="Q65" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="R65" s="10" t="s">
+      <c r="R65" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="S65" s="10" t="s">
+      <c r="S65" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="T65" s="10" t="s">
+      <c r="T65" s="9" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="66" spans="11:20">
-      <c r="K66" s="10" t="s">
+      <c r="K66" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="L66" s="10" t="s">
+      <c r="L66" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="M66" s="10" t="s">
+      <c r="M66" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="N66" s="12" t="s">
+      <c r="N66" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="O66" s="10" t="s">
+      <c r="O66" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="P66" s="14" t="s">
+      <c r="P66" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="Q66" s="10" t="s">
+      <c r="Q66" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="R66" s="10" t="s">
+      <c r="R66" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="S66" s="10" t="s">
+      <c r="S66" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="T66" s="10" t="s">
+      <c r="T66" s="9" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="67" spans="11:20">
-      <c r="K67" s="11" t="s">
+      <c r="K67" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="L67" s="11" t="s">
+      <c r="L67" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="M67" s="11" t="s">
+      <c r="M67" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="N67" s="13" t="s">
+      <c r="N67" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="O67" s="11" t="s">
+      <c r="O67" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="P67" s="15" t="s">
+      <c r="P67" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="Q67" s="11" t="s">
+      <c r="Q67" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="R67" s="11" t="s">
+      <c r="R67" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="S67" s="11" t="s">
+      <c r="S67" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="T67" s="10" t="s">
+      <c r="T67" s="9" t="s">
         <v>164</v>
       </c>
     </row>
@@ -7756,13 +7816,13 @@
       <c r="M68" t="s">
         <v>221</v>
       </c>
-      <c r="N68" s="12" t="s">
+      <c r="N68" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="O68" s="10" t="s">
+      <c r="O68" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="P68" s="14" t="s">
+      <c r="P68" s="13" t="s">
         <v>224</v>
       </c>
       <c r="Q68" t="s">
@@ -7788,13 +7848,13 @@
       <c r="M69" t="s">
         <v>230</v>
       </c>
-      <c r="N69" s="12" t="s">
+      <c r="N69" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="O69" s="10" t="s">
+      <c r="O69" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="P69" s="14" t="s">
+      <c r="P69" s="13" t="s">
         <v>233</v>
       </c>
       <c r="Q69" t="s">
@@ -7820,13 +7880,13 @@
       <c r="M70" t="s">
         <v>239</v>
       </c>
-      <c r="N70" s="12" t="s">
+      <c r="N70" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="O70" s="10" t="s">
+      <c r="O70" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="P70" s="14" t="s">
+      <c r="P70" s="13" t="s">
         <v>242</v>
       </c>
       <c r="Q70" t="s">

</xml_diff>